<commit_message>
Starting Engine inputted into NMotor object
Finding that reading xlsx is a little slower. Looking into turning
efficiency of engine to be proportional to fuel flowrate * pressure /HP.

Stilll need to incorporate gears because it errors out when looking into
track gearRatio's
</commit_message>
<xml_diff>
--- a/Functions/SetupSheets.xlsx
+++ b/Functions/SetupSheets.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Journey\Documents\MATLAB\Combined LapSim\Functions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Journey\Documents\GitHub\LapSimCombined\Functions\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="200" windowWidth="15200" windowHeight="7140"/>
+    <workbookView xWindow="1820" yWindow="200" windowWidth="15200" windowHeight="7140" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Electric" sheetId="8" r:id="rId1"/>
@@ -652,8 +652,8 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1396,11 +1396,11 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:CQ50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="AY6" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="BC6" sqref="BC6"/>
+      <selection pane="bottomRight" activeCell="BA10" sqref="BA10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1593,7 +1593,7 @@
       <c r="BD1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="BE1" s="2" t="s">
+      <c r="BE1" s="38" t="s">
         <v>25</v>
       </c>
       <c r="BF1" s="2" t="s">
@@ -1870,7 +1870,7 @@
         <v>79</v>
       </c>
       <c r="BD2" s="9"/>
-      <c r="BE2" s="10" t="s">
+      <c r="BE2" s="39" t="s">
         <v>56</v>
       </c>
       <c r="BF2" s="10" t="s">
@@ -5120,19 +5120,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8193" r:id="rId4" name="SetDateTimeRef">
+        <control shapeId="8195" r:id="rId4" name="SetDateTimeMain">
           <controlPr print="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>2</xdr:row>
                 <xdr:rowOff>6350</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>12700</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -5140,7 +5140,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8193" r:id="rId4" name="SetDateTimeRef"/>
+        <control shapeId="8195" r:id="rId4" name="SetDateTimeMain"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -5170,19 +5170,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8195" r:id="rId8" name="SetDateTimeMain">
+        <control shapeId="8193" r:id="rId8" name="SetDateTimeRef">
           <controlPr print="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>6350</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>12700</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -5190,7 +5190,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8195" r:id="rId8" name="SetDateTimeMain"/>
+        <control shapeId="8193" r:id="rId8" name="SetDateTimeRef"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -5202,11 +5202,11 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:CQ50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="5" topLeftCell="CC6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="CG6" sqref="CG6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -5399,7 +5399,7 @@
       <c r="BD1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="BE1" s="2" t="s">
+      <c r="BE1" s="38" t="s">
         <v>25</v>
       </c>
       <c r="BF1" s="2" t="s">
@@ -5676,7 +5676,7 @@
         <v>79</v>
       </c>
       <c r="BD2" s="9"/>
-      <c r="BE2" s="10" t="s">
+      <c r="BE2" s="39" t="s">
         <v>56</v>
       </c>
       <c r="BF2" s="10" t="s">
@@ -6497,25 +6497,26 @@
         <v>0</v>
       </c>
       <c r="BF6" s="12">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="BG6" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BH6" s="12">
-        <v>0</v>
+        <v>1.6319999999999999</v>
       </c>
       <c r="BI6" s="12">
-        <v>0</v>
+        <v>1.333</v>
       </c>
       <c r="BJ6" s="12">
-        <v>0</v>
+        <v>1.095</v>
       </c>
       <c r="BK6" s="12">
-        <v>0</v>
-      </c>
-      <c r="BL6" s="12">
-        <v>0</v>
+        <v>2.6524999999999999</v>
+      </c>
+      <c r="BL6" s="44">
+        <f>38/14</f>
+        <v>2.7142857142857144</v>
       </c>
       <c r="BM6" s="12">
         <v>0.9</v>
@@ -6523,10 +6524,10 @@
       <c r="BN6" s="12">
         <v>0</v>
       </c>
-      <c r="BO6" s="44">
-        <v>0</v>
-      </c>
-      <c r="BP6" s="44">
+      <c r="BO6" s="12">
+        <v>0</v>
+      </c>
+      <c r="BP6" s="12">
         <v>0</v>
       </c>
       <c r="BQ6" s="12">
@@ -6572,22 +6573,22 @@
       </c>
       <c r="CF6" s="17"/>
       <c r="CG6" s="18">
-        <v>6.3</v>
+        <v>24</v>
       </c>
       <c r="CH6" s="18">
         <v>0</v>
       </c>
       <c r="CI6" s="18">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="CJ6" s="18">
-        <v>0</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="CK6" s="18">
-        <v>0</v>
+        <v>5.9999999999999995E-4</v>
       </c>
       <c r="CL6" s="18">
-        <v>0</v>
+        <v>5.9999999999999995E-4</v>
       </c>
       <c r="CM6" s="18">
         <v>0</v>
@@ -8921,24 +8922,27 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
+  <ignoredErrors>
+    <ignoredError sqref="BL6" unlockedFormula="1"/>
+  </ignoredErrors>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="4097" r:id="rId4" name="SetDateTimeRef">
+        <control shapeId="4099" r:id="rId4" name="SetDateTimeMain">
           <controlPr print="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>2</xdr:row>
                 <xdr:rowOff>6350</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>12700</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -8946,7 +8950,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="4097" r:id="rId4" name="SetDateTimeRef"/>
+        <control shapeId="4099" r:id="rId4" name="SetDateTimeMain"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8976,19 +8980,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="4099" r:id="rId8" name="SetDateTimeMain">
+        <control shapeId="4097" r:id="rId8" name="SetDateTimeRef">
           <controlPr print="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>6350</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>12700</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -8996,7 +9000,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="4099" r:id="rId8" name="SetDateTimeMain"/>
+        <control shapeId="4097" r:id="rId8" name="SetDateTimeRef"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
Now opens setupsheet, Debugging combustion issues
StraightThrottle is a 1x11 matrix, where the next line calls for the
second row. The car has no exit velocity, no entrance velocity.
Dimensions issue in Simulate.

Additionally tried adding some logic inside Car.Driveline to handle both
cars depending on gear reductions. However, switch and for loops aren't
happy around a function it appears.
</commit_message>
<xml_diff>
--- a/Functions/SetupSheets.xlsx
+++ b/Functions/SetupSheets.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="200" windowWidth="15200" windowHeight="7140" activeTab="1"/>
+    <workbookView xWindow="1820" yWindow="200" windowWidth="15200" windowHeight="7140"/>
   </bookViews>
   <sheets>
     <sheet name="Electric" sheetId="8" r:id="rId1"/>
@@ -1396,7 +1396,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:CQ50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
@@ -5120,19 +5120,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8195" r:id="rId4" name="SetDateTimeMain">
+        <control shapeId="8193" r:id="rId4" name="SetDateTimeRef">
           <controlPr print="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>6350</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>12700</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -5140,7 +5140,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8195" r:id="rId4" name="SetDateTimeMain"/>
+        <control shapeId="8193" r:id="rId4" name="SetDateTimeRef"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -5170,19 +5170,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8193" r:id="rId8" name="SetDateTimeRef">
+        <control shapeId="8195" r:id="rId8" name="SetDateTimeMain">
           <controlPr print="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>2</xdr:row>
                 <xdr:rowOff>6350</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>12700</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -5190,7 +5190,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8193" r:id="rId8" name="SetDateTimeRef"/>
+        <control shapeId="8195" r:id="rId8" name="SetDateTimeMain"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -5202,11 +5202,11 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:CQ50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="CC6" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="CG6" sqref="CG6"/>
+      <selection pane="bottomRight" activeCell="CR8" sqref="CR8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -6598,7 +6598,7 @@
         <v>280</v>
       </c>
       <c r="CP6" s="18">
-        <v>9900</v>
+        <v>9000</v>
       </c>
       <c r="CQ6" s="18">
         <v>0</v>
@@ -8930,19 +8930,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="4099" r:id="rId4" name="SetDateTimeMain">
+        <control shapeId="4097" r:id="rId4" name="SetDateTimeRef">
           <controlPr print="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>6350</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>12700</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -8950,7 +8950,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="4099" r:id="rId4" name="SetDateTimeMain"/>
+        <control shapeId="4097" r:id="rId4" name="SetDateTimeRef"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8980,19 +8980,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="4097" r:id="rId8" name="SetDateTimeRef">
+        <control shapeId="4099" r:id="rId8" name="SetDateTimeMain">
           <controlPr print="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>2</xdr:row>
                 <xdr:rowOff>6350</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>12700</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -9000,7 +9000,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="4097" r:id="rId8" name="SetDateTimeRef"/>
+        <control shapeId="4099" r:id="rId8" name="SetDateTimeMain"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
Thomas made edits to reading in setupsheet faster
I reverted it back to "tabs" because I felt it was easier to read. Still
having issue with straightthrottle function not being populated enough.
No entry, exit velocity. Efficiency NaN
</commit_message>
<xml_diff>
--- a/Functions/SetupSheets.xlsx
+++ b/Functions/SetupSheets.xlsx
@@ -9,18 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="200" windowWidth="15200" windowHeight="7140"/>
+    <workbookView xWindow="1820" yWindow="200" windowWidth="15200" windowHeight="7140" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Electric" sheetId="8" r:id="rId1"/>
-    <sheet name="Combustion" sheetId="6" r:id="rId2"/>
+    <sheet name="Combustion" sheetId="10" r:id="rId1"/>
+    <sheet name="Electric" sheetId="8" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="112">
   <si>
     <t>Date</t>
   </si>
@@ -328,31 +328,34 @@
     <t>slug/ft2</t>
   </si>
   <si>
+    <t>Driveline Sprung Mass</t>
+  </si>
+  <si>
+    <t>Driveline Unsprung Mass Front</t>
+  </si>
+  <si>
+    <t>Driveline Unsprung Mass Rear</t>
+  </si>
+  <si>
+    <t>Brake Unsprung Mass Front</t>
+  </si>
+  <si>
+    <t>Brake Unsprung Mass Rear</t>
+  </si>
+  <si>
+    <t>Fuel/Battery Weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[kwh] or Gal </t>
+  </si>
+  <si>
+    <t>Capacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chassis Parameters </t>
+  </si>
+  <si>
     <t>Chassis Parameters</t>
-  </si>
-  <si>
-    <t>Driveline Sprung Mass</t>
-  </si>
-  <si>
-    <t>Driveline Unsprung Mass Front</t>
-  </si>
-  <si>
-    <t>Driveline Unsprung Mass Rear</t>
-  </si>
-  <si>
-    <t>Brake Unsprung Mass Front</t>
-  </si>
-  <si>
-    <t>Brake Unsprung Mass Rear</t>
-  </si>
-  <si>
-    <t>Fuel/Battery Weight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[kwh] or Gal </t>
-  </si>
-  <si>
-    <t>Capacity</t>
   </si>
 </sst>
 </file>
@@ -499,7 +502,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -652,10 +655,6 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -698,6 +697,231 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>6350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>12700</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9217" name="SetDateTimeRef" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9217"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData fPrintsWithSheet="0"/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>12700</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9218" name="ToggleValues" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9218"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData fPrintsWithSheet="0"/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>6350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>12700</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9219" name="SetDateTimeMain" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9219"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData fPrintsWithSheet="0"/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>798917</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5" descr="logo_530x170"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="2571750" cy="798917"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
@@ -902,231 +1126,6 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>0</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
-          <xdr:row>3</xdr:row>
-          <xdr:rowOff>6350</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>12700</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="4097" name="SetDateTimeRef" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s4097"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData fPrintsWithSheet="0"/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>44450</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>711200</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>811617</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="logo_530x170"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="44450" y="12700"/>
-          <a:ext cx="2571750" cy="798917"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>0</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
-          <xdr:row>1</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>12700</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="4098" name="ToggleValues" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s4098"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData fPrintsWithSheet="0"/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>0</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>6350</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>12700</xdr:colOff>
-          <xdr:row>3</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="4099" name="SetDateTimeMain" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s4099"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData fPrintsWithSheet="0"/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
@@ -1393,14 +1392,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet5"/>
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:CQ50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="BA10" sqref="BA10"/>
+      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1408,7 +1407,7 @@
     <col min="1" max="1" width="15" style="23" customWidth="1"/>
     <col min="2" max="2" width="12.26953125" style="33" customWidth="1"/>
     <col min="3" max="3" width="12.26953125" style="34" customWidth="1"/>
-    <col min="4" max="4" width="6.81640625" style="24" customWidth="1"/>
+    <col min="4" max="4" width="10.36328125" style="24" customWidth="1"/>
     <col min="5" max="25" width="6.81640625" style="23" customWidth="1"/>
     <col min="26" max="26" width="6.81640625" style="24" customWidth="1"/>
     <col min="27" max="48" width="6.81640625" style="23" customWidth="1"/>
@@ -1435,7 +1434,7 @@
       <c r="B1" s="5"/>
       <c r="C1" s="7"/>
       <c r="D1" s="3" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -1621,13 +1620,13 @@
         <v>51</v>
       </c>
       <c r="BN1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="BO1" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="BO1" s="2" t="s">
+      <c r="BP1" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="BP1" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="BQ1" s="2" t="s">
         <v>49</v>
@@ -1645,10 +1644,10 @@
         <v>43</v>
       </c>
       <c r="BV1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="BW1" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="BW1" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="BX1" s="2" t="s">
         <v>49</v>
@@ -1678,10 +1677,10 @@
         <v>84</v>
       </c>
       <c r="CG1" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="CH1" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="CI1" s="6" t="s">
         <v>87</v>
@@ -1949,7 +1948,7 @@
       </c>
       <c r="CF2" s="9"/>
       <c r="CG2" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="CH2" s="11" t="s">
         <v>38</v>
@@ -2180,10 +2179,7 @@
       </c>
       <c r="B5" s="29"/>
       <c r="C5" s="30"/>
-      <c r="D5" s="21">
-        <f>D3-D4</f>
-        <v>0</v>
-      </c>
+      <c r="D5" s="21"/>
       <c r="E5" s="43">
         <f t="shared" ref="E5:BP5" si="0">E3-E4</f>
         <v>0</v>
@@ -2817,7 +2813,7 @@
       <c r="Q7" s="18"/>
       <c r="R7" s="18"/>
       <c r="S7" s="18"/>
-      <c r="T7" s="18"/>
+      <c r="T7" s="41"/>
       <c r="U7" s="18"/>
       <c r="V7" s="18"/>
       <c r="W7" s="18"/>
@@ -2832,6 +2828,7 @@
       <c r="AF7" s="18"/>
       <c r="AG7" s="18"/>
       <c r="AH7" s="18"/>
+      <c r="AI7" s="18"/>
       <c r="AJ7" s="18"/>
       <c r="AK7" s="18"/>
       <c r="AL7" s="18"/>
@@ -2851,7 +2848,7 @@
       <c r="AZ7" s="18"/>
       <c r="BA7" s="18"/>
       <c r="BB7" s="18"/>
-      <c r="BC7" s="18"/>
+      <c r="BC7" s="40"/>
       <c r="BD7" s="17"/>
       <c r="BE7" s="12"/>
       <c r="BF7" s="12"/>
@@ -2867,6 +2864,7 @@
       <c r="BP7" s="12"/>
       <c r="BQ7" s="12"/>
       <c r="BR7" s="17"/>
+      <c r="BS7" s="12"/>
       <c r="BT7" s="12"/>
       <c r="BU7" s="12"/>
       <c r="BV7" s="12"/>
@@ -5120,19 +5118,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8193" r:id="rId4" name="SetDateTimeRef">
+        <control shapeId="9219" r:id="rId4" name="SetDateTimeMain">
           <controlPr print="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>2</xdr:row>
                 <xdr:rowOff>6350</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>12700</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -5140,12 +5138,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8193" r:id="rId4" name="SetDateTimeRef"/>
+        <control shapeId="9219" r:id="rId4" name="SetDateTimeMain"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8194" r:id="rId6" name="ToggleValues">
+        <control shapeId="9218" r:id="rId6" name="ToggleValues">
           <controlPr print="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -5165,24 +5163,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8194" r:id="rId6" name="ToggleValues"/>
+        <control shapeId="9218" r:id="rId6" name="ToggleValues"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8195" r:id="rId8" name="SetDateTimeMain">
+        <control shapeId="9217" r:id="rId8" name="SetDateTimeRef">
           <controlPr print="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>6350</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>12700</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -5190,7 +5188,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8195" r:id="rId8" name="SetDateTimeMain"/>
+        <control shapeId="9217" r:id="rId8" name="SetDateTimeRef"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -5199,14 +5197,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet4"/>
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:CQ50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="CR8" sqref="CR8"/>
+      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -5214,7 +5212,7 @@
     <col min="1" max="1" width="15" style="23" customWidth="1"/>
     <col min="2" max="2" width="12.26953125" style="33" customWidth="1"/>
     <col min="3" max="3" width="12.26953125" style="34" customWidth="1"/>
-    <col min="4" max="4" width="6.81640625" style="24" customWidth="1"/>
+    <col min="4" max="4" width="10.36328125" style="24" customWidth="1"/>
     <col min="5" max="25" width="6.81640625" style="23" customWidth="1"/>
     <col min="26" max="26" width="6.81640625" style="24" customWidth="1"/>
     <col min="27" max="48" width="6.81640625" style="23" customWidth="1"/>
@@ -5241,7 +5239,7 @@
       <c r="B1" s="5"/>
       <c r="C1" s="7"/>
       <c r="D1" s="3" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -5427,13 +5425,13 @@
         <v>51</v>
       </c>
       <c r="BN1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="BO1" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="BO1" s="2" t="s">
+      <c r="BP1" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="BP1" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="BQ1" s="2" t="s">
         <v>49</v>
@@ -5451,10 +5449,10 @@
         <v>43</v>
       </c>
       <c r="BV1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="BW1" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="BW1" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="BX1" s="2" t="s">
         <v>49</v>
@@ -5484,10 +5482,10 @@
         <v>84</v>
       </c>
       <c r="CG1" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="CH1" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="CI1" s="6" t="s">
         <v>87</v>
@@ -5755,7 +5753,7 @@
       </c>
       <c r="CF2" s="9"/>
       <c r="CG2" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="CH2" s="11" t="s">
         <v>38</v>
@@ -5986,12 +5984,9 @@
       </c>
       <c r="B5" s="29"/>
       <c r="C5" s="30"/>
-      <c r="D5" s="21">
-        <f>D3-D4</f>
-        <v>0</v>
-      </c>
+      <c r="D5" s="21"/>
       <c r="E5" s="43">
-        <f t="shared" ref="E5:BR5" si="0">E3-E4</f>
+        <f t="shared" ref="E5:BP5" si="0">E3-E4</f>
         <v>0</v>
       </c>
       <c r="F5" s="43">
@@ -6095,24 +6090,24 @@
         <v>0</v>
       </c>
       <c r="AE5" s="43">
-        <f t="shared" ref="AE5" si="1">AE3-AE4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AF5" s="43"/>
       <c r="AG5" s="43">
-        <f t="shared" ref="AG5" si="2">AG3-AG4</f>
+        <f t="shared" ref="AG5:AJ5" si="1">AG3-AG4</f>
         <v>0</v>
       </c>
       <c r="AH5" s="43">
-        <f t="shared" ref="AH5" si="3">AH3-AH4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AI5" s="43">
-        <f t="shared" ref="AI5" si="4">AI3-AI4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AJ5" s="43">
-        <f t="shared" ref="AJ5" si="5">AJ3-AJ4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AK5" s="43">
@@ -6241,96 +6236,96 @@
         <v>0</v>
       </c>
       <c r="BQ5" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="BQ5:CQ5" si="2">BQ3-BQ4</f>
         <v>0</v>
       </c>
       <c r="BR5" s="21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BS5" s="43">
-        <f t="shared" ref="BS5:CQ5" si="6">BS3-BS4</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BT5" s="43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BU5" s="43"/>
       <c r="BV5" s="43"/>
       <c r="BW5" s="43"/>
       <c r="BX5" s="43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BY5" s="21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BZ5" s="43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CA5" s="43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CB5" s="43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CC5" s="43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CD5" s="43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CE5" s="43"/>
       <c r="CF5" s="21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CG5" s="43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CH5" s="43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CI5" s="43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CJ5" s="43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CK5" s="43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CL5" s="43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CM5" s="43"/>
       <c r="CN5" s="21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CO5" s="43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CP5" s="43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CQ5" s="43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -6342,7 +6337,9 @@
       <c r="C6" s="8">
         <v>0.375</v>
       </c>
-      <c r="D6" s="17"/>
+      <c r="D6" s="17">
+        <v>1</v>
+      </c>
       <c r="E6" s="18">
         <v>60</v>
       </c>
@@ -6497,26 +6494,25 @@
         <v>0</v>
       </c>
       <c r="BF6" s="12">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="BG6" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BH6" s="12">
-        <v>1.6319999999999999</v>
+        <v>0</v>
       </c>
       <c r="BI6" s="12">
-        <v>1.333</v>
+        <v>0</v>
       </c>
       <c r="BJ6" s="12">
-        <v>1.095</v>
+        <v>0</v>
       </c>
       <c r="BK6" s="12">
-        <v>2.6524999999999999</v>
-      </c>
-      <c r="BL6" s="44">
-        <f>38/14</f>
-        <v>2.7142857142857144</v>
+        <v>0</v>
+      </c>
+      <c r="BL6" s="12">
+        <v>0</v>
       </c>
       <c r="BM6" s="12">
         <v>0.9</v>
@@ -6573,22 +6569,22 @@
       </c>
       <c r="CF6" s="17"/>
       <c r="CG6" s="18">
-        <v>24</v>
+        <v>6.3</v>
       </c>
       <c r="CH6" s="18">
         <v>0</v>
       </c>
       <c r="CI6" s="18">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="CJ6" s="18">
-        <v>8.0000000000000004E-4</v>
+        <v>0</v>
       </c>
       <c r="CK6" s="18">
-        <v>5.9999999999999995E-4</v>
+        <v>0</v>
       </c>
       <c r="CL6" s="18">
-        <v>5.9999999999999995E-4</v>
+        <v>0</v>
       </c>
       <c r="CM6" s="18">
         <v>0</v>
@@ -6598,7 +6594,7 @@
         <v>280</v>
       </c>
       <c r="CP6" s="18">
-        <v>9000</v>
+        <v>9900</v>
       </c>
       <c r="CQ6" s="18">
         <v>0</v>
@@ -6624,7 +6620,7 @@
       <c r="Q7" s="18"/>
       <c r="R7" s="18"/>
       <c r="S7" s="18"/>
-      <c r="T7" s="18"/>
+      <c r="T7" s="41"/>
       <c r="U7" s="18"/>
       <c r="V7" s="18"/>
       <c r="W7" s="18"/>
@@ -6639,6 +6635,7 @@
       <c r="AF7" s="18"/>
       <c r="AG7" s="18"/>
       <c r="AH7" s="18"/>
+      <c r="AI7" s="18"/>
       <c r="AJ7" s="18"/>
       <c r="AK7" s="18"/>
       <c r="AL7" s="18"/>
@@ -6658,7 +6655,7 @@
       <c r="AZ7" s="18"/>
       <c r="BA7" s="18"/>
       <c r="BB7" s="18"/>
-      <c r="BC7" s="18"/>
+      <c r="BC7" s="40"/>
       <c r="BD7" s="17"/>
       <c r="BE7" s="12"/>
       <c r="BF7" s="12"/>
@@ -6674,6 +6671,7 @@
       <c r="BP7" s="12"/>
       <c r="BQ7" s="12"/>
       <c r="BR7" s="17"/>
+      <c r="BS7" s="12"/>
       <c r="BT7" s="12"/>
       <c r="BU7" s="12"/>
       <c r="BV7" s="12"/>
@@ -8922,15 +8920,12 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
-  <ignoredErrors>
-    <ignoredError sqref="BL6" unlockedFormula="1"/>
-  </ignoredErrors>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="4097" r:id="rId4" name="SetDateTimeRef">
+        <control shapeId="8193" r:id="rId4" name="SetDateTimeRef">
           <controlPr print="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -8950,12 +8945,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="4097" r:id="rId4" name="SetDateTimeRef"/>
+        <control shapeId="8193" r:id="rId4" name="SetDateTimeRef"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="4098" r:id="rId6" name="ToggleValues">
+        <control shapeId="8194" r:id="rId6" name="ToggleValues">
           <controlPr print="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -8975,12 +8970,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="4098" r:id="rId6" name="ToggleValues"/>
+        <control shapeId="8194" r:id="rId6" name="ToggleValues"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="4099" r:id="rId8" name="SetDateTimeMain">
+        <control shapeId="8195" r:id="rId8" name="SetDateTimeMain">
           <controlPr print="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -9000,7 +8995,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="4099" r:id="rId8" name="SetDateTimeMain"/>
+        <control shapeId="8195" r:id="rId8" name="SetDateTimeMain"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
Reading in Torque, RPM, and HP as 0
Found MotorA is reading negative for the combustion, but the electric is
reading positive. May not be ideal for forwardG logic
</commit_message>
<xml_diff>
--- a/Functions/SetupSheets.xlsx
+++ b/Functions/SetupSheets.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="200" windowWidth="15200" windowHeight="7140" activeTab="1"/>
+    <workbookView xWindow="1820" yWindow="200" windowWidth="15200" windowHeight="7140"/>
   </bookViews>
   <sheets>
     <sheet name="Combustion" sheetId="10" r:id="rId1"/>
@@ -1395,11 +1395,11 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:CQ50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="5" topLeftCell="BD6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
+      <selection pane="bottomRight" activeCell="BF9" sqref="BF9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2684,7 +2684,7 @@
       </c>
       <c r="BD6" s="17"/>
       <c r="BE6" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF6" s="12">
         <v>3.5</v>
@@ -2702,10 +2702,10 @@
         <v>0</v>
       </c>
       <c r="BK6" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL6" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BM6" s="12">
         <v>0.9</v>
@@ -5200,7 +5200,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:CQ50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>

</xml_diff>

<commit_message>
Add lift, rho, and center of pressure to setup sheet.
</commit_message>
<xml_diff>
--- a/Functions/SetupSheets.xlsx
+++ b/Functions/SetupSheets.xlsx
@@ -5,22 +5,22 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Journey\Documents\GitHub\LapSimCombined\Functions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Code\LapSimCombined\Functions\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="200" windowWidth="15200" windowHeight="7140"/>
+    <workbookView xWindow="1815" yWindow="195" windowWidth="15195" windowHeight="7140" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Combustion" sheetId="10" r:id="rId1"/>
     <sheet name="Electric" sheetId="8" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="117">
   <si>
     <t>Date</t>
   </si>
@@ -356,6 +356,21 @@
   </si>
   <si>
     <t>Chassis Parameters</t>
+  </si>
+  <si>
+    <t>Lift</t>
+  </si>
+  <si>
+    <t>slug/ft3</t>
+  </si>
+  <si>
+    <t>CoP X</t>
+  </si>
+  <si>
+    <t>CoP Y</t>
+  </si>
+  <si>
+    <t>CoP Z</t>
   </si>
 </sst>
 </file>
@@ -502,7 +517,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -655,6 +670,10 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -705,11 +724,11 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>6350</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>12700</xdr:colOff>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -764,7 +783,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>12700</xdr:colOff>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -815,11 +834,11 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>6350</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>12700</xdr:colOff>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -930,11 +949,11 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>6350</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>12700</xdr:colOff>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -989,7 +1008,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>12700</xdr:colOff>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -1040,11 +1059,11 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>6350</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>12700</xdr:colOff>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -1395,39 +1414,39 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:CQ50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="BD6" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="5" topLeftCell="BB6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="BF9" sqref="BF9"/>
+      <selection pane="bottomRight" activeCell="CE1" sqref="CE1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" style="23" customWidth="1"/>
-    <col min="2" max="2" width="12.26953125" style="33" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" style="34" customWidth="1"/>
-    <col min="4" max="4" width="10.36328125" style="24" customWidth="1"/>
-    <col min="5" max="25" width="6.81640625" style="23" customWidth="1"/>
-    <col min="26" max="26" width="6.81640625" style="24" customWidth="1"/>
-    <col min="27" max="48" width="6.81640625" style="23" customWidth="1"/>
-    <col min="49" max="49" width="6.81640625" style="24" customWidth="1"/>
-    <col min="50" max="54" width="6.81640625" style="23" customWidth="1"/>
-    <col min="55" max="55" width="10.81640625" style="23" customWidth="1"/>
-    <col min="56" max="56" width="6.81640625" style="24" customWidth="1"/>
-    <col min="57" max="69" width="6.81640625" style="23" customWidth="1"/>
-    <col min="70" max="70" width="6.81640625" style="24" customWidth="1"/>
-    <col min="71" max="76" width="6.81640625" style="23" customWidth="1"/>
-    <col min="77" max="77" width="6.81640625" style="24" customWidth="1"/>
-    <col min="78" max="83" width="6.81640625" style="23" customWidth="1"/>
-    <col min="84" max="84" width="6.81640625" style="24" customWidth="1"/>
-    <col min="85" max="91" width="6.81640625" style="23" customWidth="1"/>
-    <col min="92" max="92" width="6.81640625" style="24" customWidth="1"/>
-    <col min="93" max="95" width="6.81640625" style="23" customWidth="1"/>
-    <col min="96" max="16384" width="9.1796875" style="23"/>
+    <col min="2" max="2" width="12.28515625" style="33" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="34" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="24" customWidth="1"/>
+    <col min="5" max="25" width="6.85546875" style="23" customWidth="1"/>
+    <col min="26" max="26" width="6.85546875" style="24" customWidth="1"/>
+    <col min="27" max="48" width="6.85546875" style="23" customWidth="1"/>
+    <col min="49" max="49" width="6.85546875" style="24" customWidth="1"/>
+    <col min="50" max="54" width="6.85546875" style="23" customWidth="1"/>
+    <col min="55" max="55" width="10.85546875" style="23" customWidth="1"/>
+    <col min="56" max="56" width="6.85546875" style="24" customWidth="1"/>
+    <col min="57" max="69" width="6.85546875" style="23" customWidth="1"/>
+    <col min="70" max="70" width="6.85546875" style="24" customWidth="1"/>
+    <col min="71" max="76" width="6.85546875" style="23" customWidth="1"/>
+    <col min="77" max="77" width="6.85546875" style="24" customWidth="1"/>
+    <col min="78" max="83" width="6.85546875" style="23" customWidth="1"/>
+    <col min="84" max="84" width="6.85546875" style="24" customWidth="1"/>
+    <col min="85" max="91" width="6.85546875" style="23" customWidth="1"/>
+    <col min="92" max="92" width="6.85546875" style="24" customWidth="1"/>
+    <col min="93" max="95" width="6.85546875" style="23" customWidth="1"/>
+    <col min="96" max="16384" width="9.140625" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:95" s="25" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:95" s="25" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="35" t="s">
         <v>35</v>
       </c>
@@ -1710,7 +1729,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:95" s="28" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:95" s="28" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="36"/>
       <c r="B2" s="26" t="s">
         <v>0</v>
@@ -1979,7 +1998,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:95" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:95" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="37"/>
       <c r="B3" s="29"/>
       <c r="C3" s="30"/>
@@ -2076,7 +2095,7 @@
       <c r="CP3" s="15"/>
       <c r="CQ3" s="15"/>
     </row>
-    <row r="4" spans="1:95" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:95" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="37"/>
       <c r="B4" s="29"/>
       <c r="C4" s="30"/>
@@ -2173,7 +2192,7 @@
       <c r="CP4" s="15"/>
       <c r="CQ4" s="15"/>
     </row>
-    <row r="5" spans="1:95" s="22" customFormat="1" ht="13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:95" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="37" t="s">
         <v>36</v>
       </c>
@@ -2524,7 +2543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:95" ht="13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:95" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="16"/>
       <c r="B6" s="1">
         <v>35065</v>
@@ -2793,7 +2812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:95" ht="13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A7" s="16"/>
       <c r="B7" s="1"/>
       <c r="C7" s="8"/>
@@ -2890,7 +2909,7 @@
       <c r="CP7" s="18"/>
       <c r="CQ7" s="18"/>
     </row>
-    <row r="8" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A8" s="19"/>
       <c r="B8" s="1"/>
       <c r="C8" s="8"/>
@@ -2986,7 +3005,7 @@
       <c r="CP8" s="18"/>
       <c r="CQ8" s="18"/>
     </row>
-    <row r="9" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A9" s="19"/>
       <c r="B9" s="1"/>
       <c r="C9" s="8"/>
@@ -3083,7 +3102,7 @@
       <c r="CP9" s="18"/>
       <c r="CQ9" s="18"/>
     </row>
-    <row r="10" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A10" s="19"/>
       <c r="B10" s="1"/>
       <c r="C10" s="8"/>
@@ -3180,7 +3199,7 @@
       <c r="CP10" s="18"/>
       <c r="CQ10" s="18"/>
     </row>
-    <row r="11" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A11" s="19"/>
       <c r="B11" s="1"/>
       <c r="C11" s="8"/>
@@ -3277,7 +3296,7 @@
       <c r="CP11" s="18"/>
       <c r="CQ11" s="18"/>
     </row>
-    <row r="12" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A12" s="19"/>
       <c r="B12" s="1"/>
       <c r="C12" s="8"/>
@@ -3374,7 +3393,7 @@
       <c r="CP12" s="18"/>
       <c r="CQ12" s="18"/>
     </row>
-    <row r="13" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A13" s="19"/>
       <c r="B13" s="1"/>
       <c r="C13" s="8"/>
@@ -3471,7 +3490,7 @@
       <c r="CP13" s="18"/>
       <c r="CQ13" s="18"/>
     </row>
-    <row r="14" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A14" s="19"/>
       <c r="B14" s="1"/>
       <c r="C14" s="8"/>
@@ -3568,7 +3587,7 @@
       <c r="CP14" s="18"/>
       <c r="CQ14" s="18"/>
     </row>
-    <row r="15" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A15" s="19"/>
       <c r="B15" s="1"/>
       <c r="C15" s="8"/>
@@ -3665,7 +3684,7 @@
       <c r="CP15" s="18"/>
       <c r="CQ15" s="18"/>
     </row>
-    <row r="16" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A16" s="19"/>
       <c r="B16" s="1"/>
       <c r="C16" s="8"/>
@@ -3762,7 +3781,7 @@
       <c r="CP16" s="18"/>
       <c r="CQ16" s="18"/>
     </row>
-    <row r="17" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A17" s="19"/>
       <c r="B17" s="1"/>
       <c r="C17" s="8"/>
@@ -3859,7 +3878,7 @@
       <c r="CP17" s="18"/>
       <c r="CQ17" s="18"/>
     </row>
-    <row r="18" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A18" s="19"/>
       <c r="B18" s="1"/>
       <c r="C18" s="8"/>
@@ -3956,7 +3975,7 @@
       <c r="CP18" s="18"/>
       <c r="CQ18" s="18"/>
     </row>
-    <row r="19" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A19" s="19"/>
       <c r="B19" s="1"/>
       <c r="C19" s="8"/>
@@ -4053,7 +4072,7 @@
       <c r="CP19" s="18"/>
       <c r="CQ19" s="18"/>
     </row>
-    <row r="20" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A20" s="19"/>
       <c r="B20" s="1"/>
       <c r="C20" s="8"/>
@@ -4150,7 +4169,7 @@
       <c r="CP20" s="18"/>
       <c r="CQ20" s="18"/>
     </row>
-    <row r="21" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A21" s="19"/>
       <c r="B21" s="1"/>
       <c r="C21" s="8"/>
@@ -4247,7 +4266,7 @@
       <c r="CP21" s="18"/>
       <c r="CQ21" s="18"/>
     </row>
-    <row r="22" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A22" s="19"/>
       <c r="B22" s="1"/>
       <c r="C22" s="8"/>
@@ -4344,7 +4363,7 @@
       <c r="CP22" s="18"/>
       <c r="CQ22" s="18"/>
     </row>
-    <row r="23" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A23" s="19"/>
       <c r="B23" s="1"/>
       <c r="C23" s="8"/>
@@ -4441,7 +4460,7 @@
       <c r="CP23" s="18"/>
       <c r="CQ23" s="18"/>
     </row>
-    <row r="24" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A24" s="19"/>
       <c r="B24" s="1"/>
       <c r="C24" s="8"/>
@@ -4538,7 +4557,7 @@
       <c r="CP24" s="18"/>
       <c r="CQ24" s="18"/>
     </row>
-    <row r="25" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A25" s="19"/>
       <c r="B25" s="1"/>
       <c r="C25" s="8"/>
@@ -4635,7 +4654,7 @@
       <c r="CP25" s="18"/>
       <c r="CQ25" s="18"/>
     </row>
-    <row r="26" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A26" s="19"/>
       <c r="B26" s="1"/>
       <c r="C26" s="8"/>
@@ -4732,7 +4751,7 @@
       <c r="CP26" s="18"/>
       <c r="CQ26" s="18"/>
     </row>
-    <row r="27" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A27" s="19"/>
       <c r="B27" s="1"/>
       <c r="C27" s="8"/>
@@ -4829,7 +4848,7 @@
       <c r="CP27" s="18"/>
       <c r="CQ27" s="18"/>
     </row>
-    <row r="28" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A28" s="19"/>
       <c r="B28" s="1"/>
       <c r="C28" s="8"/>
@@ -4926,7 +4945,7 @@
       <c r="CP28" s="18"/>
       <c r="CQ28" s="18"/>
     </row>
-    <row r="29" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A29" s="19"/>
       <c r="B29" s="1"/>
       <c r="C29" s="8"/>
@@ -5023,87 +5042,87 @@
       <c r="CP29" s="18"/>
       <c r="CQ29" s="18"/>
     </row>
-    <row r="30" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:95" x14ac:dyDescent="0.2">
       <c r="B30" s="31"/>
       <c r="C30" s="32"/>
     </row>
-    <row r="31" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:95" x14ac:dyDescent="0.2">
       <c r="B31" s="31"/>
       <c r="C31" s="32"/>
     </row>
-    <row r="32" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:95" x14ac:dyDescent="0.2">
       <c r="B32" s="31"/>
       <c r="C32" s="32"/>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B33" s="31"/>
       <c r="C33" s="32"/>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B34" s="31"/>
       <c r="C34" s="32"/>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B35" s="31"/>
       <c r="C35" s="32"/>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B36" s="31"/>
       <c r="C36" s="32"/>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B37" s="31"/>
       <c r="C37" s="32"/>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B38" s="31"/>
       <c r="C38" s="32"/>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B39" s="31"/>
       <c r="C39" s="32"/>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B40" s="31"/>
       <c r="C40" s="32"/>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B41" s="31"/>
       <c r="C41" s="32"/>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B42" s="31"/>
       <c r="C42" s="32"/>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B43" s="31"/>
       <c r="C43" s="32"/>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B44" s="31"/>
       <c r="C44" s="32"/>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B45" s="31"/>
       <c r="C45" s="32"/>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B46" s="31"/>
       <c r="C46" s="32"/>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B47" s="31"/>
       <c r="C47" s="32"/>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B48" s="31"/>
       <c r="C48" s="32"/>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B49" s="31"/>
       <c r="C49" s="32"/>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B50" s="31"/>
       <c r="C50" s="32"/>
     </row>
@@ -5118,19 +5137,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="9219" r:id="rId4" name="SetDateTimeMain">
+        <control shapeId="9217" r:id="rId4" name="SetDateTimeRef">
           <controlPr print="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>6350</xdr:rowOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>12700</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -5138,7 +5157,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="9219" r:id="rId4" name="SetDateTimeMain"/>
+        <control shapeId="9217" r:id="rId4" name="SetDateTimeRef"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -5154,7 +5173,7 @@
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>12700</xdr:colOff>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
@@ -5168,19 +5187,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="9217" r:id="rId8" name="SetDateTimeRef">
+        <control shapeId="9219" r:id="rId8" name="SetDateTimeMain">
           <controlPr print="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>6350</xdr:rowOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>12700</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -5188,7 +5207,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="9217" r:id="rId8" name="SetDateTimeRef"/>
+        <control shapeId="9219" r:id="rId8" name="SetDateTimeMain"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -5198,41 +5217,41 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:CQ50"/>
+  <dimension ref="A1:CU50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="5" topLeftCell="BT6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomRight" activeCell="CH7" sqref="CH7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" style="23" customWidth="1"/>
-    <col min="2" max="2" width="12.26953125" style="33" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" style="34" customWidth="1"/>
-    <col min="4" max="4" width="10.36328125" style="24" customWidth="1"/>
-    <col min="5" max="25" width="6.81640625" style="23" customWidth="1"/>
-    <col min="26" max="26" width="6.81640625" style="24" customWidth="1"/>
-    <col min="27" max="48" width="6.81640625" style="23" customWidth="1"/>
-    <col min="49" max="49" width="6.81640625" style="24" customWidth="1"/>
-    <col min="50" max="54" width="6.81640625" style="23" customWidth="1"/>
-    <col min="55" max="55" width="10.81640625" style="23" customWidth="1"/>
-    <col min="56" max="56" width="6.81640625" style="24" customWidth="1"/>
-    <col min="57" max="69" width="6.81640625" style="23" customWidth="1"/>
-    <col min="70" max="70" width="6.81640625" style="24" customWidth="1"/>
-    <col min="71" max="76" width="6.81640625" style="23" customWidth="1"/>
-    <col min="77" max="77" width="6.81640625" style="24" customWidth="1"/>
-    <col min="78" max="83" width="6.81640625" style="23" customWidth="1"/>
-    <col min="84" max="84" width="6.81640625" style="24" customWidth="1"/>
-    <col min="85" max="91" width="6.81640625" style="23" customWidth="1"/>
-    <col min="92" max="92" width="6.81640625" style="24" customWidth="1"/>
-    <col min="93" max="95" width="6.81640625" style="23" customWidth="1"/>
-    <col min="96" max="16384" width="9.1796875" style="23"/>
+    <col min="2" max="2" width="12.28515625" style="33" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="34" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="24" customWidth="1"/>
+    <col min="5" max="25" width="6.85546875" style="23" customWidth="1"/>
+    <col min="26" max="26" width="6.85546875" style="24" customWidth="1"/>
+    <col min="27" max="48" width="6.85546875" style="23" customWidth="1"/>
+    <col min="49" max="49" width="6.85546875" style="24" customWidth="1"/>
+    <col min="50" max="54" width="6.85546875" style="23" customWidth="1"/>
+    <col min="55" max="55" width="10.85546875" style="23" customWidth="1"/>
+    <col min="56" max="56" width="6.85546875" style="24" customWidth="1"/>
+    <col min="57" max="69" width="6.85546875" style="23" customWidth="1"/>
+    <col min="70" max="70" width="6.85546875" style="24" customWidth="1"/>
+    <col min="71" max="76" width="6.85546875" style="23" customWidth="1"/>
+    <col min="77" max="77" width="6.85546875" style="24" customWidth="1"/>
+    <col min="78" max="87" width="6.85546875" style="23" customWidth="1"/>
+    <col min="88" max="88" width="6.85546875" style="24" customWidth="1"/>
+    <col min="89" max="95" width="6.85546875" style="23" customWidth="1"/>
+    <col min="96" max="96" width="6.85546875" style="24" customWidth="1"/>
+    <col min="97" max="99" width="6.85546875" style="23" customWidth="1"/>
+    <col min="100" max="16384" width="9.140625" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:95" s="25" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:99" s="25" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="35" t="s">
         <v>35</v>
       </c>
@@ -5473,49 +5492,61 @@
         <v>53</v>
       </c>
       <c r="CD1" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="CE1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="CE1" s="2" t="s">
+      <c r="CF1" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="CF1" s="3" t="s">
+      <c r="CG1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="CH1" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="CI1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="CJ1" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="CG1" s="6" t="s">
+      <c r="CK1" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="CH1" s="6" t="s">
+      <c r="CL1" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="CI1" s="6" t="s">
+      <c r="CM1" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="CJ1" s="6" t="s">
+      <c r="CN1" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="CK1" s="6" t="s">
+      <c r="CO1" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="CL1" s="6" t="s">
+      <c r="CP1" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="CM1" s="6" t="s">
+      <c r="CQ1" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="CN1" s="3" t="s">
+      <c r="CR1" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="CO1" s="6" t="s">
+      <c r="CS1" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="CP1" s="6" t="s">
+      <c r="CT1" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="CQ1" s="6" t="s">
+      <c r="CU1" s="6" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:95" s="28" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:99" s="28" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="36"/>
       <c r="B2" s="26" t="s">
         <v>0</v>
@@ -5746,45 +5777,57 @@
         <v>56</v>
       </c>
       <c r="CD2" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="CE2" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="CE2" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="CF2" s="9"/>
-      <c r="CG2" s="11" t="s">
+      <c r="CF2" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="CG2" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="CH2" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="CI2" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="CJ2" s="9"/>
+      <c r="CK2" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="CH2" s="11" t="s">
+      <c r="CL2" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="CI2" s="42" t="s">
+      <c r="CM2" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="CJ2" s="42" t="s">
+      <c r="CN2" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="CK2" s="42" t="s">
+      <c r="CO2" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="CL2" s="42" t="s">
+      <c r="CP2" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="CM2" s="42" t="s">
+      <c r="CQ2" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="CN2" s="9"/>
-      <c r="CO2" s="11" t="s">
+      <c r="CR2" s="9"/>
+      <c r="CS2" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="CP2" s="11" t="s">
+      <c r="CT2" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="CQ2" s="11" t="s">
+      <c r="CU2" s="11" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:95" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:99" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="37"/>
       <c r="B3" s="29"/>
       <c r="C3" s="30"/>
@@ -5868,20 +5911,24 @@
       <c r="CC3" s="13"/>
       <c r="CD3" s="13"/>
       <c r="CE3" s="13"/>
-      <c r="CF3" s="14"/>
-      <c r="CG3" s="15"/>
-      <c r="CH3" s="15"/>
-      <c r="CI3" s="15"/>
-      <c r="CJ3" s="15"/>
+      <c r="CF3" s="13"/>
+      <c r="CG3" s="13"/>
+      <c r="CH3" s="13"/>
+      <c r="CI3" s="13"/>
+      <c r="CJ3" s="14"/>
       <c r="CK3" s="15"/>
       <c r="CL3" s="15"/>
       <c r="CM3" s="15"/>
-      <c r="CN3" s="14"/>
+      <c r="CN3" s="15"/>
       <c r="CO3" s="15"/>
       <c r="CP3" s="15"/>
       <c r="CQ3" s="15"/>
-    </row>
-    <row r="4" spans="1:95" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CR3" s="14"/>
+      <c r="CS3" s="15"/>
+      <c r="CT3" s="15"/>
+      <c r="CU3" s="15"/>
+    </row>
+    <row r="4" spans="1:99" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="37"/>
       <c r="B4" s="29"/>
       <c r="C4" s="30"/>
@@ -5965,20 +6012,24 @@
       <c r="CC4" s="13"/>
       <c r="CD4" s="13"/>
       <c r="CE4" s="13"/>
-      <c r="CF4" s="14"/>
-      <c r="CG4" s="15"/>
-      <c r="CH4" s="15"/>
-      <c r="CI4" s="15"/>
-      <c r="CJ4" s="15"/>
+      <c r="CF4" s="13"/>
+      <c r="CG4" s="13"/>
+      <c r="CH4" s="13"/>
+      <c r="CI4" s="13"/>
+      <c r="CJ4" s="14"/>
       <c r="CK4" s="15"/>
       <c r="CL4" s="15"/>
       <c r="CM4" s="15"/>
-      <c r="CN4" s="14"/>
+      <c r="CN4" s="15"/>
       <c r="CO4" s="15"/>
       <c r="CP4" s="15"/>
       <c r="CQ4" s="15"/>
-    </row>
-    <row r="5" spans="1:95" s="22" customFormat="1" ht="13" x14ac:dyDescent="0.25">
+      <c r="CR4" s="14"/>
+      <c r="CS4" s="15"/>
+      <c r="CT4" s="15"/>
+      <c r="CU4" s="15"/>
+    </row>
+    <row r="5" spans="1:99" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="37" t="s">
         <v>36</v>
       </c>
@@ -6236,7 +6287,7 @@
         <v>0</v>
       </c>
       <c r="BQ5" s="43">
-        <f t="shared" ref="BQ5:CQ5" si="2">BQ3-BQ4</f>
+        <f t="shared" ref="BQ5:CU5" si="2">BQ3-BQ4</f>
         <v>0</v>
       </c>
       <c r="BR5" s="21">
@@ -6278,28 +6329,16 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="CD5" s="43">
+      <c r="CD5" s="43"/>
+      <c r="CE5" s="43">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="CE5" s="43"/>
-      <c r="CF5" s="21">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="CG5" s="43">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="CH5" s="43">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="CI5" s="43">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="CJ5" s="43">
+      <c r="CF5" s="43"/>
+      <c r="CG5" s="43"/>
+      <c r="CH5" s="43"/>
+      <c r="CI5" s="43"/>
+      <c r="CJ5" s="21">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -6311,8 +6350,11 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="CM5" s="43"/>
-      <c r="CN5" s="21">
+      <c r="CM5" s="43">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="CN5" s="43">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -6324,12 +6366,25 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="CQ5" s="43">
+      <c r="CQ5" s="43"/>
+      <c r="CR5" s="21">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:95" ht="13" x14ac:dyDescent="0.25">
+      <c r="CS5" s="43">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="CT5" s="43">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="CU5" s="43">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:99" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="16"/>
       <c r="B6" s="1">
         <v>35065</v>
@@ -6562,45 +6617,57 @@
         <v>0.6</v>
       </c>
       <c r="CD6" s="12">
+        <v>0.6</v>
+      </c>
+      <c r="CE6" s="12">
         <v>2015</v>
       </c>
-      <c r="CE6" s="12">
-        <v>0</v>
-      </c>
-      <c r="CF6" s="17"/>
-      <c r="CG6" s="18">
+      <c r="CF6" s="12">
+        <v>0</v>
+      </c>
+      <c r="CG6" s="12">
+        <v>34.25</v>
+      </c>
+      <c r="CH6" s="12">
+        <v>0</v>
+      </c>
+      <c r="CI6" s="12">
+        <v>13</v>
+      </c>
+      <c r="CJ6" s="17"/>
+      <c r="CK6" s="18">
         <v>6.3</v>
       </c>
-      <c r="CH6" s="18">
-        <v>0</v>
-      </c>
-      <c r="CI6" s="18">
-        <v>0</v>
-      </c>
-      <c r="CJ6" s="18">
-        <v>0</v>
-      </c>
-      <c r="CK6" s="18">
-        <v>0</v>
-      </c>
       <c r="CL6" s="18">
         <v>0</v>
       </c>
       <c r="CM6" s="18">
         <v>0</v>
       </c>
-      <c r="CN6" s="17"/>
+      <c r="CN6" s="18">
+        <v>0</v>
+      </c>
       <c r="CO6" s="18">
+        <v>0</v>
+      </c>
+      <c r="CP6" s="18">
+        <v>0</v>
+      </c>
+      <c r="CQ6" s="18">
+        <v>0</v>
+      </c>
+      <c r="CR6" s="17"/>
+      <c r="CS6" s="18">
         <v>280</v>
       </c>
-      <c r="CP6" s="18">
+      <c r="CT6" s="18">
         <v>9900</v>
       </c>
-      <c r="CQ6" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:95" ht="13" x14ac:dyDescent="0.25">
+      <c r="CU6" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A7" s="16"/>
       <c r="B7" s="1"/>
       <c r="C7" s="8"/>
@@ -6684,20 +6751,24 @@
       <c r="CC7" s="12"/>
       <c r="CD7" s="12"/>
       <c r="CE7" s="12"/>
-      <c r="CF7" s="17"/>
-      <c r="CG7" s="18"/>
-      <c r="CH7" s="18"/>
-      <c r="CI7" s="18"/>
-      <c r="CJ7" s="18"/>
+      <c r="CF7" s="12"/>
+      <c r="CG7" s="12"/>
+      <c r="CH7" s="12"/>
+      <c r="CI7" s="12"/>
+      <c r="CJ7" s="17"/>
       <c r="CK7" s="18"/>
       <c r="CL7" s="18"/>
       <c r="CM7" s="18"/>
-      <c r="CN7" s="17"/>
+      <c r="CN7" s="18"/>
       <c r="CO7" s="18"/>
       <c r="CP7" s="18"/>
       <c r="CQ7" s="18"/>
-    </row>
-    <row r="8" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="CR7" s="17"/>
+      <c r="CS7" s="18"/>
+      <c r="CT7" s="18"/>
+      <c r="CU7" s="18"/>
+    </row>
+    <row r="8" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A8" s="19"/>
       <c r="B8" s="1"/>
       <c r="C8" s="8"/>
@@ -6780,20 +6851,24 @@
       <c r="CC8" s="12"/>
       <c r="CD8" s="12"/>
       <c r="CE8" s="12"/>
-      <c r="CF8" s="17"/>
-      <c r="CG8" s="18"/>
-      <c r="CH8" s="18"/>
-      <c r="CI8" s="18"/>
-      <c r="CJ8" s="18"/>
+      <c r="CF8" s="12"/>
+      <c r="CG8" s="12"/>
+      <c r="CH8" s="12"/>
+      <c r="CI8" s="12"/>
+      <c r="CJ8" s="17"/>
       <c r="CK8" s="18"/>
       <c r="CL8" s="18"/>
       <c r="CM8" s="18"/>
-      <c r="CN8" s="17"/>
+      <c r="CN8" s="18"/>
       <c r="CO8" s="18"/>
       <c r="CP8" s="18"/>
       <c r="CQ8" s="18"/>
-    </row>
-    <row r="9" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="CR8" s="17"/>
+      <c r="CS8" s="18"/>
+      <c r="CT8" s="18"/>
+      <c r="CU8" s="18"/>
+    </row>
+    <row r="9" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A9" s="19"/>
       <c r="B9" s="1"/>
       <c r="C9" s="8"/>
@@ -6877,20 +6952,24 @@
       <c r="CC9" s="18"/>
       <c r="CD9" s="18"/>
       <c r="CE9" s="18"/>
-      <c r="CF9" s="17"/>
+      <c r="CF9" s="18"/>
       <c r="CG9" s="18"/>
       <c r="CH9" s="18"/>
       <c r="CI9" s="18"/>
-      <c r="CJ9" s="18"/>
+      <c r="CJ9" s="17"/>
       <c r="CK9" s="18"/>
       <c r="CL9" s="18"/>
       <c r="CM9" s="18"/>
-      <c r="CN9" s="17"/>
+      <c r="CN9" s="18"/>
       <c r="CO9" s="18"/>
       <c r="CP9" s="18"/>
       <c r="CQ9" s="18"/>
-    </row>
-    <row r="10" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="CR9" s="17"/>
+      <c r="CS9" s="18"/>
+      <c r="CT9" s="18"/>
+      <c r="CU9" s="18"/>
+    </row>
+    <row r="10" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A10" s="19"/>
       <c r="B10" s="1"/>
       <c r="C10" s="8"/>
@@ -6974,20 +7053,24 @@
       <c r="CC10" s="18"/>
       <c r="CD10" s="18"/>
       <c r="CE10" s="18"/>
-      <c r="CF10" s="17"/>
+      <c r="CF10" s="18"/>
       <c r="CG10" s="18"/>
       <c r="CH10" s="18"/>
       <c r="CI10" s="18"/>
-      <c r="CJ10" s="18"/>
+      <c r="CJ10" s="17"/>
       <c r="CK10" s="18"/>
       <c r="CL10" s="18"/>
       <c r="CM10" s="18"/>
-      <c r="CN10" s="17"/>
+      <c r="CN10" s="18"/>
       <c r="CO10" s="18"/>
       <c r="CP10" s="18"/>
       <c r="CQ10" s="18"/>
-    </row>
-    <row r="11" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="CR10" s="17"/>
+      <c r="CS10" s="18"/>
+      <c r="CT10" s="18"/>
+      <c r="CU10" s="18"/>
+    </row>
+    <row r="11" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A11" s="19"/>
       <c r="B11" s="1"/>
       <c r="C11" s="8"/>
@@ -7071,20 +7154,24 @@
       <c r="CC11" s="18"/>
       <c r="CD11" s="18"/>
       <c r="CE11" s="18"/>
-      <c r="CF11" s="17"/>
+      <c r="CF11" s="18"/>
       <c r="CG11" s="18"/>
       <c r="CH11" s="18"/>
       <c r="CI11" s="18"/>
-      <c r="CJ11" s="18"/>
+      <c r="CJ11" s="17"/>
       <c r="CK11" s="18"/>
       <c r="CL11" s="18"/>
       <c r="CM11" s="18"/>
-      <c r="CN11" s="17"/>
+      <c r="CN11" s="18"/>
       <c r="CO11" s="18"/>
       <c r="CP11" s="18"/>
       <c r="CQ11" s="18"/>
-    </row>
-    <row r="12" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="CR11" s="17"/>
+      <c r="CS11" s="18"/>
+      <c r="CT11" s="18"/>
+      <c r="CU11" s="18"/>
+    </row>
+    <row r="12" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A12" s="19"/>
       <c r="B12" s="1"/>
       <c r="C12" s="8"/>
@@ -7168,20 +7255,24 @@
       <c r="CC12" s="18"/>
       <c r="CD12" s="18"/>
       <c r="CE12" s="18"/>
-      <c r="CF12" s="17"/>
+      <c r="CF12" s="18"/>
       <c r="CG12" s="18"/>
       <c r="CH12" s="18"/>
       <c r="CI12" s="18"/>
-      <c r="CJ12" s="18"/>
+      <c r="CJ12" s="17"/>
       <c r="CK12" s="18"/>
       <c r="CL12" s="18"/>
       <c r="CM12" s="18"/>
-      <c r="CN12" s="17"/>
+      <c r="CN12" s="18"/>
       <c r="CO12" s="18"/>
       <c r="CP12" s="18"/>
       <c r="CQ12" s="18"/>
-    </row>
-    <row r="13" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="CR12" s="17"/>
+      <c r="CS12" s="18"/>
+      <c r="CT12" s="18"/>
+      <c r="CU12" s="18"/>
+    </row>
+    <row r="13" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A13" s="19"/>
       <c r="B13" s="1"/>
       <c r="C13" s="8"/>
@@ -7265,20 +7356,24 @@
       <c r="CC13" s="18"/>
       <c r="CD13" s="18"/>
       <c r="CE13" s="18"/>
-      <c r="CF13" s="17"/>
+      <c r="CF13" s="18"/>
       <c r="CG13" s="18"/>
       <c r="CH13" s="18"/>
       <c r="CI13" s="18"/>
-      <c r="CJ13" s="18"/>
+      <c r="CJ13" s="17"/>
       <c r="CK13" s="18"/>
       <c r="CL13" s="18"/>
       <c r="CM13" s="18"/>
-      <c r="CN13" s="17"/>
+      <c r="CN13" s="18"/>
       <c r="CO13" s="18"/>
       <c r="CP13" s="18"/>
       <c r="CQ13" s="18"/>
-    </row>
-    <row r="14" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="CR13" s="17"/>
+      <c r="CS13" s="18"/>
+      <c r="CT13" s="18"/>
+      <c r="CU13" s="18"/>
+    </row>
+    <row r="14" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A14" s="19"/>
       <c r="B14" s="1"/>
       <c r="C14" s="8"/>
@@ -7362,20 +7457,24 @@
       <c r="CC14" s="18"/>
       <c r="CD14" s="18"/>
       <c r="CE14" s="18"/>
-      <c r="CF14" s="17"/>
+      <c r="CF14" s="18"/>
       <c r="CG14" s="18"/>
       <c r="CH14" s="18"/>
       <c r="CI14" s="18"/>
-      <c r="CJ14" s="18"/>
+      <c r="CJ14" s="17"/>
       <c r="CK14" s="18"/>
       <c r="CL14" s="18"/>
       <c r="CM14" s="18"/>
-      <c r="CN14" s="17"/>
+      <c r="CN14" s="18"/>
       <c r="CO14" s="18"/>
       <c r="CP14" s="18"/>
       <c r="CQ14" s="18"/>
-    </row>
-    <row r="15" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="CR14" s="17"/>
+      <c r="CS14" s="18"/>
+      <c r="CT14" s="18"/>
+      <c r="CU14" s="18"/>
+    </row>
+    <row r="15" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A15" s="19"/>
       <c r="B15" s="1"/>
       <c r="C15" s="8"/>
@@ -7459,20 +7558,24 @@
       <c r="CC15" s="18"/>
       <c r="CD15" s="18"/>
       <c r="CE15" s="18"/>
-      <c r="CF15" s="17"/>
+      <c r="CF15" s="18"/>
       <c r="CG15" s="18"/>
       <c r="CH15" s="18"/>
       <c r="CI15" s="18"/>
-      <c r="CJ15" s="18"/>
+      <c r="CJ15" s="17"/>
       <c r="CK15" s="18"/>
       <c r="CL15" s="18"/>
       <c r="CM15" s="18"/>
-      <c r="CN15" s="17"/>
+      <c r="CN15" s="18"/>
       <c r="CO15" s="18"/>
       <c r="CP15" s="18"/>
       <c r="CQ15" s="18"/>
-    </row>
-    <row r="16" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="CR15" s="17"/>
+      <c r="CS15" s="18"/>
+      <c r="CT15" s="18"/>
+      <c r="CU15" s="18"/>
+    </row>
+    <row r="16" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A16" s="19"/>
       <c r="B16" s="1"/>
       <c r="C16" s="8"/>
@@ -7556,20 +7659,24 @@
       <c r="CC16" s="18"/>
       <c r="CD16" s="18"/>
       <c r="CE16" s="18"/>
-      <c r="CF16" s="17"/>
+      <c r="CF16" s="18"/>
       <c r="CG16" s="18"/>
       <c r="CH16" s="18"/>
       <c r="CI16" s="18"/>
-      <c r="CJ16" s="18"/>
+      <c r="CJ16" s="17"/>
       <c r="CK16" s="18"/>
       <c r="CL16" s="18"/>
       <c r="CM16" s="18"/>
-      <c r="CN16" s="17"/>
+      <c r="CN16" s="18"/>
       <c r="CO16" s="18"/>
       <c r="CP16" s="18"/>
       <c r="CQ16" s="18"/>
-    </row>
-    <row r="17" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="CR16" s="17"/>
+      <c r="CS16" s="18"/>
+      <c r="CT16" s="18"/>
+      <c r="CU16" s="18"/>
+    </row>
+    <row r="17" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A17" s="19"/>
       <c r="B17" s="1"/>
       <c r="C17" s="8"/>
@@ -7653,20 +7760,24 @@
       <c r="CC17" s="18"/>
       <c r="CD17" s="18"/>
       <c r="CE17" s="18"/>
-      <c r="CF17" s="17"/>
+      <c r="CF17" s="18"/>
       <c r="CG17" s="18"/>
       <c r="CH17" s="18"/>
       <c r="CI17" s="18"/>
-      <c r="CJ17" s="18"/>
+      <c r="CJ17" s="17"/>
       <c r="CK17" s="18"/>
       <c r="CL17" s="18"/>
       <c r="CM17" s="18"/>
-      <c r="CN17" s="17"/>
+      <c r="CN17" s="18"/>
       <c r="CO17" s="18"/>
       <c r="CP17" s="18"/>
       <c r="CQ17" s="18"/>
-    </row>
-    <row r="18" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="CR17" s="17"/>
+      <c r="CS17" s="18"/>
+      <c r="CT17" s="18"/>
+      <c r="CU17" s="18"/>
+    </row>
+    <row r="18" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A18" s="19"/>
       <c r="B18" s="1"/>
       <c r="C18" s="8"/>
@@ -7750,20 +7861,24 @@
       <c r="CC18" s="18"/>
       <c r="CD18" s="18"/>
       <c r="CE18" s="18"/>
-      <c r="CF18" s="17"/>
+      <c r="CF18" s="18"/>
       <c r="CG18" s="18"/>
       <c r="CH18" s="18"/>
       <c r="CI18" s="18"/>
-      <c r="CJ18" s="18"/>
+      <c r="CJ18" s="17"/>
       <c r="CK18" s="18"/>
       <c r="CL18" s="18"/>
       <c r="CM18" s="18"/>
-      <c r="CN18" s="17"/>
+      <c r="CN18" s="18"/>
       <c r="CO18" s="18"/>
       <c r="CP18" s="18"/>
       <c r="CQ18" s="18"/>
-    </row>
-    <row r="19" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="CR18" s="17"/>
+      <c r="CS18" s="18"/>
+      <c r="CT18" s="18"/>
+      <c r="CU18" s="18"/>
+    </row>
+    <row r="19" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A19" s="19"/>
       <c r="B19" s="1"/>
       <c r="C19" s="8"/>
@@ -7847,20 +7962,24 @@
       <c r="CC19" s="18"/>
       <c r="CD19" s="18"/>
       <c r="CE19" s="18"/>
-      <c r="CF19" s="17"/>
+      <c r="CF19" s="18"/>
       <c r="CG19" s="18"/>
       <c r="CH19" s="18"/>
       <c r="CI19" s="18"/>
-      <c r="CJ19" s="18"/>
+      <c r="CJ19" s="17"/>
       <c r="CK19" s="18"/>
       <c r="CL19" s="18"/>
       <c r="CM19" s="18"/>
-      <c r="CN19" s="17"/>
+      <c r="CN19" s="18"/>
       <c r="CO19" s="18"/>
       <c r="CP19" s="18"/>
       <c r="CQ19" s="18"/>
-    </row>
-    <row r="20" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="CR19" s="17"/>
+      <c r="CS19" s="18"/>
+      <c r="CT19" s="18"/>
+      <c r="CU19" s="18"/>
+    </row>
+    <row r="20" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A20" s="19"/>
       <c r="B20" s="1"/>
       <c r="C20" s="8"/>
@@ -7944,20 +8063,24 @@
       <c r="CC20" s="18"/>
       <c r="CD20" s="18"/>
       <c r="CE20" s="18"/>
-      <c r="CF20" s="17"/>
+      <c r="CF20" s="18"/>
       <c r="CG20" s="18"/>
       <c r="CH20" s="18"/>
       <c r="CI20" s="18"/>
-      <c r="CJ20" s="18"/>
+      <c r="CJ20" s="17"/>
       <c r="CK20" s="18"/>
       <c r="CL20" s="18"/>
       <c r="CM20" s="18"/>
-      <c r="CN20" s="17"/>
+      <c r="CN20" s="18"/>
       <c r="CO20" s="18"/>
       <c r="CP20" s="18"/>
       <c r="CQ20" s="18"/>
-    </row>
-    <row r="21" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="CR20" s="17"/>
+      <c r="CS20" s="18"/>
+      <c r="CT20" s="18"/>
+      <c r="CU20" s="18"/>
+    </row>
+    <row r="21" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A21" s="19"/>
       <c r="B21" s="1"/>
       <c r="C21" s="8"/>
@@ -8041,20 +8164,24 @@
       <c r="CC21" s="18"/>
       <c r="CD21" s="18"/>
       <c r="CE21" s="18"/>
-      <c r="CF21" s="17"/>
+      <c r="CF21" s="18"/>
       <c r="CG21" s="18"/>
       <c r="CH21" s="18"/>
       <c r="CI21" s="18"/>
-      <c r="CJ21" s="18"/>
+      <c r="CJ21" s="17"/>
       <c r="CK21" s="18"/>
       <c r="CL21" s="18"/>
       <c r="CM21" s="18"/>
-      <c r="CN21" s="17"/>
+      <c r="CN21" s="18"/>
       <c r="CO21" s="18"/>
       <c r="CP21" s="18"/>
       <c r="CQ21" s="18"/>
-    </row>
-    <row r="22" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="CR21" s="17"/>
+      <c r="CS21" s="18"/>
+      <c r="CT21" s="18"/>
+      <c r="CU21" s="18"/>
+    </row>
+    <row r="22" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A22" s="19"/>
       <c r="B22" s="1"/>
       <c r="C22" s="8"/>
@@ -8138,20 +8265,24 @@
       <c r="CC22" s="18"/>
       <c r="CD22" s="18"/>
       <c r="CE22" s="18"/>
-      <c r="CF22" s="17"/>
+      <c r="CF22" s="18"/>
       <c r="CG22" s="18"/>
       <c r="CH22" s="18"/>
       <c r="CI22" s="18"/>
-      <c r="CJ22" s="18"/>
+      <c r="CJ22" s="17"/>
       <c r="CK22" s="18"/>
       <c r="CL22" s="18"/>
       <c r="CM22" s="18"/>
-      <c r="CN22" s="17"/>
+      <c r="CN22" s="18"/>
       <c r="CO22" s="18"/>
       <c r="CP22" s="18"/>
       <c r="CQ22" s="18"/>
-    </row>
-    <row r="23" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="CR22" s="17"/>
+      <c r="CS22" s="18"/>
+      <c r="CT22" s="18"/>
+      <c r="CU22" s="18"/>
+    </row>
+    <row r="23" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A23" s="19"/>
       <c r="B23" s="1"/>
       <c r="C23" s="8"/>
@@ -8235,20 +8366,24 @@
       <c r="CC23" s="18"/>
       <c r="CD23" s="18"/>
       <c r="CE23" s="18"/>
-      <c r="CF23" s="17"/>
+      <c r="CF23" s="18"/>
       <c r="CG23" s="18"/>
       <c r="CH23" s="18"/>
       <c r="CI23" s="18"/>
-      <c r="CJ23" s="18"/>
+      <c r="CJ23" s="17"/>
       <c r="CK23" s="18"/>
       <c r="CL23" s="18"/>
       <c r="CM23" s="18"/>
-      <c r="CN23" s="17"/>
+      <c r="CN23" s="18"/>
       <c r="CO23" s="18"/>
       <c r="CP23" s="18"/>
       <c r="CQ23" s="18"/>
-    </row>
-    <row r="24" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="CR23" s="17"/>
+      <c r="CS23" s="18"/>
+      <c r="CT23" s="18"/>
+      <c r="CU23" s="18"/>
+    </row>
+    <row r="24" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A24" s="19"/>
       <c r="B24" s="1"/>
       <c r="C24" s="8"/>
@@ -8332,20 +8467,24 @@
       <c r="CC24" s="18"/>
       <c r="CD24" s="18"/>
       <c r="CE24" s="18"/>
-      <c r="CF24" s="17"/>
+      <c r="CF24" s="18"/>
       <c r="CG24" s="18"/>
       <c r="CH24" s="18"/>
       <c r="CI24" s="18"/>
-      <c r="CJ24" s="18"/>
+      <c r="CJ24" s="17"/>
       <c r="CK24" s="18"/>
       <c r="CL24" s="18"/>
       <c r="CM24" s="18"/>
-      <c r="CN24" s="17"/>
+      <c r="CN24" s="18"/>
       <c r="CO24" s="18"/>
       <c r="CP24" s="18"/>
       <c r="CQ24" s="18"/>
-    </row>
-    <row r="25" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="CR24" s="17"/>
+      <c r="CS24" s="18"/>
+      <c r="CT24" s="18"/>
+      <c r="CU24" s="18"/>
+    </row>
+    <row r="25" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A25" s="19"/>
       <c r="B25" s="1"/>
       <c r="C25" s="8"/>
@@ -8429,20 +8568,24 @@
       <c r="CC25" s="18"/>
       <c r="CD25" s="18"/>
       <c r="CE25" s="18"/>
-      <c r="CF25" s="17"/>
+      <c r="CF25" s="18"/>
       <c r="CG25" s="18"/>
       <c r="CH25" s="18"/>
       <c r="CI25" s="18"/>
-      <c r="CJ25" s="18"/>
+      <c r="CJ25" s="17"/>
       <c r="CK25" s="18"/>
       <c r="CL25" s="18"/>
       <c r="CM25" s="18"/>
-      <c r="CN25" s="17"/>
+      <c r="CN25" s="18"/>
       <c r="CO25" s="18"/>
       <c r="CP25" s="18"/>
       <c r="CQ25" s="18"/>
-    </row>
-    <row r="26" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="CR25" s="17"/>
+      <c r="CS25" s="18"/>
+      <c r="CT25" s="18"/>
+      <c r="CU25" s="18"/>
+    </row>
+    <row r="26" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A26" s="19"/>
       <c r="B26" s="1"/>
       <c r="C26" s="8"/>
@@ -8526,20 +8669,24 @@
       <c r="CC26" s="18"/>
       <c r="CD26" s="18"/>
       <c r="CE26" s="18"/>
-      <c r="CF26" s="17"/>
+      <c r="CF26" s="18"/>
       <c r="CG26" s="18"/>
       <c r="CH26" s="18"/>
       <c r="CI26" s="18"/>
-      <c r="CJ26" s="18"/>
+      <c r="CJ26" s="17"/>
       <c r="CK26" s="18"/>
       <c r="CL26" s="18"/>
       <c r="CM26" s="18"/>
-      <c r="CN26" s="17"/>
+      <c r="CN26" s="18"/>
       <c r="CO26" s="18"/>
       <c r="CP26" s="18"/>
       <c r="CQ26" s="18"/>
-    </row>
-    <row r="27" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="CR26" s="17"/>
+      <c r="CS26" s="18"/>
+      <c r="CT26" s="18"/>
+      <c r="CU26" s="18"/>
+    </row>
+    <row r="27" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A27" s="19"/>
       <c r="B27" s="1"/>
       <c r="C27" s="8"/>
@@ -8623,20 +8770,24 @@
       <c r="CC27" s="18"/>
       <c r="CD27" s="18"/>
       <c r="CE27" s="18"/>
-      <c r="CF27" s="17"/>
+      <c r="CF27" s="18"/>
       <c r="CG27" s="18"/>
       <c r="CH27" s="18"/>
       <c r="CI27" s="18"/>
-      <c r="CJ27" s="18"/>
+      <c r="CJ27" s="17"/>
       <c r="CK27" s="18"/>
       <c r="CL27" s="18"/>
       <c r="CM27" s="18"/>
-      <c r="CN27" s="17"/>
+      <c r="CN27" s="18"/>
       <c r="CO27" s="18"/>
       <c r="CP27" s="18"/>
       <c r="CQ27" s="18"/>
-    </row>
-    <row r="28" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="CR27" s="17"/>
+      <c r="CS27" s="18"/>
+      <c r="CT27" s="18"/>
+      <c r="CU27" s="18"/>
+    </row>
+    <row r="28" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A28" s="19"/>
       <c r="B28" s="1"/>
       <c r="C28" s="8"/>
@@ -8720,20 +8871,24 @@
       <c r="CC28" s="18"/>
       <c r="CD28" s="18"/>
       <c r="CE28" s="18"/>
-      <c r="CF28" s="17"/>
+      <c r="CF28" s="18"/>
       <c r="CG28" s="18"/>
       <c r="CH28" s="18"/>
       <c r="CI28" s="18"/>
-      <c r="CJ28" s="18"/>
+      <c r="CJ28" s="17"/>
       <c r="CK28" s="18"/>
       <c r="CL28" s="18"/>
       <c r="CM28" s="18"/>
-      <c r="CN28" s="17"/>
+      <c r="CN28" s="18"/>
       <c r="CO28" s="18"/>
       <c r="CP28" s="18"/>
       <c r="CQ28" s="18"/>
-    </row>
-    <row r="29" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="CR28" s="17"/>
+      <c r="CS28" s="18"/>
+      <c r="CT28" s="18"/>
+      <c r="CU28" s="18"/>
+    </row>
+    <row r="29" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A29" s="19"/>
       <c r="B29" s="1"/>
       <c r="C29" s="8"/>
@@ -8817,100 +8972,104 @@
       <c r="CC29" s="18"/>
       <c r="CD29" s="18"/>
       <c r="CE29" s="18"/>
-      <c r="CF29" s="17"/>
+      <c r="CF29" s="18"/>
       <c r="CG29" s="18"/>
       <c r="CH29" s="18"/>
       <c r="CI29" s="18"/>
-      <c r="CJ29" s="18"/>
+      <c r="CJ29" s="17"/>
       <c r="CK29" s="18"/>
       <c r="CL29" s="18"/>
       <c r="CM29" s="18"/>
-      <c r="CN29" s="17"/>
+      <c r="CN29" s="18"/>
       <c r="CO29" s="18"/>
       <c r="CP29" s="18"/>
       <c r="CQ29" s="18"/>
-    </row>
-    <row r="30" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="CR29" s="17"/>
+      <c r="CS29" s="18"/>
+      <c r="CT29" s="18"/>
+      <c r="CU29" s="18"/>
+    </row>
+    <row r="30" spans="1:99" x14ac:dyDescent="0.2">
       <c r="B30" s="31"/>
       <c r="C30" s="32"/>
     </row>
-    <row r="31" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:99" x14ac:dyDescent="0.2">
       <c r="B31" s="31"/>
       <c r="C31" s="32"/>
     </row>
-    <row r="32" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:99" x14ac:dyDescent="0.2">
       <c r="B32" s="31"/>
       <c r="C32" s="32"/>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B33" s="31"/>
       <c r="C33" s="32"/>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B34" s="31"/>
       <c r="C34" s="32"/>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B35" s="31"/>
       <c r="C35" s="32"/>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B36" s="31"/>
       <c r="C36" s="32"/>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B37" s="31"/>
       <c r="C37" s="32"/>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B38" s="31"/>
       <c r="C38" s="32"/>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B39" s="31"/>
       <c r="C39" s="32"/>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B40" s="31"/>
       <c r="C40" s="32"/>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B41" s="31"/>
       <c r="C41" s="32"/>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B42" s="31"/>
       <c r="C42" s="32"/>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B43" s="31"/>
       <c r="C43" s="32"/>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B44" s="31"/>
       <c r="C44" s="32"/>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B45" s="31"/>
       <c r="C45" s="32"/>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B46" s="31"/>
       <c r="C46" s="32"/>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B47" s="31"/>
       <c r="C47" s="32"/>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B48" s="31"/>
       <c r="C48" s="32"/>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B49" s="31"/>
       <c r="C49" s="32"/>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B50" s="31"/>
       <c r="C50" s="32"/>
     </row>
@@ -8925,19 +9084,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8193" r:id="rId4" name="SetDateTimeRef">
+        <control shapeId="8195" r:id="rId4" name="SetDateTimeMain">
           <controlPr print="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>6350</xdr:rowOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>12700</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -8945,7 +9104,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8193" r:id="rId4" name="SetDateTimeRef"/>
+        <control shapeId="8195" r:id="rId4" name="SetDateTimeMain"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8961,7 +9120,7 @@
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>12700</xdr:colOff>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
@@ -8975,19 +9134,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8195" r:id="rId8" name="SetDateTimeMain">
+        <control shapeId="8193" r:id="rId8" name="SetDateTimeRef">
           <controlPr print="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>6350</xdr:rowOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>12700</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -8995,7 +9154,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8195" r:id="rId8" name="SetDateTimeMain"/>
+        <control shapeId="8193" r:id="rId8" name="SetDateTimeRef"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
Fill aero values into setup sheet.
</commit_message>
<xml_diff>
--- a/Functions/SetupSheets.xlsx
+++ b/Functions/SetupSheets.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1815" yWindow="195" windowWidth="15195" windowHeight="7140" activeTab="1"/>
+    <workbookView xWindow="1815" yWindow="540" windowWidth="9705" windowHeight="3240" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Combustion" sheetId="10" r:id="rId1"/>
@@ -5220,10 +5220,10 @@
   <dimension ref="A1:CU50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="BT6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="CA6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="CH7" sqref="CH7"/>
+      <selection pane="bottomRight" activeCell="CC7" sqref="CC7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6614,16 +6614,16 @@
         <v>0</v>
       </c>
       <c r="CC6" s="12">
-        <v>0.6</v>
+        <v>0.45</v>
       </c>
       <c r="CD6" s="12">
-        <v>0.6</v>
+        <v>0.89</v>
       </c>
       <c r="CE6" s="12">
         <v>2015</v>
       </c>
       <c r="CF6" s="12">
-        <v>0</v>
+        <v>2.3289999999999999E-3</v>
       </c>
       <c r="CG6" s="12">
         <v>34.25</v>

</xml_diff>

<commit_message>
Lift should be negative in setup sheet.
</commit_message>
<xml_diff>
--- a/Functions/SetupSheets.xlsx
+++ b/Functions/SetupSheets.xlsx
@@ -5223,7 +5223,7 @@
       <pane xSplit="3" ySplit="5" topLeftCell="CA6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="CC7" sqref="CC7"/>
+      <selection pane="bottomRight" activeCell="CD7" sqref="CD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6617,7 +6617,7 @@
         <v>0.45</v>
       </c>
       <c r="CD6" s="12">
-        <v>0.89</v>
+        <v>-0.89</v>
       </c>
       <c r="CE6" s="12">
         <v>2015</v>

</xml_diff>

<commit_message>
Update Aero values with correct values for 2016.
</commit_message>
<xml_diff>
--- a/Functions/SetupSheets.xlsx
+++ b/Functions/SetupSheets.xlsx
@@ -5220,10 +5220,10 @@
   <dimension ref="A1:CU50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="CA6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="BW6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="CD7" sqref="CD7"/>
+      <selection pane="bottomRight" activeCell="CC6" sqref="CC6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6620,7 +6620,7 @@
         <v>-0.89</v>
       </c>
       <c r="CE6" s="12">
-        <v>2015</v>
+        <v>1872</v>
       </c>
       <c r="CF6" s="12">
         <v>2.3289999999999999E-3</v>

</xml_diff>

<commit_message>
Fix calculation of axle output curve for single gear cars and add final drive ratio back in.
</commit_message>
<xml_diff>
--- a/Functions/SetupSheets.xlsx
+++ b/Functions/SetupSheets.xlsx
@@ -5220,10 +5220,10 @@
   <dimension ref="A1:CU50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="BS6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="BB6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="CC7" sqref="CC7"/>
+      <selection pane="bottomRight" activeCell="BH6" sqref="BH6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6546,10 +6546,10 @@
       </c>
       <c r="BD6" s="17"/>
       <c r="BE6" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF6" s="12">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="BG6" s="12">
         <v>0</v>

</xml_diff>

<commit_message>
Add actual gear ratio data for combustion car.
</commit_message>
<xml_diff>
--- a/Functions/SetupSheets.xlsx
+++ b/Functions/SetupSheets.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1815" yWindow="540" windowWidth="9705" windowHeight="3240" activeTab="1"/>
+    <workbookView xWindow="1815" yWindow="540" windowWidth="9705" windowHeight="3240"/>
   </bookViews>
   <sheets>
     <sheet name="Combustion" sheetId="10" r:id="rId1"/>
@@ -1414,11 +1414,11 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:CQ50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="5" topLeftCell="BB6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="CE1" sqref="CE1"/>
+      <selection pane="bottomRight" activeCell="BK7" sqref="BK7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2706,25 +2706,25 @@
         <v>1</v>
       </c>
       <c r="BF6" s="12">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="BG6" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BH6" s="12">
-        <v>0</v>
+        <v>1.6319999999999999</v>
       </c>
       <c r="BI6" s="12">
-        <v>0</v>
+        <v>1.333</v>
       </c>
       <c r="BJ6" s="12">
-        <v>0</v>
+        <v>1.095</v>
       </c>
       <c r="BK6" s="12">
-        <v>1</v>
+        <v>2.6520000000000001</v>
       </c>
       <c r="BL6" s="12">
-        <v>1</v>
+        <v>2.714</v>
       </c>
       <c r="BM6" s="12">
         <v>0.9</v>
@@ -5219,7 +5219,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:CU50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="5" topLeftCell="BB6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>

</xml_diff>

<commit_message>
Fully updated Electric setup numbers.
</commit_message>
<xml_diff>
--- a/Functions/SetupSheets.xlsx
+++ b/Functions/SetupSheets.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Code\LapSimCombined\Functions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Code\LapSimCombined\Functions\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1815" yWindow="540" windowWidth="9705" windowHeight="3240"/>
+    <workbookView xWindow="1815" yWindow="540" windowWidth="9705" windowHeight="3240" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Combustion" sheetId="10" r:id="rId1"/>
@@ -1414,11 +1414,11 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:CQ50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="BB6" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="BK7" sqref="BK7"/>
+      <selection pane="bottomRight" activeCell="Y6" sqref="R6:Y6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2592,13 +2592,13 @@
         <v>0</v>
       </c>
       <c r="R6" s="18">
-        <v>33</v>
+        <v>34.200000000000003</v>
       </c>
       <c r="S6" s="18">
         <v>0</v>
       </c>
       <c r="T6" s="41">
-        <v>9.5</v>
+        <v>10.25</v>
       </c>
       <c r="U6" s="18">
         <v>0</v>
@@ -2613,7 +2613,7 @@
         <v>9.5</v>
       </c>
       <c r="Y6" s="12">
-        <v>564</v>
+        <v>670</v>
       </c>
       <c r="Z6" s="17"/>
       <c r="AA6" s="18">
@@ -5137,19 +5137,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="9217" r:id="rId4" name="SetDateTimeRef">
+        <control shapeId="9219" r:id="rId4" name="SetDateTimeMain">
           <controlPr print="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>2</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -5157,7 +5157,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="9217" r:id="rId4" name="SetDateTimeRef"/>
+        <control shapeId="9219" r:id="rId4" name="SetDateTimeMain"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -5187,19 +5187,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="9219" r:id="rId8" name="SetDateTimeMain">
+        <control shapeId="9217" r:id="rId8" name="SetDateTimeRef">
           <controlPr print="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -5207,7 +5207,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="9219" r:id="rId8" name="SetDateTimeMain"/>
+        <control shapeId="9217" r:id="rId8" name="SetDateTimeRef"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -5219,11 +5219,11 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:CU50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="BB6" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="BH6" sqref="BH6"/>
+      <selection pane="bottomRight" activeCell="CK7" sqref="CK7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6435,13 +6435,13 @@
         <v>0</v>
       </c>
       <c r="R6" s="18">
-        <v>33</v>
+        <v>34.200000000000003</v>
       </c>
       <c r="S6" s="18">
         <v>0</v>
       </c>
       <c r="T6" s="41">
-        <v>9.5</v>
+        <v>10.25</v>
       </c>
       <c r="U6" s="18">
         <v>0</v>
@@ -6456,20 +6456,20 @@
         <v>9.5</v>
       </c>
       <c r="Y6" s="12">
-        <v>564</v>
+        <v>670</v>
       </c>
       <c r="Z6" s="17"/>
       <c r="AA6" s="18">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="AB6" s="18">
         <v>250</v>
       </c>
       <c r="AC6" s="18">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="AD6" s="18">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="AE6" s="18">
         <v>0</v>
@@ -6484,16 +6484,16 @@
         <v>0</v>
       </c>
       <c r="AI6" s="18">
-        <v>10.5</v>
+        <v>10.25</v>
       </c>
       <c r="AJ6" s="18">
-        <v>10.5</v>
+        <v>10.25</v>
       </c>
       <c r="AK6" s="18">
-        <v>-1.542</v>
+        <v>-0.25</v>
       </c>
       <c r="AL6" s="18">
-        <v>-1.542</v>
+        <v>1.7</v>
       </c>
       <c r="AM6" s="18">
         <v>0</v>
@@ -6614,10 +6614,10 @@
         <v>0</v>
       </c>
       <c r="CC6" s="12">
-        <v>0.6</v>
+        <v>0.45</v>
       </c>
       <c r="CD6" s="12">
-        <v>-0.01</v>
+        <v>-0.89</v>
       </c>
       <c r="CE6" s="12">
         <v>2015</v>
@@ -6636,7 +6636,7 @@
       </c>
       <c r="CJ6" s="17"/>
       <c r="CK6" s="18">
-        <v>6.3</v>
+        <v>4.7</v>
       </c>
       <c r="CL6" s="18">
         <v>0</v>
@@ -9084,19 +9084,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8195" r:id="rId4" name="SetDateTimeMain">
+        <control shapeId="8193" r:id="rId4" name="SetDateTimeRef">
           <controlPr print="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -9104,7 +9104,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8195" r:id="rId4" name="SetDateTimeMain"/>
+        <control shapeId="8193" r:id="rId4" name="SetDateTimeRef"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9134,19 +9134,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8193" r:id="rId8" name="SetDateTimeRef">
+        <control shapeId="8195" r:id="rId8" name="SetDateTimeMain">
           <controlPr print="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>2</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -9154,7 +9154,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8193" r:id="rId8" name="SetDateTimeRef"/>
+        <control shapeId="8195" r:id="rId8" name="SetDateTimeMain"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
Committing to have Thomas Look at it
</commit_message>
<xml_diff>
--- a/Functions/SetupSheets.xlsx
+++ b/Functions/SetupSheets.xlsx
@@ -1409,10 +1409,10 @@
   <dimension ref="A1:CU50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="BA6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="BV6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="BO6" sqref="BO6"/>
+      <selection pane="bottomRight" activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2628,7 +2628,7 @@
         <v>0</v>
       </c>
       <c r="T6" s="41">
-        <v>17.04</v>
+        <v>12</v>
       </c>
       <c r="U6" s="18">
         <v>175</v>
@@ -2640,7 +2640,7 @@
         <v>0</v>
       </c>
       <c r="X6" s="18">
-        <v>17.04</v>
+        <v>12</v>
       </c>
       <c r="Y6" s="12">
         <v>404</v>
@@ -2726,7 +2726,7 @@
         <v>120.628</v>
       </c>
       <c r="BB6" s="18">
-        <v>67.95</v>
+        <v>70.396699999999996</v>
       </c>
       <c r="BC6" s="40" t="s">
         <v>80</v>
@@ -2823,7 +2823,7 @@
       </c>
       <c r="CJ6" s="17"/>
       <c r="CK6" s="18">
-        <v>4.7</v>
+        <v>0.7</v>
       </c>
       <c r="CL6" s="18">
         <v>0</v>
@@ -5354,10 +5354,10 @@
   <dimension ref="A1:CU50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="BV6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A16" sqref="A16"/>
+      <selection pane="bottomRight" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -6526,17 +6526,15 @@
       <c r="C6" s="8">
         <v>0.375</v>
       </c>
-      <c r="D6" s="17">
-        <v>1</v>
-      </c>
+      <c r="D6" s="17"/>
       <c r="E6" s="18">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="F6" s="18">
         <v>48</v>
       </c>
       <c r="G6" s="18">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H6" s="18">
         <v>0</v>

</xml_diff>

<commit_message>
Cal Poly Engine data, FSAEMichigan, parafor issue
Engine data for Cal Poly seems to be throwing a cellfun issue, other
data works fine. FSAEMichigian2015 track added from Reiley it worked at
first, but now it hasnt been. Points were added. Trying to sweep with
excelSweep, but throwing parafor issue for valid variable indices
</commit_message>
<xml_diff>
--- a/Functions/SetupSheets.xlsx
+++ b/Functions/SetupSheets.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="116">
   <si>
     <t>Date</t>
   </si>
@@ -365,6 +365,9 @@
   </si>
   <si>
     <t>CoP Z</t>
+  </si>
+  <si>
+    <t>Wf</t>
   </si>
 </sst>
 </file>
@@ -511,7 +514,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -666,6 +669,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1409,10 +1416,10 @@
   <dimension ref="A1:CU50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="BV6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="T10" sqref="T10"/>
+      <selection pane="bottomRight" activeCell="D6" sqref="D6:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2219,8 +2226,8 @@
       <c r="CU4" s="15"/>
     </row>
     <row r="5" spans="1:99" s="22" customFormat="1" ht="13" x14ac:dyDescent="0.25">
-      <c r="A5" s="37" t="s">
-        <v>36</v>
+      <c r="A5" s="45" t="s">
+        <v>115</v>
       </c>
       <c r="B5" s="29"/>
       <c r="C5" s="30"/>
@@ -2573,15 +2580,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:99" ht="13" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
+    <row r="6" spans="1:99" x14ac:dyDescent="0.25">
+      <c r="A6" s="19">
+        <v>0.41</v>
+      </c>
       <c r="B6" s="1">
         <v>35065</v>
       </c>
       <c r="C6" s="8">
         <v>0.375</v>
       </c>
-      <c r="D6" s="17"/>
+      <c r="D6" s="17">
+        <v>0</v>
+      </c>
       <c r="E6" s="18">
         <v>63</v>
       </c>
@@ -2622,7 +2633,8 @@
         <v>0</v>
       </c>
       <c r="R6" s="18">
-        <v>33.9</v>
+        <f>E6*(1-A6)</f>
+        <v>37.17</v>
       </c>
       <c r="S6" s="18">
         <v>0</v>
@@ -2728,8 +2740,8 @@
       <c r="BB6" s="18">
         <v>70.396699999999996</v>
       </c>
-      <c r="BC6" s="40" t="s">
-        <v>80</v>
+      <c r="BC6" s="18">
+        <v>0</v>
       </c>
       <c r="BD6" s="17"/>
       <c r="BE6" s="12">
@@ -2854,913 +2866,2536 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:99" ht="13" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
+    <row r="7" spans="1:99" x14ac:dyDescent="0.25">
+      <c r="A7" s="23">
+        <v>0.42</v>
+      </c>
       <c r="B7" s="1"/>
       <c r="C7" s="8"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
-      <c r="R7" s="18"/>
-      <c r="S7" s="18"/>
-      <c r="T7" s="41"/>
-      <c r="U7" s="18"/>
-      <c r="V7" s="18"/>
-      <c r="W7" s="18"/>
-      <c r="X7" s="18"/>
-      <c r="Y7" s="12"/>
+      <c r="D7" s="17">
+        <v>0</v>
+      </c>
+      <c r="E7" s="18">
+        <v>63</v>
+      </c>
+      <c r="F7" s="18">
+        <v>47</v>
+      </c>
+      <c r="G7" s="18">
+        <v>46</v>
+      </c>
+      <c r="H7" s="18">
+        <v>0</v>
+      </c>
+      <c r="I7" s="18">
+        <v>0</v>
+      </c>
+      <c r="J7" s="18">
+        <v>0</v>
+      </c>
+      <c r="K7" s="18">
+        <v>0</v>
+      </c>
+      <c r="L7" s="18">
+        <v>0</v>
+      </c>
+      <c r="M7" s="18">
+        <v>0</v>
+      </c>
+      <c r="N7" s="18">
+        <v>0</v>
+      </c>
+      <c r="O7" s="18">
+        <v>0</v>
+      </c>
+      <c r="P7" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="18">
+        <v>0</v>
+      </c>
+      <c r="R7" s="18">
+        <f t="shared" ref="R7:R8" si="3">E7*(1-A7)</f>
+        <v>36.540000000000006</v>
+      </c>
+      <c r="S7" s="18">
+        <v>0</v>
+      </c>
+      <c r="T7" s="41">
+        <v>12</v>
+      </c>
+      <c r="U7" s="18">
+        <v>175</v>
+      </c>
+      <c r="V7" s="18">
+        <v>33.9</v>
+      </c>
+      <c r="W7" s="18">
+        <v>0</v>
+      </c>
+      <c r="X7" s="18">
+        <v>12</v>
+      </c>
+      <c r="Y7" s="12">
+        <v>404</v>
+      </c>
       <c r="Z7" s="17"/>
-      <c r="AA7" s="18"/>
-      <c r="AB7" s="18"/>
-      <c r="AC7" s="18"/>
-      <c r="AD7" s="18"/>
-      <c r="AE7" s="18"/>
-      <c r="AF7" s="18"/>
-      <c r="AG7" s="18"/>
-      <c r="AH7" s="18"/>
-      <c r="AI7" s="18"/>
-      <c r="AJ7" s="18"/>
-      <c r="AK7" s="18"/>
-      <c r="AL7" s="18"/>
-      <c r="AM7" s="18"/>
-      <c r="AN7" s="18"/>
-      <c r="AO7" s="18"/>
-      <c r="AP7" s="18"/>
-      <c r="AQ7" s="18"/>
-      <c r="AR7" s="18"/>
-      <c r="AS7" s="18"/>
-      <c r="AT7" s="18"/>
-      <c r="AU7" s="18"/>
-      <c r="AV7" s="18"/>
+      <c r="AA7" s="18">
+        <v>175</v>
+      </c>
+      <c r="AB7" s="18">
+        <v>200</v>
+      </c>
+      <c r="AC7" s="18">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="18">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="18">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="18">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="18">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="18">
+        <v>0</v>
+      </c>
+      <c r="AI7" s="18">
+        <v>10.25</v>
+      </c>
+      <c r="AJ7" s="18">
+        <v>10.25</v>
+      </c>
+      <c r="AK7" s="18">
+        <v>-0.25</v>
+      </c>
+      <c r="AL7" s="18">
+        <v>1.9</v>
+      </c>
+      <c r="AM7" s="18">
+        <v>0</v>
+      </c>
+      <c r="AN7" s="18">
+        <v>0</v>
+      </c>
+      <c r="AO7" s="18">
+        <v>0</v>
+      </c>
+      <c r="AP7" s="18">
+        <v>0</v>
+      </c>
+      <c r="AQ7" s="18">
+        <v>0</v>
+      </c>
+      <c r="AR7" s="18">
+        <v>0</v>
+      </c>
+      <c r="AS7" s="18">
+        <v>0</v>
+      </c>
+      <c r="AT7" s="18">
+        <v>0</v>
+      </c>
+      <c r="AU7" s="18">
+        <v>10</v>
+      </c>
+      <c r="AV7" s="18">
+        <v>30</v>
+      </c>
       <c r="AW7" s="17"/>
-      <c r="AX7" s="18"/>
-      <c r="AY7" s="18"/>
-      <c r="AZ7" s="18"/>
-      <c r="BA7" s="18"/>
-      <c r="BB7" s="18"/>
-      <c r="BC7" s="40"/>
+      <c r="AX7" s="18">
+        <v>900</v>
+      </c>
+      <c r="AY7" s="18">
+        <v>10.5</v>
+      </c>
+      <c r="AZ7" s="18">
+        <v>0.03</v>
+      </c>
+      <c r="BA7" s="18">
+        <v>120.628</v>
+      </c>
+      <c r="BB7" s="18">
+        <v>70.396699999999996</v>
+      </c>
+      <c r="BC7" s="18">
+        <v>0</v>
+      </c>
       <c r="BD7" s="17"/>
-      <c r="BE7" s="12"/>
-      <c r="BF7" s="12"/>
-      <c r="BG7" s="12"/>
-      <c r="BH7" s="12"/>
-      <c r="BI7" s="12"/>
-      <c r="BJ7" s="12"/>
-      <c r="BK7" s="12"/>
-      <c r="BL7" s="12"/>
-      <c r="BM7" s="12"/>
-      <c r="BN7" s="12"/>
-      <c r="BO7" s="12"/>
-      <c r="BP7" s="12"/>
-      <c r="BQ7" s="12"/>
+      <c r="BE7" s="12">
+        <v>1</v>
+      </c>
+      <c r="BF7" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="BG7" s="12">
+        <v>2</v>
+      </c>
+      <c r="BH7" s="12">
+        <v>1.62</v>
+      </c>
+      <c r="BI7" s="12">
+        <v>1.333</v>
+      </c>
+      <c r="BJ7" s="12">
+        <v>1.095</v>
+      </c>
+      <c r="BK7" s="12">
+        <v>2.6520000000000001</v>
+      </c>
+      <c r="BL7" s="12">
+        <v>2.714</v>
+      </c>
+      <c r="BM7" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="BN7" s="12">
+        <v>0</v>
+      </c>
+      <c r="BO7" s="12">
+        <v>0</v>
+      </c>
+      <c r="BP7" s="12">
+        <v>0</v>
+      </c>
+      <c r="BQ7" s="12">
+        <v>20</v>
+      </c>
       <c r="BR7" s="17"/>
-      <c r="BS7" s="12"/>
-      <c r="BT7" s="12"/>
-      <c r="BU7" s="12"/>
-      <c r="BV7" s="12"/>
-      <c r="BW7" s="12"/>
-      <c r="BX7" s="12"/>
+      <c r="BS7" s="12">
+        <v>6762.75</v>
+      </c>
+      <c r="BT7" s="12">
+        <v>3238.5</v>
+      </c>
+      <c r="BU7" s="12">
+        <v>0</v>
+      </c>
+      <c r="BV7" s="12">
+        <v>0</v>
+      </c>
+      <c r="BW7" s="12">
+        <v>0</v>
+      </c>
+      <c r="BX7" s="12">
+        <v>0.96699999999999997</v>
+      </c>
       <c r="BY7" s="17"/>
-      <c r="BZ7" s="12"/>
-      <c r="CA7" s="12"/>
-      <c r="CB7" s="12"/>
-      <c r="CC7" s="12"/>
-      <c r="CD7" s="12"/>
-      <c r="CE7" s="12"/>
-      <c r="CF7" s="12"/>
-      <c r="CG7" s="12"/>
-      <c r="CH7" s="12"/>
-      <c r="CI7" s="12"/>
+      <c r="BZ7" s="12">
+        <v>0</v>
+      </c>
+      <c r="CA7" s="12">
+        <v>0</v>
+      </c>
+      <c r="CB7" s="12">
+        <v>0</v>
+      </c>
+      <c r="CC7" s="12">
+        <v>0.45</v>
+      </c>
+      <c r="CD7" s="12">
+        <v>-0.89</v>
+      </c>
+      <c r="CE7" s="12">
+        <v>2015</v>
+      </c>
+      <c r="CF7" s="12">
+        <v>2.3289999999999999E-3</v>
+      </c>
+      <c r="CG7" s="12">
+        <v>34.25</v>
+      </c>
+      <c r="CH7" s="12">
+        <v>0</v>
+      </c>
+      <c r="CI7" s="12">
+        <v>10</v>
+      </c>
       <c r="CJ7" s="17"/>
-      <c r="CK7" s="18"/>
-      <c r="CL7" s="18"/>
-      <c r="CM7" s="18"/>
-      <c r="CN7" s="18"/>
-      <c r="CO7" s="18"/>
-      <c r="CP7" s="18"/>
-      <c r="CQ7" s="18"/>
+      <c r="CK7" s="18">
+        <v>0.7</v>
+      </c>
+      <c r="CL7" s="18">
+        <v>0</v>
+      </c>
+      <c r="CM7" s="18">
+        <v>0</v>
+      </c>
+      <c r="CN7" s="18">
+        <v>0</v>
+      </c>
+      <c r="CO7" s="18">
+        <v>0</v>
+      </c>
+      <c r="CP7" s="18">
+        <v>0</v>
+      </c>
+      <c r="CQ7" s="18">
+        <v>0</v>
+      </c>
       <c r="CR7" s="17"/>
-      <c r="CS7" s="18"/>
-      <c r="CT7" s="18"/>
-      <c r="CU7" s="18"/>
+      <c r="CS7" s="18">
+        <v>280</v>
+      </c>
+      <c r="CT7" s="18">
+        <v>9900</v>
+      </c>
+      <c r="CU7" s="18">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
+      <c r="A8" s="19">
+        <v>0.43</v>
+      </c>
       <c r="B8" s="1"/>
       <c r="C8" s="8"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
-      <c r="P8" s="18"/>
-      <c r="Q8" s="18"/>
-      <c r="R8" s="18"/>
-      <c r="S8" s="18"/>
-      <c r="T8" s="18"/>
-      <c r="U8" s="18"/>
-      <c r="V8" s="18"/>
-      <c r="W8" s="18"/>
-      <c r="X8" s="18"/>
-      <c r="Y8" s="12"/>
+      <c r="D8" s="17">
+        <v>0</v>
+      </c>
+      <c r="E8" s="18">
+        <v>63</v>
+      </c>
+      <c r="F8" s="18">
+        <v>47</v>
+      </c>
+      <c r="G8" s="18">
+        <v>46</v>
+      </c>
+      <c r="H8" s="18">
+        <v>0</v>
+      </c>
+      <c r="I8" s="18">
+        <v>0</v>
+      </c>
+      <c r="J8" s="18">
+        <v>0</v>
+      </c>
+      <c r="K8" s="18">
+        <v>0</v>
+      </c>
+      <c r="L8" s="18">
+        <v>0</v>
+      </c>
+      <c r="M8" s="18">
+        <v>0</v>
+      </c>
+      <c r="N8" s="18">
+        <v>0</v>
+      </c>
+      <c r="O8" s="18">
+        <v>0</v>
+      </c>
+      <c r="P8" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="18">
+        <v>0</v>
+      </c>
+      <c r="R8" s="18">
+        <f t="shared" si="3"/>
+        <v>35.910000000000004</v>
+      </c>
+      <c r="S8" s="18">
+        <v>0</v>
+      </c>
+      <c r="T8" s="41">
+        <v>12</v>
+      </c>
+      <c r="U8" s="18">
+        <v>175</v>
+      </c>
+      <c r="V8" s="18">
+        <v>33.9</v>
+      </c>
+      <c r="W8" s="18">
+        <v>0</v>
+      </c>
+      <c r="X8" s="18">
+        <v>12</v>
+      </c>
+      <c r="Y8" s="12">
+        <v>404</v>
+      </c>
       <c r="Z8" s="17"/>
-      <c r="AA8" s="18"/>
-      <c r="AB8" s="18"/>
-      <c r="AC8" s="18"/>
-      <c r="AD8" s="18"/>
-      <c r="AE8" s="18"/>
-      <c r="AF8" s="18"/>
-      <c r="AG8" s="18"/>
-      <c r="AH8" s="18"/>
-      <c r="AJ8" s="18"/>
-      <c r="AK8" s="18"/>
-      <c r="AL8" s="18"/>
-      <c r="AM8" s="18"/>
-      <c r="AN8" s="18"/>
-      <c r="AO8" s="18"/>
-      <c r="AP8" s="18"/>
-      <c r="AQ8" s="18"/>
-      <c r="AR8" s="18"/>
-      <c r="AS8" s="18"/>
-      <c r="AT8" s="18"/>
-      <c r="AU8" s="18"/>
-      <c r="AV8" s="18"/>
+      <c r="AA8" s="18">
+        <v>175</v>
+      </c>
+      <c r="AB8" s="18">
+        <v>200</v>
+      </c>
+      <c r="AC8" s="18">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="18">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="18">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="18">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="18">
+        <v>0</v>
+      </c>
+      <c r="AH8" s="18">
+        <v>0</v>
+      </c>
+      <c r="AI8" s="18">
+        <v>10.25</v>
+      </c>
+      <c r="AJ8" s="18">
+        <v>10.25</v>
+      </c>
+      <c r="AK8" s="18">
+        <v>-0.25</v>
+      </c>
+      <c r="AL8" s="18">
+        <v>1.9</v>
+      </c>
+      <c r="AM8" s="18">
+        <v>0</v>
+      </c>
+      <c r="AN8" s="18">
+        <v>0</v>
+      </c>
+      <c r="AO8" s="18">
+        <v>0</v>
+      </c>
+      <c r="AP8" s="18">
+        <v>0</v>
+      </c>
+      <c r="AQ8" s="18">
+        <v>0</v>
+      </c>
+      <c r="AR8" s="18">
+        <v>0</v>
+      </c>
+      <c r="AS8" s="18">
+        <v>0</v>
+      </c>
+      <c r="AT8" s="18">
+        <v>0</v>
+      </c>
+      <c r="AU8" s="18">
+        <v>10</v>
+      </c>
+      <c r="AV8" s="18">
+        <v>30</v>
+      </c>
       <c r="AW8" s="17"/>
-      <c r="AX8" s="18"/>
-      <c r="AY8" s="18"/>
-      <c r="AZ8" s="18"/>
-      <c r="BA8" s="18"/>
-      <c r="BB8" s="18"/>
-      <c r="BC8" s="18"/>
+      <c r="AX8" s="18">
+        <v>900</v>
+      </c>
+      <c r="AY8" s="18">
+        <v>10.5</v>
+      </c>
+      <c r="AZ8" s="18">
+        <v>0.03</v>
+      </c>
+      <c r="BA8" s="18">
+        <v>120.628</v>
+      </c>
+      <c r="BB8" s="18">
+        <v>70.396699999999996</v>
+      </c>
+      <c r="BC8" s="18">
+        <v>0</v>
+      </c>
       <c r="BD8" s="17"/>
-      <c r="BE8" s="12"/>
-      <c r="BF8" s="12"/>
-      <c r="BG8" s="12"/>
-      <c r="BH8" s="12"/>
-      <c r="BI8" s="12"/>
-      <c r="BJ8" s="12"/>
-      <c r="BK8" s="12"/>
-      <c r="BL8" s="12"/>
-      <c r="BM8" s="12"/>
-      <c r="BN8" s="12"/>
-      <c r="BO8" s="12"/>
-      <c r="BP8" s="12"/>
-      <c r="BQ8" s="12"/>
+      <c r="BE8" s="12">
+        <v>1</v>
+      </c>
+      <c r="BF8" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="BG8" s="12">
+        <v>2</v>
+      </c>
+      <c r="BH8" s="12">
+        <v>1.62</v>
+      </c>
+      <c r="BI8" s="12">
+        <v>1.333</v>
+      </c>
+      <c r="BJ8" s="12">
+        <v>1.095</v>
+      </c>
+      <c r="BK8" s="12">
+        <v>2.6520000000000001</v>
+      </c>
+      <c r="BL8" s="12">
+        <v>2.714</v>
+      </c>
+      <c r="BM8" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="BN8" s="12">
+        <v>0</v>
+      </c>
+      <c r="BO8" s="12">
+        <v>0</v>
+      </c>
+      <c r="BP8" s="12">
+        <v>0</v>
+      </c>
+      <c r="BQ8" s="12">
+        <v>20</v>
+      </c>
       <c r="BR8" s="17"/>
-      <c r="BS8" s="12"/>
-      <c r="BT8" s="12"/>
-      <c r="BU8" s="12"/>
-      <c r="BV8" s="12"/>
-      <c r="BW8" s="12"/>
-      <c r="BX8" s="12"/>
+      <c r="BS8" s="12">
+        <v>6762.75</v>
+      </c>
+      <c r="BT8" s="12">
+        <v>3238.5</v>
+      </c>
+      <c r="BU8" s="12">
+        <v>0</v>
+      </c>
+      <c r="BV8" s="12">
+        <v>0</v>
+      </c>
+      <c r="BW8" s="12">
+        <v>0</v>
+      </c>
+      <c r="BX8" s="12">
+        <v>0.96699999999999997</v>
+      </c>
       <c r="BY8" s="17"/>
-      <c r="BZ8" s="12"/>
-      <c r="CA8" s="12"/>
-      <c r="CB8" s="12"/>
-      <c r="CC8" s="12"/>
-      <c r="CD8" s="12"/>
-      <c r="CE8" s="12"/>
-      <c r="CF8" s="12"/>
-      <c r="CG8" s="12"/>
-      <c r="CH8" s="12"/>
-      <c r="CI8" s="12"/>
+      <c r="BZ8" s="12">
+        <v>0</v>
+      </c>
+      <c r="CA8" s="12">
+        <v>0</v>
+      </c>
+      <c r="CB8" s="12">
+        <v>0</v>
+      </c>
+      <c r="CC8" s="12">
+        <v>0.45</v>
+      </c>
+      <c r="CD8" s="12">
+        <v>-0.89</v>
+      </c>
+      <c r="CE8" s="12">
+        <v>2015</v>
+      </c>
+      <c r="CF8" s="12">
+        <v>2.3289999999999999E-3</v>
+      </c>
+      <c r="CG8" s="12">
+        <v>34.25</v>
+      </c>
+      <c r="CH8" s="12">
+        <v>0</v>
+      </c>
+      <c r="CI8" s="12">
+        <v>10</v>
+      </c>
       <c r="CJ8" s="17"/>
-      <c r="CK8" s="18"/>
-      <c r="CL8" s="18"/>
-      <c r="CM8" s="18"/>
-      <c r="CN8" s="18"/>
-      <c r="CO8" s="18"/>
-      <c r="CP8" s="18"/>
-      <c r="CQ8" s="18"/>
+      <c r="CK8" s="18">
+        <v>0.7</v>
+      </c>
+      <c r="CL8" s="18">
+        <v>0</v>
+      </c>
+      <c r="CM8" s="18">
+        <v>0</v>
+      </c>
+      <c r="CN8" s="18">
+        <v>0</v>
+      </c>
+      <c r="CO8" s="18">
+        <v>0</v>
+      </c>
+      <c r="CP8" s="18">
+        <v>0</v>
+      </c>
+      <c r="CQ8" s="18">
+        <v>0</v>
+      </c>
       <c r="CR8" s="17"/>
-      <c r="CS8" s="18"/>
-      <c r="CT8" s="18"/>
-      <c r="CU8" s="18"/>
+      <c r="CS8" s="18">
+        <v>280</v>
+      </c>
+      <c r="CT8" s="18">
+        <v>9900</v>
+      </c>
+      <c r="CU8" s="18">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
+      <c r="A9" s="19">
+        <v>0.44</v>
+      </c>
       <c r="B9" s="1"/>
       <c r="C9" s="8"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18"/>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="18"/>
-      <c r="R9" s="18"/>
-      <c r="S9" s="18"/>
-      <c r="T9" s="18"/>
-      <c r="U9" s="18"/>
-      <c r="V9" s="18"/>
-      <c r="W9" s="18"/>
-      <c r="X9" s="18"/>
-      <c r="Y9" s="18"/>
+      <c r="D9" s="17">
+        <v>0</v>
+      </c>
+      <c r="E9" s="18">
+        <v>63</v>
+      </c>
+      <c r="F9" s="18">
+        <v>47</v>
+      </c>
+      <c r="G9" s="18">
+        <v>46</v>
+      </c>
+      <c r="H9" s="18">
+        <v>0</v>
+      </c>
+      <c r="I9" s="18">
+        <v>0</v>
+      </c>
+      <c r="J9" s="18">
+        <v>0</v>
+      </c>
+      <c r="K9" s="18">
+        <v>0</v>
+      </c>
+      <c r="L9" s="18">
+        <v>0</v>
+      </c>
+      <c r="M9" s="18">
+        <v>0</v>
+      </c>
+      <c r="N9" s="18">
+        <v>0</v>
+      </c>
+      <c r="O9" s="18">
+        <v>0</v>
+      </c>
+      <c r="P9" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="18">
+        <v>0</v>
+      </c>
+      <c r="R9" s="18">
+        <v>35.28</v>
+      </c>
+      <c r="S9" s="18">
+        <v>0</v>
+      </c>
+      <c r="T9" s="41">
+        <v>12</v>
+      </c>
+      <c r="U9" s="18">
+        <v>175</v>
+      </c>
+      <c r="V9" s="18">
+        <v>33.9</v>
+      </c>
+      <c r="W9" s="18">
+        <v>0</v>
+      </c>
+      <c r="X9" s="18">
+        <v>12</v>
+      </c>
+      <c r="Y9" s="12">
+        <v>404</v>
+      </c>
       <c r="Z9" s="17"/>
-      <c r="AA9" s="18"/>
-      <c r="AB9" s="18"/>
-      <c r="AC9" s="18"/>
-      <c r="AD9" s="18"/>
-      <c r="AE9" s="18"/>
-      <c r="AF9" s="18"/>
-      <c r="AG9" s="18"/>
-      <c r="AH9" s="18"/>
-      <c r="AI9" s="18"/>
-      <c r="AJ9" s="18"/>
-      <c r="AK9" s="18"/>
-      <c r="AL9" s="18"/>
-      <c r="AM9" s="18"/>
-      <c r="AN9" s="18"/>
-      <c r="AO9" s="18"/>
-      <c r="AP9" s="18"/>
-      <c r="AQ9" s="18"/>
-      <c r="AR9" s="18"/>
-      <c r="AS9" s="18"/>
-      <c r="AT9" s="18"/>
-      <c r="AU9" s="18"/>
-      <c r="AV9" s="18"/>
+      <c r="AA9" s="18">
+        <v>175</v>
+      </c>
+      <c r="AB9" s="18">
+        <v>200</v>
+      </c>
+      <c r="AC9" s="18">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="18">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="18">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="18">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="18">
+        <v>0</v>
+      </c>
+      <c r="AH9" s="18">
+        <v>0</v>
+      </c>
+      <c r="AI9" s="18">
+        <v>10.25</v>
+      </c>
+      <c r="AJ9" s="18">
+        <v>10.25</v>
+      </c>
+      <c r="AK9" s="18">
+        <v>-0.25</v>
+      </c>
+      <c r="AL9" s="18">
+        <v>1.9</v>
+      </c>
+      <c r="AM9" s="18">
+        <v>0</v>
+      </c>
+      <c r="AN9" s="18">
+        <v>0</v>
+      </c>
+      <c r="AO9" s="18">
+        <v>0</v>
+      </c>
+      <c r="AP9" s="18">
+        <v>0</v>
+      </c>
+      <c r="AQ9" s="18">
+        <v>0</v>
+      </c>
+      <c r="AR9" s="18">
+        <v>0</v>
+      </c>
+      <c r="AS9" s="18">
+        <v>0</v>
+      </c>
+      <c r="AT9" s="18">
+        <v>0</v>
+      </c>
+      <c r="AU9" s="18">
+        <v>10</v>
+      </c>
+      <c r="AV9" s="18">
+        <v>30</v>
+      </c>
       <c r="AW9" s="17"/>
-      <c r="AX9" s="18"/>
-      <c r="AY9" s="18"/>
-      <c r="AZ9" s="18"/>
-      <c r="BA9" s="18"/>
-      <c r="BB9" s="18"/>
-      <c r="BC9" s="18"/>
+      <c r="AX9" s="18">
+        <v>900</v>
+      </c>
+      <c r="AY9" s="18">
+        <v>10.5</v>
+      </c>
+      <c r="AZ9" s="18">
+        <v>0.03</v>
+      </c>
+      <c r="BA9" s="18">
+        <v>120.628</v>
+      </c>
+      <c r="BB9" s="18">
+        <v>70.396699999999996</v>
+      </c>
+      <c r="BC9" s="18">
+        <v>0</v>
+      </c>
       <c r="BD9" s="17"/>
-      <c r="BE9" s="18"/>
-      <c r="BF9" s="18"/>
-      <c r="BG9" s="18"/>
-      <c r="BH9" s="18"/>
-      <c r="BI9" s="18"/>
-      <c r="BJ9" s="18"/>
-      <c r="BK9" s="18"/>
-      <c r="BL9" s="18"/>
-      <c r="BM9" s="18"/>
-      <c r="BN9" s="18"/>
-      <c r="BO9" s="18"/>
-      <c r="BP9" s="18"/>
-      <c r="BQ9" s="18"/>
+      <c r="BE9" s="12">
+        <v>1</v>
+      </c>
+      <c r="BF9" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="BG9" s="12">
+        <v>2</v>
+      </c>
+      <c r="BH9" s="12">
+        <v>1.62</v>
+      </c>
+      <c r="BI9" s="12">
+        <v>1.333</v>
+      </c>
+      <c r="BJ9" s="12">
+        <v>1.095</v>
+      </c>
+      <c r="BK9" s="12">
+        <v>2.6520000000000001</v>
+      </c>
+      <c r="BL9" s="12">
+        <v>2.714</v>
+      </c>
+      <c r="BM9" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="BN9" s="12">
+        <v>0</v>
+      </c>
+      <c r="BO9" s="12">
+        <v>0</v>
+      </c>
+      <c r="BP9" s="12">
+        <v>0</v>
+      </c>
+      <c r="BQ9" s="12">
+        <v>20</v>
+      </c>
       <c r="BR9" s="17"/>
-      <c r="BS9" s="18"/>
-      <c r="BT9" s="18"/>
-      <c r="BU9" s="18"/>
-      <c r="BV9" s="18"/>
-      <c r="BW9" s="18"/>
-      <c r="BX9" s="18"/>
+      <c r="BS9" s="12">
+        <v>6762.75</v>
+      </c>
+      <c r="BT9" s="12">
+        <v>3238.5</v>
+      </c>
+      <c r="BU9" s="12">
+        <v>0</v>
+      </c>
+      <c r="BV9" s="12">
+        <v>0</v>
+      </c>
+      <c r="BW9" s="12">
+        <v>0</v>
+      </c>
+      <c r="BX9" s="12">
+        <v>0.96699999999999997</v>
+      </c>
       <c r="BY9" s="17"/>
-      <c r="BZ9" s="18"/>
-      <c r="CA9" s="18"/>
-      <c r="CB9" s="18"/>
-      <c r="CC9" s="18"/>
-      <c r="CD9" s="18"/>
-      <c r="CE9" s="18"/>
-      <c r="CF9" s="18"/>
-      <c r="CG9" s="18"/>
-      <c r="CH9" s="18"/>
-      <c r="CI9" s="18"/>
+      <c r="BZ9" s="12">
+        <v>0</v>
+      </c>
+      <c r="CA9" s="12">
+        <v>0</v>
+      </c>
+      <c r="CB9" s="12">
+        <v>0</v>
+      </c>
+      <c r="CC9" s="12">
+        <v>0.45</v>
+      </c>
+      <c r="CD9" s="12">
+        <v>-0.89</v>
+      </c>
+      <c r="CE9" s="12">
+        <v>2015</v>
+      </c>
+      <c r="CF9" s="12">
+        <v>2.3289999999999999E-3</v>
+      </c>
+      <c r="CG9" s="12">
+        <v>34.25</v>
+      </c>
+      <c r="CH9" s="12">
+        <v>0</v>
+      </c>
+      <c r="CI9" s="12">
+        <v>10</v>
+      </c>
       <c r="CJ9" s="17"/>
-      <c r="CK9" s="18"/>
-      <c r="CL9" s="18"/>
-      <c r="CM9" s="18"/>
-      <c r="CN9" s="18"/>
-      <c r="CO9" s="18"/>
-      <c r="CP9" s="18"/>
-      <c r="CQ9" s="18"/>
+      <c r="CK9" s="18">
+        <v>0.7</v>
+      </c>
+      <c r="CL9" s="18">
+        <v>0</v>
+      </c>
+      <c r="CM9" s="18">
+        <v>0</v>
+      </c>
+      <c r="CN9" s="18">
+        <v>0</v>
+      </c>
+      <c r="CO9" s="18">
+        <v>0</v>
+      </c>
+      <c r="CP9" s="18">
+        <v>0</v>
+      </c>
+      <c r="CQ9" s="18">
+        <v>0</v>
+      </c>
       <c r="CR9" s="17"/>
-      <c r="CS9" s="18"/>
-      <c r="CT9" s="18"/>
-      <c r="CU9" s="18"/>
+      <c r="CS9" s="18">
+        <v>280</v>
+      </c>
+      <c r="CT9" s="18">
+        <v>9900</v>
+      </c>
+      <c r="CU9" s="18">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
+      <c r="A10" s="23">
+        <v>0.45</v>
+      </c>
       <c r="B10" s="1"/>
       <c r="C10" s="8"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="18"/>
-      <c r="S10" s="18"/>
-      <c r="T10" s="18"/>
-      <c r="U10" s="18"/>
-      <c r="V10" s="18"/>
-      <c r="W10" s="18"/>
-      <c r="X10" s="18"/>
-      <c r="Y10" s="18"/>
+      <c r="D10" s="17">
+        <v>0</v>
+      </c>
+      <c r="E10" s="18">
+        <v>63</v>
+      </c>
+      <c r="F10" s="18">
+        <v>47</v>
+      </c>
+      <c r="G10" s="18">
+        <v>46</v>
+      </c>
+      <c r="H10" s="18">
+        <v>0</v>
+      </c>
+      <c r="I10" s="18">
+        <v>0</v>
+      </c>
+      <c r="J10" s="18">
+        <v>0</v>
+      </c>
+      <c r="K10" s="18">
+        <v>0</v>
+      </c>
+      <c r="L10" s="18">
+        <v>0</v>
+      </c>
+      <c r="M10" s="18">
+        <v>0</v>
+      </c>
+      <c r="N10" s="18">
+        <v>0</v>
+      </c>
+      <c r="O10" s="18">
+        <v>0</v>
+      </c>
+      <c r="P10" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="18">
+        <v>0</v>
+      </c>
+      <c r="R10" s="18">
+        <v>34.650000000000006</v>
+      </c>
+      <c r="S10" s="18">
+        <v>0</v>
+      </c>
+      <c r="T10" s="41">
+        <v>12</v>
+      </c>
+      <c r="U10" s="18">
+        <v>175</v>
+      </c>
+      <c r="V10" s="18">
+        <v>33.9</v>
+      </c>
+      <c r="W10" s="18">
+        <v>0</v>
+      </c>
+      <c r="X10" s="18">
+        <v>12</v>
+      </c>
+      <c r="Y10" s="12">
+        <v>404</v>
+      </c>
       <c r="Z10" s="17"/>
-      <c r="AA10" s="18"/>
-      <c r="AB10" s="18"/>
-      <c r="AC10" s="18"/>
-      <c r="AD10" s="18"/>
-      <c r="AE10" s="18"/>
-      <c r="AF10" s="18"/>
-      <c r="AG10" s="18"/>
-      <c r="AH10" s="18"/>
-      <c r="AI10" s="18"/>
-      <c r="AJ10" s="18"/>
-      <c r="AK10" s="18"/>
-      <c r="AL10" s="18"/>
-      <c r="AM10" s="18"/>
-      <c r="AN10" s="18"/>
-      <c r="AO10" s="18"/>
-      <c r="AP10" s="18"/>
-      <c r="AQ10" s="18"/>
-      <c r="AR10" s="18"/>
-      <c r="AS10" s="18"/>
-      <c r="AT10" s="18"/>
-      <c r="AU10" s="18"/>
-      <c r="AV10" s="18"/>
+      <c r="AA10" s="18">
+        <v>175</v>
+      </c>
+      <c r="AB10" s="18">
+        <v>200</v>
+      </c>
+      <c r="AC10" s="18">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="18">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="18">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="18">
+        <v>0</v>
+      </c>
+      <c r="AG10" s="18">
+        <v>0</v>
+      </c>
+      <c r="AH10" s="18">
+        <v>0</v>
+      </c>
+      <c r="AI10" s="18">
+        <v>10.25</v>
+      </c>
+      <c r="AJ10" s="18">
+        <v>10.25</v>
+      </c>
+      <c r="AK10" s="18">
+        <v>-0.25</v>
+      </c>
+      <c r="AL10" s="18">
+        <v>1.9</v>
+      </c>
+      <c r="AM10" s="18">
+        <v>0</v>
+      </c>
+      <c r="AN10" s="18">
+        <v>0</v>
+      </c>
+      <c r="AO10" s="18">
+        <v>0</v>
+      </c>
+      <c r="AP10" s="18">
+        <v>0</v>
+      </c>
+      <c r="AQ10" s="18">
+        <v>0</v>
+      </c>
+      <c r="AR10" s="18">
+        <v>0</v>
+      </c>
+      <c r="AS10" s="18">
+        <v>0</v>
+      </c>
+      <c r="AT10" s="18">
+        <v>0</v>
+      </c>
+      <c r="AU10" s="18">
+        <v>10</v>
+      </c>
+      <c r="AV10" s="18">
+        <v>30</v>
+      </c>
       <c r="AW10" s="17"/>
-      <c r="AX10" s="18"/>
-      <c r="AY10" s="18"/>
-      <c r="AZ10" s="18"/>
-      <c r="BA10" s="18"/>
-      <c r="BB10" s="18"/>
-      <c r="BC10" s="18"/>
+      <c r="AX10" s="18">
+        <v>900</v>
+      </c>
+      <c r="AY10" s="18">
+        <v>10.5</v>
+      </c>
+      <c r="AZ10" s="18">
+        <v>0.03</v>
+      </c>
+      <c r="BA10" s="18">
+        <v>120.628</v>
+      </c>
+      <c r="BB10" s="18">
+        <v>70.396699999999996</v>
+      </c>
+      <c r="BC10" s="18">
+        <v>0</v>
+      </c>
       <c r="BD10" s="17"/>
-      <c r="BE10" s="18"/>
-      <c r="BF10" s="18"/>
-      <c r="BG10" s="18"/>
-      <c r="BH10" s="18"/>
-      <c r="BI10" s="18"/>
-      <c r="BJ10" s="18"/>
-      <c r="BK10" s="18"/>
-      <c r="BL10" s="18"/>
-      <c r="BM10" s="18"/>
-      <c r="BN10" s="18"/>
-      <c r="BO10" s="18"/>
-      <c r="BP10" s="18"/>
-      <c r="BQ10" s="18"/>
+      <c r="BE10" s="12">
+        <v>1</v>
+      </c>
+      <c r="BF10" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="BG10" s="12">
+        <v>2</v>
+      </c>
+      <c r="BH10" s="12">
+        <v>1.62</v>
+      </c>
+      <c r="BI10" s="12">
+        <v>1.333</v>
+      </c>
+      <c r="BJ10" s="12">
+        <v>1.095</v>
+      </c>
+      <c r="BK10" s="12">
+        <v>2.6520000000000001</v>
+      </c>
+      <c r="BL10" s="12">
+        <v>2.714</v>
+      </c>
+      <c r="BM10" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="BN10" s="12">
+        <v>0</v>
+      </c>
+      <c r="BO10" s="12">
+        <v>0</v>
+      </c>
+      <c r="BP10" s="12">
+        <v>0</v>
+      </c>
+      <c r="BQ10" s="12">
+        <v>20</v>
+      </c>
       <c r="BR10" s="17"/>
-      <c r="BS10" s="18"/>
-      <c r="BT10" s="18"/>
-      <c r="BU10" s="18"/>
-      <c r="BV10" s="18"/>
-      <c r="BW10" s="18"/>
-      <c r="BX10" s="18"/>
+      <c r="BS10" s="12">
+        <v>6762.75</v>
+      </c>
+      <c r="BT10" s="12">
+        <v>3238.5</v>
+      </c>
+      <c r="BU10" s="12">
+        <v>0</v>
+      </c>
+      <c r="BV10" s="12">
+        <v>0</v>
+      </c>
+      <c r="BW10" s="12">
+        <v>0</v>
+      </c>
+      <c r="BX10" s="12">
+        <v>0.96699999999999997</v>
+      </c>
       <c r="BY10" s="17"/>
-      <c r="BZ10" s="18"/>
-      <c r="CA10" s="18"/>
-      <c r="CB10" s="18"/>
-      <c r="CC10" s="18"/>
-      <c r="CD10" s="18"/>
-      <c r="CE10" s="18"/>
-      <c r="CF10" s="18"/>
-      <c r="CG10" s="18"/>
-      <c r="CH10" s="18"/>
-      <c r="CI10" s="18"/>
+      <c r="BZ10" s="12">
+        <v>0</v>
+      </c>
+      <c r="CA10" s="12">
+        <v>0</v>
+      </c>
+      <c r="CB10" s="12">
+        <v>0</v>
+      </c>
+      <c r="CC10" s="12">
+        <v>0.45</v>
+      </c>
+      <c r="CD10" s="12">
+        <v>-0.89</v>
+      </c>
+      <c r="CE10" s="12">
+        <v>2015</v>
+      </c>
+      <c r="CF10" s="12">
+        <v>2.3289999999999999E-3</v>
+      </c>
+      <c r="CG10" s="12">
+        <v>34.25</v>
+      </c>
+      <c r="CH10" s="12">
+        <v>0</v>
+      </c>
+      <c r="CI10" s="12">
+        <v>10</v>
+      </c>
       <c r="CJ10" s="17"/>
-      <c r="CK10" s="18"/>
-      <c r="CL10" s="18"/>
-      <c r="CM10" s="18"/>
-      <c r="CN10" s="18"/>
-      <c r="CO10" s="18"/>
-      <c r="CP10" s="18"/>
-      <c r="CQ10" s="18"/>
+      <c r="CK10" s="18">
+        <v>0.7</v>
+      </c>
+      <c r="CL10" s="18">
+        <v>0</v>
+      </c>
+      <c r="CM10" s="18">
+        <v>0</v>
+      </c>
+      <c r="CN10" s="18">
+        <v>0</v>
+      </c>
+      <c r="CO10" s="18">
+        <v>0</v>
+      </c>
+      <c r="CP10" s="18">
+        <v>0</v>
+      </c>
+      <c r="CQ10" s="18">
+        <v>0</v>
+      </c>
       <c r="CR10" s="17"/>
-      <c r="CS10" s="18"/>
-      <c r="CT10" s="18"/>
-      <c r="CU10" s="18"/>
+      <c r="CS10" s="18">
+        <v>280</v>
+      </c>
+      <c r="CT10" s="18">
+        <v>9900</v>
+      </c>
+      <c r="CU10" s="18">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
+      <c r="A11" s="19">
+        <v>0.46</v>
+      </c>
       <c r="B11" s="1"/>
       <c r="C11" s="8"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="18"/>
-      <c r="R11" s="18"/>
-      <c r="S11" s="18"/>
-      <c r="T11" s="18"/>
-      <c r="U11" s="18"/>
-      <c r="V11" s="18"/>
-      <c r="W11" s="18"/>
-      <c r="X11" s="18"/>
-      <c r="Y11" s="18"/>
+      <c r="D11" s="17">
+        <v>0</v>
+      </c>
+      <c r="E11" s="18">
+        <v>63</v>
+      </c>
+      <c r="F11" s="18">
+        <v>47</v>
+      </c>
+      <c r="G11" s="18">
+        <v>46</v>
+      </c>
+      <c r="H11" s="18">
+        <v>0</v>
+      </c>
+      <c r="I11" s="18">
+        <v>0</v>
+      </c>
+      <c r="J11" s="18">
+        <v>0</v>
+      </c>
+      <c r="K11" s="18">
+        <v>0</v>
+      </c>
+      <c r="L11" s="18">
+        <v>0</v>
+      </c>
+      <c r="M11" s="18">
+        <v>0</v>
+      </c>
+      <c r="N11" s="18">
+        <v>0</v>
+      </c>
+      <c r="O11" s="18">
+        <v>0</v>
+      </c>
+      <c r="P11" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="18">
+        <v>0</v>
+      </c>
+      <c r="R11" s="18">
+        <v>34.020000000000003</v>
+      </c>
+      <c r="S11" s="18">
+        <v>0</v>
+      </c>
+      <c r="T11" s="41">
+        <v>12</v>
+      </c>
+      <c r="U11" s="18">
+        <v>175</v>
+      </c>
+      <c r="V11" s="18">
+        <v>33.9</v>
+      </c>
+      <c r="W11" s="18">
+        <v>0</v>
+      </c>
+      <c r="X11" s="18">
+        <v>12</v>
+      </c>
+      <c r="Y11" s="12">
+        <v>404</v>
+      </c>
       <c r="Z11" s="17"/>
-      <c r="AA11" s="18"/>
-      <c r="AB11" s="18"/>
-      <c r="AC11" s="18"/>
-      <c r="AD11" s="18"/>
-      <c r="AE11" s="18"/>
-      <c r="AF11" s="18"/>
-      <c r="AG11" s="18"/>
-      <c r="AH11" s="18"/>
-      <c r="AI11" s="18"/>
-      <c r="AJ11" s="18"/>
-      <c r="AK11" s="18"/>
-      <c r="AL11" s="18"/>
-      <c r="AM11" s="18"/>
-      <c r="AN11" s="18"/>
-      <c r="AO11" s="18"/>
-      <c r="AP11" s="18"/>
-      <c r="AQ11" s="18"/>
-      <c r="AR11" s="18"/>
-      <c r="AS11" s="18"/>
-      <c r="AT11" s="18"/>
-      <c r="AU11" s="18"/>
-      <c r="AV11" s="18"/>
+      <c r="AA11" s="18">
+        <v>175</v>
+      </c>
+      <c r="AB11" s="18">
+        <v>200</v>
+      </c>
+      <c r="AC11" s="18">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="18">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="18">
+        <v>0</v>
+      </c>
+      <c r="AF11" s="18">
+        <v>0</v>
+      </c>
+      <c r="AG11" s="18">
+        <v>0</v>
+      </c>
+      <c r="AH11" s="18">
+        <v>0</v>
+      </c>
+      <c r="AI11" s="18">
+        <v>10.25</v>
+      </c>
+      <c r="AJ11" s="18">
+        <v>10.25</v>
+      </c>
+      <c r="AK11" s="18">
+        <v>-0.25</v>
+      </c>
+      <c r="AL11" s="18">
+        <v>1.9</v>
+      </c>
+      <c r="AM11" s="18">
+        <v>0</v>
+      </c>
+      <c r="AN11" s="18">
+        <v>0</v>
+      </c>
+      <c r="AO11" s="18">
+        <v>0</v>
+      </c>
+      <c r="AP11" s="18">
+        <v>0</v>
+      </c>
+      <c r="AQ11" s="18">
+        <v>0</v>
+      </c>
+      <c r="AR11" s="18">
+        <v>0</v>
+      </c>
+      <c r="AS11" s="18">
+        <v>0</v>
+      </c>
+      <c r="AT11" s="18">
+        <v>0</v>
+      </c>
+      <c r="AU11" s="18">
+        <v>10</v>
+      </c>
+      <c r="AV11" s="18">
+        <v>30</v>
+      </c>
       <c r="AW11" s="17"/>
-      <c r="AX11" s="18"/>
-      <c r="AY11" s="18"/>
-      <c r="AZ11" s="18"/>
-      <c r="BA11" s="18"/>
-      <c r="BB11" s="18"/>
-      <c r="BC11" s="18"/>
+      <c r="AX11" s="18">
+        <v>900</v>
+      </c>
+      <c r="AY11" s="18">
+        <v>10.5</v>
+      </c>
+      <c r="AZ11" s="18">
+        <v>0.03</v>
+      </c>
+      <c r="BA11" s="18">
+        <v>120.628</v>
+      </c>
+      <c r="BB11" s="18">
+        <v>70.396699999999996</v>
+      </c>
+      <c r="BC11" s="18">
+        <v>0</v>
+      </c>
       <c r="BD11" s="17"/>
-      <c r="BE11" s="18"/>
-      <c r="BF11" s="18"/>
-      <c r="BG11" s="18"/>
-      <c r="BH11" s="18"/>
-      <c r="BI11" s="18"/>
-      <c r="BJ11" s="18"/>
-      <c r="BK11" s="18"/>
-      <c r="BL11" s="18"/>
-      <c r="BM11" s="18"/>
-      <c r="BN11" s="18"/>
-      <c r="BO11" s="18"/>
-      <c r="BP11" s="18"/>
-      <c r="BQ11" s="18"/>
+      <c r="BE11" s="12">
+        <v>1</v>
+      </c>
+      <c r="BF11" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="BG11" s="12">
+        <v>2</v>
+      </c>
+      <c r="BH11" s="12">
+        <v>1.62</v>
+      </c>
+      <c r="BI11" s="12">
+        <v>1.333</v>
+      </c>
+      <c r="BJ11" s="12">
+        <v>1.095</v>
+      </c>
+      <c r="BK11" s="12">
+        <v>2.6520000000000001</v>
+      </c>
+      <c r="BL11" s="12">
+        <v>2.714</v>
+      </c>
+      <c r="BM11" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="BN11" s="12">
+        <v>0</v>
+      </c>
+      <c r="BO11" s="12">
+        <v>0</v>
+      </c>
+      <c r="BP11" s="12">
+        <v>0</v>
+      </c>
+      <c r="BQ11" s="12">
+        <v>20</v>
+      </c>
       <c r="BR11" s="17"/>
-      <c r="BS11" s="18"/>
-      <c r="BT11" s="18"/>
-      <c r="BU11" s="18"/>
-      <c r="BV11" s="18"/>
-      <c r="BW11" s="18"/>
-      <c r="BX11" s="18"/>
+      <c r="BS11" s="12">
+        <v>6762.75</v>
+      </c>
+      <c r="BT11" s="12">
+        <v>3238.5</v>
+      </c>
+      <c r="BU11" s="12">
+        <v>0</v>
+      </c>
+      <c r="BV11" s="12">
+        <v>0</v>
+      </c>
+      <c r="BW11" s="12">
+        <v>0</v>
+      </c>
+      <c r="BX11" s="12">
+        <v>0.96699999999999997</v>
+      </c>
       <c r="BY11" s="17"/>
-      <c r="BZ11" s="18"/>
-      <c r="CA11" s="18"/>
-      <c r="CB11" s="18"/>
-      <c r="CC11" s="18"/>
-      <c r="CD11" s="18"/>
-      <c r="CE11" s="18"/>
-      <c r="CF11" s="18"/>
-      <c r="CG11" s="18"/>
-      <c r="CH11" s="18"/>
-      <c r="CI11" s="18"/>
+      <c r="BZ11" s="12">
+        <v>0</v>
+      </c>
+      <c r="CA11" s="12">
+        <v>0</v>
+      </c>
+      <c r="CB11" s="12">
+        <v>0</v>
+      </c>
+      <c r="CC11" s="12">
+        <v>0.45</v>
+      </c>
+      <c r="CD11" s="12">
+        <v>-0.89</v>
+      </c>
+      <c r="CE11" s="12">
+        <v>2015</v>
+      </c>
+      <c r="CF11" s="12">
+        <v>2.3289999999999999E-3</v>
+      </c>
+      <c r="CG11" s="12">
+        <v>34.25</v>
+      </c>
+      <c r="CH11" s="12">
+        <v>0</v>
+      </c>
+      <c r="CI11" s="12">
+        <v>10</v>
+      </c>
       <c r="CJ11" s="17"/>
-      <c r="CK11" s="18"/>
-      <c r="CL11" s="18"/>
-      <c r="CM11" s="18"/>
-      <c r="CN11" s="18"/>
-      <c r="CO11" s="18"/>
-      <c r="CP11" s="18"/>
-      <c r="CQ11" s="18"/>
+      <c r="CK11" s="18">
+        <v>0.7</v>
+      </c>
+      <c r="CL11" s="18">
+        <v>0</v>
+      </c>
+      <c r="CM11" s="18">
+        <v>0</v>
+      </c>
+      <c r="CN11" s="18">
+        <v>0</v>
+      </c>
+      <c r="CO11" s="18">
+        <v>0</v>
+      </c>
+      <c r="CP11" s="18">
+        <v>0</v>
+      </c>
+      <c r="CQ11" s="18">
+        <v>0</v>
+      </c>
       <c r="CR11" s="17"/>
-      <c r="CS11" s="18"/>
-      <c r="CT11" s="18"/>
-      <c r="CU11" s="18"/>
+      <c r="CS11" s="18">
+        <v>280</v>
+      </c>
+      <c r="CT11" s="18">
+        <v>9900</v>
+      </c>
+      <c r="CU11" s="18">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
+      <c r="A12" s="19">
+        <v>0.47</v>
+      </c>
       <c r="B12" s="1"/>
       <c r="C12" s="8"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="18"/>
-      <c r="S12" s="18"/>
-      <c r="T12" s="18"/>
-      <c r="U12" s="18"/>
-      <c r="V12" s="18"/>
-      <c r="W12" s="18"/>
-      <c r="X12" s="18"/>
-      <c r="Y12" s="18"/>
+      <c r="D12" s="17">
+        <v>0</v>
+      </c>
+      <c r="E12" s="18">
+        <v>63</v>
+      </c>
+      <c r="F12" s="18">
+        <v>47</v>
+      </c>
+      <c r="G12" s="18">
+        <v>46</v>
+      </c>
+      <c r="H12" s="18">
+        <v>0</v>
+      </c>
+      <c r="I12" s="18">
+        <v>0</v>
+      </c>
+      <c r="J12" s="18">
+        <v>0</v>
+      </c>
+      <c r="K12" s="18">
+        <v>0</v>
+      </c>
+      <c r="L12" s="18">
+        <v>0</v>
+      </c>
+      <c r="M12" s="18">
+        <v>0</v>
+      </c>
+      <c r="N12" s="18">
+        <v>0</v>
+      </c>
+      <c r="O12" s="18">
+        <v>0</v>
+      </c>
+      <c r="P12" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="18">
+        <v>0</v>
+      </c>
+      <c r="R12" s="18">
+        <v>33.39</v>
+      </c>
+      <c r="S12" s="18">
+        <v>0</v>
+      </c>
+      <c r="T12" s="41">
+        <v>12</v>
+      </c>
+      <c r="U12" s="18">
+        <v>175</v>
+      </c>
+      <c r="V12" s="18">
+        <v>33.9</v>
+      </c>
+      <c r="W12" s="18">
+        <v>0</v>
+      </c>
+      <c r="X12" s="18">
+        <v>12</v>
+      </c>
+      <c r="Y12" s="12">
+        <v>404</v>
+      </c>
       <c r="Z12" s="17"/>
-      <c r="AA12" s="18"/>
-      <c r="AB12" s="18"/>
-      <c r="AC12" s="18"/>
-      <c r="AD12" s="18"/>
-      <c r="AE12" s="18"/>
-      <c r="AF12" s="18"/>
-      <c r="AG12" s="18"/>
-      <c r="AH12" s="18"/>
-      <c r="AI12" s="18"/>
-      <c r="AJ12" s="18"/>
-      <c r="AK12" s="18"/>
-      <c r="AL12" s="18"/>
-      <c r="AM12" s="18"/>
-      <c r="AN12" s="18"/>
-      <c r="AO12" s="18"/>
-      <c r="AP12" s="18"/>
-      <c r="AQ12" s="18"/>
-      <c r="AR12" s="18"/>
-      <c r="AS12" s="18"/>
-      <c r="AT12" s="18"/>
-      <c r="AU12" s="18"/>
-      <c r="AV12" s="18"/>
+      <c r="AA12" s="18">
+        <v>175</v>
+      </c>
+      <c r="AB12" s="18">
+        <v>200</v>
+      </c>
+      <c r="AC12" s="18">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="18">
+        <v>0</v>
+      </c>
+      <c r="AE12" s="18">
+        <v>0</v>
+      </c>
+      <c r="AF12" s="18">
+        <v>0</v>
+      </c>
+      <c r="AG12" s="18">
+        <v>0</v>
+      </c>
+      <c r="AH12" s="18">
+        <v>0</v>
+      </c>
+      <c r="AI12" s="18">
+        <v>10.25</v>
+      </c>
+      <c r="AJ12" s="18">
+        <v>10.25</v>
+      </c>
+      <c r="AK12" s="18">
+        <v>-0.25</v>
+      </c>
+      <c r="AL12" s="18">
+        <v>1.9</v>
+      </c>
+      <c r="AM12" s="18">
+        <v>0</v>
+      </c>
+      <c r="AN12" s="18">
+        <v>0</v>
+      </c>
+      <c r="AO12" s="18">
+        <v>0</v>
+      </c>
+      <c r="AP12" s="18">
+        <v>0</v>
+      </c>
+      <c r="AQ12" s="18">
+        <v>0</v>
+      </c>
+      <c r="AR12" s="18">
+        <v>0</v>
+      </c>
+      <c r="AS12" s="18">
+        <v>0</v>
+      </c>
+      <c r="AT12" s="18">
+        <v>0</v>
+      </c>
+      <c r="AU12" s="18">
+        <v>10</v>
+      </c>
+      <c r="AV12" s="18">
+        <v>30</v>
+      </c>
       <c r="AW12" s="17"/>
-      <c r="AX12" s="18"/>
-      <c r="AY12" s="18"/>
-      <c r="AZ12" s="18"/>
-      <c r="BA12" s="18"/>
-      <c r="BB12" s="18"/>
-      <c r="BC12" s="18"/>
+      <c r="AX12" s="18">
+        <v>900</v>
+      </c>
+      <c r="AY12" s="18">
+        <v>10.5</v>
+      </c>
+      <c r="AZ12" s="18">
+        <v>0.03</v>
+      </c>
+      <c r="BA12" s="18">
+        <v>120.628</v>
+      </c>
+      <c r="BB12" s="18">
+        <v>70.396699999999996</v>
+      </c>
+      <c r="BC12" s="18">
+        <v>0</v>
+      </c>
       <c r="BD12" s="17"/>
-      <c r="BE12" s="18"/>
-      <c r="BF12" s="18"/>
-      <c r="BG12" s="18"/>
-      <c r="BH12" s="18"/>
-      <c r="BI12" s="18"/>
-      <c r="BJ12" s="18"/>
-      <c r="BK12" s="18"/>
-      <c r="BL12" s="18"/>
-      <c r="BM12" s="18"/>
-      <c r="BN12" s="18"/>
-      <c r="BO12" s="18"/>
-      <c r="BP12" s="18"/>
-      <c r="BQ12" s="18"/>
+      <c r="BE12" s="12">
+        <v>1</v>
+      </c>
+      <c r="BF12" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="BG12" s="12">
+        <v>2</v>
+      </c>
+      <c r="BH12" s="12">
+        <v>1.62</v>
+      </c>
+      <c r="BI12" s="12">
+        <v>1.333</v>
+      </c>
+      <c r="BJ12" s="12">
+        <v>1.095</v>
+      </c>
+      <c r="BK12" s="12">
+        <v>2.6520000000000001</v>
+      </c>
+      <c r="BL12" s="12">
+        <v>2.714</v>
+      </c>
+      <c r="BM12" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="BN12" s="12">
+        <v>0</v>
+      </c>
+      <c r="BO12" s="12">
+        <v>0</v>
+      </c>
+      <c r="BP12" s="12">
+        <v>0</v>
+      </c>
+      <c r="BQ12" s="12">
+        <v>20</v>
+      </c>
       <c r="BR12" s="17"/>
-      <c r="BS12" s="18"/>
-      <c r="BT12" s="18"/>
-      <c r="BU12" s="18"/>
-      <c r="BV12" s="18"/>
-      <c r="BW12" s="18"/>
-      <c r="BX12" s="18"/>
+      <c r="BS12" s="12">
+        <v>6762.75</v>
+      </c>
+      <c r="BT12" s="12">
+        <v>3238.5</v>
+      </c>
+      <c r="BU12" s="12">
+        <v>0</v>
+      </c>
+      <c r="BV12" s="12">
+        <v>0</v>
+      </c>
+      <c r="BW12" s="12">
+        <v>0</v>
+      </c>
+      <c r="BX12" s="12">
+        <v>0.96699999999999997</v>
+      </c>
       <c r="BY12" s="17"/>
-      <c r="BZ12" s="18"/>
-      <c r="CA12" s="18"/>
-      <c r="CB12" s="18"/>
-      <c r="CC12" s="18"/>
-      <c r="CD12" s="18"/>
-      <c r="CE12" s="18"/>
-      <c r="CF12" s="18"/>
-      <c r="CG12" s="18"/>
-      <c r="CH12" s="18"/>
-      <c r="CI12" s="18"/>
+      <c r="BZ12" s="12">
+        <v>0</v>
+      </c>
+      <c r="CA12" s="12">
+        <v>0</v>
+      </c>
+      <c r="CB12" s="12">
+        <v>0</v>
+      </c>
+      <c r="CC12" s="12">
+        <v>0.45</v>
+      </c>
+      <c r="CD12" s="12">
+        <v>-0.89</v>
+      </c>
+      <c r="CE12" s="12">
+        <v>2015</v>
+      </c>
+      <c r="CF12" s="12">
+        <v>2.3289999999999999E-3</v>
+      </c>
+      <c r="CG12" s="12">
+        <v>34.25</v>
+      </c>
+      <c r="CH12" s="12">
+        <v>0</v>
+      </c>
+      <c r="CI12" s="12">
+        <v>10</v>
+      </c>
       <c r="CJ12" s="17"/>
-      <c r="CK12" s="18"/>
-      <c r="CL12" s="18"/>
-      <c r="CM12" s="18"/>
-      <c r="CN12" s="18"/>
-      <c r="CO12" s="18"/>
-      <c r="CP12" s="18"/>
-      <c r="CQ12" s="18"/>
+      <c r="CK12" s="18">
+        <v>0.7</v>
+      </c>
+      <c r="CL12" s="18">
+        <v>0</v>
+      </c>
+      <c r="CM12" s="18">
+        <v>0</v>
+      </c>
+      <c r="CN12" s="18">
+        <v>0</v>
+      </c>
+      <c r="CO12" s="18">
+        <v>0</v>
+      </c>
+      <c r="CP12" s="18">
+        <v>0</v>
+      </c>
+      <c r="CQ12" s="18">
+        <v>0</v>
+      </c>
       <c r="CR12" s="17"/>
-      <c r="CS12" s="18"/>
-      <c r="CT12" s="18"/>
-      <c r="CU12" s="18"/>
+      <c r="CS12" s="18">
+        <v>280</v>
+      </c>
+      <c r="CT12" s="18">
+        <v>9900</v>
+      </c>
+      <c r="CU12" s="18">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
+      <c r="A13" s="23">
+        <v>0.48</v>
+      </c>
       <c r="B13" s="1"/>
       <c r="C13" s="8"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="18"/>
-      <c r="S13" s="18"/>
-      <c r="T13" s="18"/>
-      <c r="U13" s="18"/>
-      <c r="V13" s="18"/>
-      <c r="W13" s="18"/>
-      <c r="X13" s="18"/>
-      <c r="Y13" s="18"/>
+      <c r="D13" s="17">
+        <v>0</v>
+      </c>
+      <c r="E13" s="18">
+        <v>63</v>
+      </c>
+      <c r="F13" s="18">
+        <v>47</v>
+      </c>
+      <c r="G13" s="18">
+        <v>46</v>
+      </c>
+      <c r="H13" s="18">
+        <v>0</v>
+      </c>
+      <c r="I13" s="18">
+        <v>0</v>
+      </c>
+      <c r="J13" s="18">
+        <v>0</v>
+      </c>
+      <c r="K13" s="18">
+        <v>0</v>
+      </c>
+      <c r="L13" s="18">
+        <v>0</v>
+      </c>
+      <c r="M13" s="18">
+        <v>0</v>
+      </c>
+      <c r="N13" s="18">
+        <v>0</v>
+      </c>
+      <c r="O13" s="18">
+        <v>0</v>
+      </c>
+      <c r="P13" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="18">
+        <v>0</v>
+      </c>
+      <c r="R13" s="18">
+        <v>32.76</v>
+      </c>
+      <c r="S13" s="18">
+        <v>0</v>
+      </c>
+      <c r="T13" s="41">
+        <v>12</v>
+      </c>
+      <c r="U13" s="18">
+        <v>175</v>
+      </c>
+      <c r="V13" s="18">
+        <v>33.9</v>
+      </c>
+      <c r="W13" s="18">
+        <v>0</v>
+      </c>
+      <c r="X13" s="18">
+        <v>12</v>
+      </c>
+      <c r="Y13" s="12">
+        <v>404</v>
+      </c>
       <c r="Z13" s="17"/>
-      <c r="AA13" s="18"/>
-      <c r="AB13" s="18"/>
-      <c r="AC13" s="18"/>
-      <c r="AD13" s="18"/>
-      <c r="AE13" s="18"/>
-      <c r="AF13" s="18"/>
-      <c r="AG13" s="18"/>
-      <c r="AH13" s="18"/>
-      <c r="AI13" s="18"/>
-      <c r="AJ13" s="18"/>
-      <c r="AK13" s="18"/>
-      <c r="AL13" s="18"/>
-      <c r="AM13" s="18"/>
-      <c r="AN13" s="18"/>
-      <c r="AO13" s="18"/>
-      <c r="AP13" s="18"/>
-      <c r="AQ13" s="18"/>
-      <c r="AR13" s="18"/>
-      <c r="AS13" s="18"/>
-      <c r="AT13" s="18"/>
-      <c r="AU13" s="18"/>
-      <c r="AV13" s="18"/>
+      <c r="AA13" s="18">
+        <v>175</v>
+      </c>
+      <c r="AB13" s="18">
+        <v>200</v>
+      </c>
+      <c r="AC13" s="18">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="18">
+        <v>0</v>
+      </c>
+      <c r="AE13" s="18">
+        <v>0</v>
+      </c>
+      <c r="AF13" s="18">
+        <v>0</v>
+      </c>
+      <c r="AG13" s="18">
+        <v>0</v>
+      </c>
+      <c r="AH13" s="18">
+        <v>0</v>
+      </c>
+      <c r="AI13" s="18">
+        <v>10.25</v>
+      </c>
+      <c r="AJ13" s="18">
+        <v>10.25</v>
+      </c>
+      <c r="AK13" s="18">
+        <v>-0.25</v>
+      </c>
+      <c r="AL13" s="18">
+        <v>1.9</v>
+      </c>
+      <c r="AM13" s="18">
+        <v>0</v>
+      </c>
+      <c r="AN13" s="18">
+        <v>0</v>
+      </c>
+      <c r="AO13" s="18">
+        <v>0</v>
+      </c>
+      <c r="AP13" s="18">
+        <v>0</v>
+      </c>
+      <c r="AQ13" s="18">
+        <v>0</v>
+      </c>
+      <c r="AR13" s="18">
+        <v>0</v>
+      </c>
+      <c r="AS13" s="18">
+        <v>0</v>
+      </c>
+      <c r="AT13" s="18">
+        <v>0</v>
+      </c>
+      <c r="AU13" s="18">
+        <v>10</v>
+      </c>
+      <c r="AV13" s="18">
+        <v>30</v>
+      </c>
       <c r="AW13" s="17"/>
-      <c r="AX13" s="18"/>
-      <c r="AY13" s="18"/>
-      <c r="AZ13" s="18"/>
-      <c r="BA13" s="18"/>
-      <c r="BB13" s="18"/>
-      <c r="BC13" s="18"/>
+      <c r="AX13" s="18">
+        <v>900</v>
+      </c>
+      <c r="AY13" s="18">
+        <v>10.5</v>
+      </c>
+      <c r="AZ13" s="18">
+        <v>0.03</v>
+      </c>
+      <c r="BA13" s="18">
+        <v>120.628</v>
+      </c>
+      <c r="BB13" s="18">
+        <v>70.396699999999996</v>
+      </c>
+      <c r="BC13" s="18">
+        <v>0</v>
+      </c>
       <c r="BD13" s="17"/>
-      <c r="BE13" s="18"/>
-      <c r="BF13" s="18"/>
-      <c r="BG13" s="18"/>
-      <c r="BH13" s="18"/>
-      <c r="BI13" s="18"/>
-      <c r="BJ13" s="18"/>
-      <c r="BK13" s="18"/>
-      <c r="BL13" s="18"/>
-      <c r="BM13" s="18"/>
-      <c r="BN13" s="18"/>
-      <c r="BO13" s="18"/>
-      <c r="BP13" s="18"/>
-      <c r="BQ13" s="18"/>
+      <c r="BE13" s="12">
+        <v>1</v>
+      </c>
+      <c r="BF13" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="BG13" s="12">
+        <v>2</v>
+      </c>
+      <c r="BH13" s="12">
+        <v>1.62</v>
+      </c>
+      <c r="BI13" s="12">
+        <v>1.333</v>
+      </c>
+      <c r="BJ13" s="12">
+        <v>1.095</v>
+      </c>
+      <c r="BK13" s="12">
+        <v>2.6520000000000001</v>
+      </c>
+      <c r="BL13" s="12">
+        <v>2.714</v>
+      </c>
+      <c r="BM13" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="BN13" s="12">
+        <v>0</v>
+      </c>
+      <c r="BO13" s="12">
+        <v>0</v>
+      </c>
+      <c r="BP13" s="12">
+        <v>0</v>
+      </c>
+      <c r="BQ13" s="12">
+        <v>20</v>
+      </c>
       <c r="BR13" s="17"/>
-      <c r="BS13" s="18"/>
-      <c r="BT13" s="18"/>
-      <c r="BU13" s="18"/>
-      <c r="BV13" s="18"/>
-      <c r="BW13" s="18"/>
-      <c r="BX13" s="18"/>
+      <c r="BS13" s="12">
+        <v>6762.75</v>
+      </c>
+      <c r="BT13" s="12">
+        <v>3238.5</v>
+      </c>
+      <c r="BU13" s="12">
+        <v>0</v>
+      </c>
+      <c r="BV13" s="12">
+        <v>0</v>
+      </c>
+      <c r="BW13" s="12">
+        <v>0</v>
+      </c>
+      <c r="BX13" s="12">
+        <v>0.96699999999999997</v>
+      </c>
       <c r="BY13" s="17"/>
-      <c r="BZ13" s="18"/>
-      <c r="CA13" s="18"/>
-      <c r="CB13" s="18"/>
-      <c r="CC13" s="18"/>
-      <c r="CD13" s="18"/>
-      <c r="CE13" s="18"/>
-      <c r="CF13" s="18"/>
-      <c r="CG13" s="18"/>
-      <c r="CH13" s="18"/>
-      <c r="CI13" s="18"/>
+      <c r="BZ13" s="12">
+        <v>0</v>
+      </c>
+      <c r="CA13" s="12">
+        <v>0</v>
+      </c>
+      <c r="CB13" s="12">
+        <v>0</v>
+      </c>
+      <c r="CC13" s="12">
+        <v>0.45</v>
+      </c>
+      <c r="CD13" s="12">
+        <v>-0.89</v>
+      </c>
+      <c r="CE13" s="12">
+        <v>2015</v>
+      </c>
+      <c r="CF13" s="12">
+        <v>2.3289999999999999E-3</v>
+      </c>
+      <c r="CG13" s="12">
+        <v>34.25</v>
+      </c>
+      <c r="CH13" s="12">
+        <v>0</v>
+      </c>
+      <c r="CI13" s="12">
+        <v>10</v>
+      </c>
       <c r="CJ13" s="17"/>
-      <c r="CK13" s="18"/>
-      <c r="CL13" s="18"/>
-      <c r="CM13" s="18"/>
-      <c r="CN13" s="18"/>
-      <c r="CO13" s="18"/>
-      <c r="CP13" s="18"/>
-      <c r="CQ13" s="18"/>
+      <c r="CK13" s="18">
+        <v>0.7</v>
+      </c>
+      <c r="CL13" s="18">
+        <v>0</v>
+      </c>
+      <c r="CM13" s="18">
+        <v>0</v>
+      </c>
+      <c r="CN13" s="18">
+        <v>0</v>
+      </c>
+      <c r="CO13" s="18">
+        <v>0</v>
+      </c>
+      <c r="CP13" s="18">
+        <v>0</v>
+      </c>
+      <c r="CQ13" s="18">
+        <v>0</v>
+      </c>
       <c r="CR13" s="17"/>
-      <c r="CS13" s="18"/>
-      <c r="CT13" s="18"/>
-      <c r="CU13" s="18"/>
+      <c r="CS13" s="18">
+        <v>280</v>
+      </c>
+      <c r="CT13" s="18">
+        <v>9900</v>
+      </c>
+      <c r="CU13" s="18">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
+      <c r="A14" s="19">
+        <v>0.49</v>
+      </c>
       <c r="B14" s="1"/>
       <c r="C14" s="8"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="18"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="18"/>
-      <c r="T14" s="18"/>
-      <c r="U14" s="18"/>
-      <c r="V14" s="18"/>
-      <c r="W14" s="18"/>
-      <c r="X14" s="18"/>
-      <c r="Y14" s="18"/>
+      <c r="D14" s="17">
+        <v>0</v>
+      </c>
+      <c r="E14" s="18">
+        <v>63</v>
+      </c>
+      <c r="F14" s="18">
+        <v>47</v>
+      </c>
+      <c r="G14" s="18">
+        <v>46</v>
+      </c>
+      <c r="H14" s="18">
+        <v>0</v>
+      </c>
+      <c r="I14" s="18">
+        <v>0</v>
+      </c>
+      <c r="J14" s="18">
+        <v>0</v>
+      </c>
+      <c r="K14" s="18">
+        <v>0</v>
+      </c>
+      <c r="L14" s="18">
+        <v>0</v>
+      </c>
+      <c r="M14" s="18">
+        <v>0</v>
+      </c>
+      <c r="N14" s="18">
+        <v>0</v>
+      </c>
+      <c r="O14" s="18">
+        <v>0</v>
+      </c>
+      <c r="P14" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="18">
+        <v>0</v>
+      </c>
+      <c r="R14" s="18">
+        <v>32.130000000000003</v>
+      </c>
+      <c r="S14" s="18">
+        <v>0</v>
+      </c>
+      <c r="T14" s="41">
+        <v>12</v>
+      </c>
+      <c r="U14" s="18">
+        <v>175</v>
+      </c>
+      <c r="V14" s="18">
+        <v>33.9</v>
+      </c>
+      <c r="W14" s="18">
+        <v>0</v>
+      </c>
+      <c r="X14" s="18">
+        <v>12</v>
+      </c>
+      <c r="Y14" s="12">
+        <v>404</v>
+      </c>
       <c r="Z14" s="17"/>
-      <c r="AA14" s="18"/>
-      <c r="AB14" s="18"/>
-      <c r="AC14" s="18"/>
-      <c r="AD14" s="18"/>
-      <c r="AE14" s="18"/>
-      <c r="AF14" s="18"/>
-      <c r="AG14" s="18"/>
-      <c r="AH14" s="18"/>
-      <c r="AI14" s="18"/>
-      <c r="AJ14" s="18"/>
-      <c r="AK14" s="18"/>
-      <c r="AL14" s="18"/>
-      <c r="AM14" s="18"/>
-      <c r="AN14" s="18"/>
-      <c r="AO14" s="18"/>
-      <c r="AP14" s="18"/>
-      <c r="AQ14" s="18"/>
-      <c r="AR14" s="18"/>
-      <c r="AS14" s="18"/>
-      <c r="AT14" s="18"/>
-      <c r="AU14" s="18"/>
-      <c r="AV14" s="18"/>
+      <c r="AA14" s="18">
+        <v>175</v>
+      </c>
+      <c r="AB14" s="18">
+        <v>200</v>
+      </c>
+      <c r="AC14" s="18">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="18">
+        <v>0</v>
+      </c>
+      <c r="AE14" s="18">
+        <v>0</v>
+      </c>
+      <c r="AF14" s="18">
+        <v>0</v>
+      </c>
+      <c r="AG14" s="18">
+        <v>0</v>
+      </c>
+      <c r="AH14" s="18">
+        <v>0</v>
+      </c>
+      <c r="AI14" s="18">
+        <v>10.25</v>
+      </c>
+      <c r="AJ14" s="18">
+        <v>10.25</v>
+      </c>
+      <c r="AK14" s="18">
+        <v>-0.25</v>
+      </c>
+      <c r="AL14" s="18">
+        <v>1.9</v>
+      </c>
+      <c r="AM14" s="18">
+        <v>0</v>
+      </c>
+      <c r="AN14" s="18">
+        <v>0</v>
+      </c>
+      <c r="AO14" s="18">
+        <v>0</v>
+      </c>
+      <c r="AP14" s="18">
+        <v>0</v>
+      </c>
+      <c r="AQ14" s="18">
+        <v>0</v>
+      </c>
+      <c r="AR14" s="18">
+        <v>0</v>
+      </c>
+      <c r="AS14" s="18">
+        <v>0</v>
+      </c>
+      <c r="AT14" s="18">
+        <v>0</v>
+      </c>
+      <c r="AU14" s="18">
+        <v>10</v>
+      </c>
+      <c r="AV14" s="18">
+        <v>30</v>
+      </c>
       <c r="AW14" s="17"/>
-      <c r="AX14" s="18"/>
-      <c r="AY14" s="18"/>
-      <c r="AZ14" s="18"/>
-      <c r="BA14" s="18"/>
-      <c r="BB14" s="18"/>
-      <c r="BC14" s="18"/>
+      <c r="AX14" s="18">
+        <v>900</v>
+      </c>
+      <c r="AY14" s="18">
+        <v>10.5</v>
+      </c>
+      <c r="AZ14" s="18">
+        <v>0.03</v>
+      </c>
+      <c r="BA14" s="18">
+        <v>120.628</v>
+      </c>
+      <c r="BB14" s="18">
+        <v>70.396699999999996</v>
+      </c>
+      <c r="BC14" s="18">
+        <v>0</v>
+      </c>
       <c r="BD14" s="17"/>
-      <c r="BE14" s="18"/>
-      <c r="BF14" s="18"/>
-      <c r="BG14" s="18"/>
-      <c r="BH14" s="18"/>
-      <c r="BI14" s="18"/>
-      <c r="BJ14" s="18"/>
-      <c r="BK14" s="18"/>
-      <c r="BL14" s="18"/>
-      <c r="BM14" s="18"/>
-      <c r="BN14" s="18"/>
-      <c r="BO14" s="18"/>
-      <c r="BP14" s="18"/>
-      <c r="BQ14" s="18"/>
+      <c r="BE14" s="12">
+        <v>1</v>
+      </c>
+      <c r="BF14" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="BG14" s="12">
+        <v>2</v>
+      </c>
+      <c r="BH14" s="12">
+        <v>1.62</v>
+      </c>
+      <c r="BI14" s="12">
+        <v>1.333</v>
+      </c>
+      <c r="BJ14" s="12">
+        <v>1.095</v>
+      </c>
+      <c r="BK14" s="12">
+        <v>2.6520000000000001</v>
+      </c>
+      <c r="BL14" s="12">
+        <v>2.714</v>
+      </c>
+      <c r="BM14" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="BN14" s="12">
+        <v>0</v>
+      </c>
+      <c r="BO14" s="12">
+        <v>0</v>
+      </c>
+      <c r="BP14" s="12">
+        <v>0</v>
+      </c>
+      <c r="BQ14" s="12">
+        <v>20</v>
+      </c>
       <c r="BR14" s="17"/>
-      <c r="BS14" s="18"/>
-      <c r="BT14" s="18"/>
-      <c r="BU14" s="18"/>
-      <c r="BV14" s="18"/>
-      <c r="BW14" s="18"/>
-      <c r="BX14" s="18"/>
+      <c r="BS14" s="12">
+        <v>6762.75</v>
+      </c>
+      <c r="BT14" s="12">
+        <v>3238.5</v>
+      </c>
+      <c r="BU14" s="12">
+        <v>0</v>
+      </c>
+      <c r="BV14" s="12">
+        <v>0</v>
+      </c>
+      <c r="BW14" s="12">
+        <v>0</v>
+      </c>
+      <c r="BX14" s="12">
+        <v>0.96699999999999997</v>
+      </c>
       <c r="BY14" s="17"/>
-      <c r="BZ14" s="18"/>
-      <c r="CA14" s="18"/>
-      <c r="CB14" s="18"/>
-      <c r="CC14" s="18"/>
-      <c r="CD14" s="18"/>
-      <c r="CE14" s="18"/>
-      <c r="CF14" s="18"/>
-      <c r="CG14" s="18"/>
-      <c r="CH14" s="18"/>
-      <c r="CI14" s="18"/>
+      <c r="BZ14" s="12">
+        <v>0</v>
+      </c>
+      <c r="CA14" s="12">
+        <v>0</v>
+      </c>
+      <c r="CB14" s="12">
+        <v>0</v>
+      </c>
+      <c r="CC14" s="12">
+        <v>0.45</v>
+      </c>
+      <c r="CD14" s="12">
+        <v>-0.89</v>
+      </c>
+      <c r="CE14" s="12">
+        <v>2015</v>
+      </c>
+      <c r="CF14" s="12">
+        <v>2.3289999999999999E-3</v>
+      </c>
+      <c r="CG14" s="12">
+        <v>34.25</v>
+      </c>
+      <c r="CH14" s="12">
+        <v>0</v>
+      </c>
+      <c r="CI14" s="12">
+        <v>10</v>
+      </c>
       <c r="CJ14" s="17"/>
-      <c r="CK14" s="18"/>
-      <c r="CL14" s="18"/>
-      <c r="CM14" s="18"/>
-      <c r="CN14" s="18"/>
-      <c r="CO14" s="18"/>
-      <c r="CP14" s="18"/>
-      <c r="CQ14" s="18"/>
+      <c r="CK14" s="18">
+        <v>0.7</v>
+      </c>
+      <c r="CL14" s="18">
+        <v>0</v>
+      </c>
+      <c r="CM14" s="18">
+        <v>0</v>
+      </c>
+      <c r="CN14" s="18">
+        <v>0</v>
+      </c>
+      <c r="CO14" s="18">
+        <v>0</v>
+      </c>
+      <c r="CP14" s="18">
+        <v>0</v>
+      </c>
+      <c r="CQ14" s="18">
+        <v>0</v>
+      </c>
       <c r="CR14" s="17"/>
-      <c r="CS14" s="18"/>
-      <c r="CT14" s="18"/>
-      <c r="CU14" s="18"/>
+      <c r="CS14" s="18">
+        <v>280</v>
+      </c>
+      <c r="CT14" s="18">
+        <v>9900</v>
+      </c>
+      <c r="CU14" s="18">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
+      <c r="A15" s="19">
+        <v>0.5</v>
+      </c>
       <c r="B15" s="1"/>
       <c r="C15" s="8"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="18"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="18"/>
-      <c r="Q15" s="18"/>
-      <c r="R15" s="18"/>
-      <c r="S15" s="18"/>
-      <c r="T15" s="18"/>
-      <c r="U15" s="18"/>
-      <c r="V15" s="18"/>
-      <c r="W15" s="18"/>
-      <c r="X15" s="18"/>
-      <c r="Y15" s="18"/>
+      <c r="D15" s="17">
+        <v>0</v>
+      </c>
+      <c r="E15" s="18">
+        <v>63</v>
+      </c>
+      <c r="F15" s="18">
+        <v>47</v>
+      </c>
+      <c r="G15" s="18">
+        <v>46</v>
+      </c>
+      <c r="H15" s="18">
+        <v>0</v>
+      </c>
+      <c r="I15" s="18">
+        <v>0</v>
+      </c>
+      <c r="J15" s="18">
+        <v>0</v>
+      </c>
+      <c r="K15" s="18">
+        <v>0</v>
+      </c>
+      <c r="L15" s="18">
+        <v>0</v>
+      </c>
+      <c r="M15" s="18">
+        <v>0</v>
+      </c>
+      <c r="N15" s="18">
+        <v>0</v>
+      </c>
+      <c r="O15" s="18">
+        <v>0</v>
+      </c>
+      <c r="P15" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="18">
+        <v>0</v>
+      </c>
+      <c r="R15" s="18">
+        <v>31.5</v>
+      </c>
+      <c r="S15" s="18">
+        <v>0</v>
+      </c>
+      <c r="T15" s="41">
+        <v>12</v>
+      </c>
+      <c r="U15" s="18">
+        <v>175</v>
+      </c>
+      <c r="V15" s="18">
+        <v>33.9</v>
+      </c>
+      <c r="W15" s="18">
+        <v>0</v>
+      </c>
+      <c r="X15" s="18">
+        <v>12</v>
+      </c>
+      <c r="Y15" s="12">
+        <v>404</v>
+      </c>
       <c r="Z15" s="17"/>
-      <c r="AA15" s="18"/>
-      <c r="AB15" s="18"/>
-      <c r="AC15" s="18"/>
-      <c r="AD15" s="18"/>
-      <c r="AE15" s="18"/>
-      <c r="AF15" s="18"/>
-      <c r="AG15" s="18"/>
-      <c r="AH15" s="18"/>
-      <c r="AI15" s="18"/>
-      <c r="AJ15" s="18"/>
-      <c r="AK15" s="18"/>
-      <c r="AL15" s="18"/>
-      <c r="AM15" s="18"/>
-      <c r="AN15" s="18"/>
-      <c r="AO15" s="18"/>
-      <c r="AP15" s="18"/>
-      <c r="AQ15" s="18"/>
-      <c r="AR15" s="18"/>
-      <c r="AS15" s="18"/>
-      <c r="AT15" s="18"/>
-      <c r="AU15" s="18"/>
-      <c r="AV15" s="18"/>
+      <c r="AA15" s="18">
+        <v>175</v>
+      </c>
+      <c r="AB15" s="18">
+        <v>200</v>
+      </c>
+      <c r="AC15" s="18">
+        <v>0</v>
+      </c>
+      <c r="AD15" s="18">
+        <v>0</v>
+      </c>
+      <c r="AE15" s="18">
+        <v>0</v>
+      </c>
+      <c r="AF15" s="18">
+        <v>0</v>
+      </c>
+      <c r="AG15" s="18">
+        <v>0</v>
+      </c>
+      <c r="AH15" s="18">
+        <v>0</v>
+      </c>
+      <c r="AI15" s="18">
+        <v>10.25</v>
+      </c>
+      <c r="AJ15" s="18">
+        <v>10.25</v>
+      </c>
+      <c r="AK15" s="18">
+        <v>-0.25</v>
+      </c>
+      <c r="AL15" s="18">
+        <v>1.9</v>
+      </c>
+      <c r="AM15" s="18">
+        <v>0</v>
+      </c>
+      <c r="AN15" s="18">
+        <v>0</v>
+      </c>
+      <c r="AO15" s="18">
+        <v>0</v>
+      </c>
+      <c r="AP15" s="18">
+        <v>0</v>
+      </c>
+      <c r="AQ15" s="18">
+        <v>0</v>
+      </c>
+      <c r="AR15" s="18">
+        <v>0</v>
+      </c>
+      <c r="AS15" s="18">
+        <v>0</v>
+      </c>
+      <c r="AT15" s="18">
+        <v>0</v>
+      </c>
+      <c r="AU15" s="18">
+        <v>10</v>
+      </c>
+      <c r="AV15" s="18">
+        <v>30</v>
+      </c>
       <c r="AW15" s="17"/>
-      <c r="AX15" s="18"/>
-      <c r="AY15" s="18"/>
-      <c r="AZ15" s="18"/>
-      <c r="BA15" s="18"/>
-      <c r="BB15" s="18"/>
-      <c r="BC15" s="18"/>
+      <c r="AX15" s="18">
+        <v>900</v>
+      </c>
+      <c r="AY15" s="18">
+        <v>10.5</v>
+      </c>
+      <c r="AZ15" s="18">
+        <v>0.03</v>
+      </c>
+      <c r="BA15" s="18">
+        <v>120.628</v>
+      </c>
+      <c r="BB15" s="18">
+        <v>70.396699999999996</v>
+      </c>
+      <c r="BC15" s="18">
+        <v>0</v>
+      </c>
       <c r="BD15" s="17"/>
-      <c r="BE15" s="18"/>
-      <c r="BF15" s="18"/>
-      <c r="BG15" s="18"/>
-      <c r="BH15" s="18"/>
-      <c r="BI15" s="18"/>
-      <c r="BJ15" s="18"/>
-      <c r="BK15" s="18"/>
-      <c r="BL15" s="18"/>
-      <c r="BM15" s="18"/>
-      <c r="BN15" s="18"/>
-      <c r="BO15" s="18"/>
-      <c r="BP15" s="18"/>
-      <c r="BQ15" s="18"/>
+      <c r="BE15" s="12">
+        <v>1</v>
+      </c>
+      <c r="BF15" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="BG15" s="12">
+        <v>2</v>
+      </c>
+      <c r="BH15" s="12">
+        <v>1.62</v>
+      </c>
+      <c r="BI15" s="12">
+        <v>1.333</v>
+      </c>
+      <c r="BJ15" s="12">
+        <v>1.095</v>
+      </c>
+      <c r="BK15" s="12">
+        <v>2.6520000000000001</v>
+      </c>
+      <c r="BL15" s="12">
+        <v>2.714</v>
+      </c>
+      <c r="BM15" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="BN15" s="12">
+        <v>0</v>
+      </c>
+      <c r="BO15" s="12">
+        <v>0</v>
+      </c>
+      <c r="BP15" s="12">
+        <v>0</v>
+      </c>
+      <c r="BQ15" s="12">
+        <v>20</v>
+      </c>
       <c r="BR15" s="17"/>
-      <c r="BS15" s="18"/>
-      <c r="BT15" s="18"/>
-      <c r="BU15" s="18"/>
-      <c r="BV15" s="18"/>
-      <c r="BW15" s="18"/>
-      <c r="BX15" s="18"/>
+      <c r="BS15" s="12">
+        <v>6762.75</v>
+      </c>
+      <c r="BT15" s="12">
+        <v>3238.5</v>
+      </c>
+      <c r="BU15" s="12">
+        <v>0</v>
+      </c>
+      <c r="BV15" s="12">
+        <v>0</v>
+      </c>
+      <c r="BW15" s="12">
+        <v>0</v>
+      </c>
+      <c r="BX15" s="12">
+        <v>0.96699999999999997</v>
+      </c>
       <c r="BY15" s="17"/>
-      <c r="BZ15" s="18"/>
-      <c r="CA15" s="18"/>
-      <c r="CB15" s="18"/>
-      <c r="CC15" s="18"/>
-      <c r="CD15" s="18"/>
-      <c r="CE15" s="18"/>
-      <c r="CF15" s="18"/>
-      <c r="CG15" s="18"/>
-      <c r="CH15" s="18"/>
-      <c r="CI15" s="18"/>
+      <c r="BZ15" s="12">
+        <v>0</v>
+      </c>
+      <c r="CA15" s="12">
+        <v>0</v>
+      </c>
+      <c r="CB15" s="12">
+        <v>0</v>
+      </c>
+      <c r="CC15" s="12">
+        <v>0.45</v>
+      </c>
+      <c r="CD15" s="12">
+        <v>-0.89</v>
+      </c>
+      <c r="CE15" s="12">
+        <v>2015</v>
+      </c>
+      <c r="CF15" s="12">
+        <v>2.3289999999999999E-3</v>
+      </c>
+      <c r="CG15" s="12">
+        <v>34.25</v>
+      </c>
+      <c r="CH15" s="12">
+        <v>0</v>
+      </c>
+      <c r="CI15" s="12">
+        <v>10</v>
+      </c>
       <c r="CJ15" s="17"/>
-      <c r="CK15" s="18"/>
-      <c r="CL15" s="18"/>
-      <c r="CM15" s="18"/>
-      <c r="CN15" s="18"/>
-      <c r="CO15" s="18"/>
-      <c r="CP15" s="18"/>
-      <c r="CQ15" s="18"/>
+      <c r="CK15" s="18">
+        <v>0.7</v>
+      </c>
+      <c r="CL15" s="18">
+        <v>0</v>
+      </c>
+      <c r="CM15" s="18">
+        <v>0</v>
+      </c>
+      <c r="CN15" s="18">
+        <v>0</v>
+      </c>
+      <c r="CO15" s="18">
+        <v>0</v>
+      </c>
+      <c r="CP15" s="18">
+        <v>0</v>
+      </c>
+      <c r="CQ15" s="18">
+        <v>0</v>
+      </c>
       <c r="CR15" s="17"/>
-      <c r="CS15" s="18"/>
-      <c r="CT15" s="18"/>
-      <c r="CU15" s="18"/>
+      <c r="CS15" s="18">
+        <v>280</v>
+      </c>
+      <c r="CT15" s="18">
+        <v>9900</v>
+      </c>
+      <c r="CU15" s="18">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A16" s="19"/>
@@ -3782,12 +5417,12 @@
       <c r="Q16" s="18"/>
       <c r="R16" s="18"/>
       <c r="S16" s="18"/>
-      <c r="T16" s="18"/>
+      <c r="T16" s="41"/>
       <c r="U16" s="18"/>
       <c r="V16" s="18"/>
       <c r="W16" s="18"/>
       <c r="X16" s="18"/>
-      <c r="Y16" s="18"/>
+      <c r="Y16" s="12"/>
       <c r="Z16" s="17"/>
       <c r="AA16" s="18"/>
       <c r="AB16" s="18"/>
@@ -3817,39 +5452,39 @@
       <c r="AZ16" s="18"/>
       <c r="BA16" s="18"/>
       <c r="BB16" s="18"/>
-      <c r="BC16" s="18"/>
+      <c r="BC16" s="40"/>
       <c r="BD16" s="17"/>
-      <c r="BE16" s="18"/>
-      <c r="BF16" s="18"/>
-      <c r="BG16" s="18"/>
-      <c r="BH16" s="18"/>
-      <c r="BI16" s="18"/>
-      <c r="BJ16" s="18"/>
-      <c r="BK16" s="18"/>
-      <c r="BL16" s="18"/>
-      <c r="BM16" s="18"/>
-      <c r="BN16" s="18"/>
-      <c r="BO16" s="18"/>
-      <c r="BP16" s="18"/>
-      <c r="BQ16" s="18"/>
+      <c r="BE16" s="12"/>
+      <c r="BF16" s="12"/>
+      <c r="BG16" s="12"/>
+      <c r="BH16" s="12"/>
+      <c r="BI16" s="12"/>
+      <c r="BJ16" s="12"/>
+      <c r="BK16" s="12"/>
+      <c r="BL16" s="12"/>
+      <c r="BM16" s="12"/>
+      <c r="BN16" s="12"/>
+      <c r="BO16" s="12"/>
+      <c r="BP16" s="12"/>
+      <c r="BQ16" s="12"/>
       <c r="BR16" s="17"/>
-      <c r="BS16" s="18"/>
-      <c r="BT16" s="18"/>
-      <c r="BU16" s="18"/>
-      <c r="BV16" s="18"/>
-      <c r="BW16" s="18"/>
-      <c r="BX16" s="18"/>
+      <c r="BS16" s="12"/>
+      <c r="BT16" s="12"/>
+      <c r="BU16" s="12"/>
+      <c r="BV16" s="12"/>
+      <c r="BW16" s="12"/>
+      <c r="BX16" s="12"/>
       <c r="BY16" s="17"/>
-      <c r="BZ16" s="18"/>
-      <c r="CA16" s="18"/>
-      <c r="CB16" s="18"/>
-      <c r="CC16" s="18"/>
-      <c r="CD16" s="18"/>
-      <c r="CE16" s="18"/>
-      <c r="CF16" s="18"/>
-      <c r="CG16" s="18"/>
-      <c r="CH16" s="18"/>
-      <c r="CI16" s="18"/>
+      <c r="BZ16" s="12"/>
+      <c r="CA16" s="12"/>
+      <c r="CB16" s="12"/>
+      <c r="CC16" s="12"/>
+      <c r="CD16" s="12"/>
+      <c r="CE16" s="12"/>
+      <c r="CF16" s="12"/>
+      <c r="CG16" s="12"/>
+      <c r="CH16" s="12"/>
+      <c r="CI16" s="12"/>
       <c r="CJ16" s="17"/>
       <c r="CK16" s="18"/>
       <c r="CL16" s="18"/>
@@ -3883,12 +5518,12 @@
       <c r="Q17" s="18"/>
       <c r="R17" s="18"/>
       <c r="S17" s="18"/>
-      <c r="T17" s="18"/>
+      <c r="T17" s="41"/>
       <c r="U17" s="18"/>
       <c r="V17" s="18"/>
       <c r="W17" s="18"/>
       <c r="X17" s="18"/>
-      <c r="Y17" s="18"/>
+      <c r="Y17" s="12"/>
       <c r="Z17" s="17"/>
       <c r="AA17" s="18"/>
       <c r="AB17" s="18"/>
@@ -3918,39 +5553,39 @@
       <c r="AZ17" s="18"/>
       <c r="BA17" s="18"/>
       <c r="BB17" s="18"/>
-      <c r="BC17" s="18"/>
+      <c r="BC17" s="40"/>
       <c r="BD17" s="17"/>
-      <c r="BE17" s="18"/>
-      <c r="BF17" s="18"/>
-      <c r="BG17" s="18"/>
-      <c r="BH17" s="18"/>
-      <c r="BI17" s="18"/>
-      <c r="BJ17" s="18"/>
-      <c r="BK17" s="18"/>
-      <c r="BL17" s="18"/>
-      <c r="BM17" s="18"/>
-      <c r="BN17" s="18"/>
-      <c r="BO17" s="18"/>
-      <c r="BP17" s="18"/>
-      <c r="BQ17" s="18"/>
+      <c r="BE17" s="12"/>
+      <c r="BF17" s="12"/>
+      <c r="BG17" s="12"/>
+      <c r="BH17" s="12"/>
+      <c r="BI17" s="12"/>
+      <c r="BJ17" s="12"/>
+      <c r="BK17" s="12"/>
+      <c r="BL17" s="12"/>
+      <c r="BM17" s="12"/>
+      <c r="BN17" s="12"/>
+      <c r="BO17" s="12"/>
+      <c r="BP17" s="12"/>
+      <c r="BQ17" s="12"/>
       <c r="BR17" s="17"/>
-      <c r="BS17" s="18"/>
-      <c r="BT17" s="18"/>
-      <c r="BU17" s="18"/>
-      <c r="BV17" s="18"/>
-      <c r="BW17" s="18"/>
-      <c r="BX17" s="18"/>
+      <c r="BS17" s="12"/>
+      <c r="BT17" s="12"/>
+      <c r="BU17" s="12"/>
+      <c r="BV17" s="12"/>
+      <c r="BW17" s="12"/>
+      <c r="BX17" s="12"/>
       <c r="BY17" s="17"/>
-      <c r="BZ17" s="18"/>
-      <c r="CA17" s="18"/>
-      <c r="CB17" s="18"/>
-      <c r="CC17" s="18"/>
-      <c r="CD17" s="18"/>
-      <c r="CE17" s="18"/>
-      <c r="CF17" s="18"/>
-      <c r="CG17" s="18"/>
-      <c r="CH17" s="18"/>
-      <c r="CI17" s="18"/>
+      <c r="BZ17" s="12"/>
+      <c r="CA17" s="12"/>
+      <c r="CB17" s="12"/>
+      <c r="CC17" s="12"/>
+      <c r="CD17" s="12"/>
+      <c r="CE17" s="12"/>
+      <c r="CF17" s="12"/>
+      <c r="CG17" s="12"/>
+      <c r="CH17" s="12"/>
+      <c r="CI17" s="12"/>
       <c r="CJ17" s="17"/>
       <c r="CK17" s="18"/>
       <c r="CL17" s="18"/>
@@ -3965,7 +5600,6 @@
       <c r="CU17" s="18"/>
     </row>
     <row r="18" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A18" s="19"/>
       <c r="B18" s="1"/>
       <c r="C18" s="8"/>
       <c r="D18" s="17"/>
@@ -3984,12 +5618,12 @@
       <c r="Q18" s="18"/>
       <c r="R18" s="18"/>
       <c r="S18" s="18"/>
-      <c r="T18" s="18"/>
+      <c r="T18" s="41"/>
       <c r="U18" s="18"/>
       <c r="V18" s="18"/>
       <c r="W18" s="18"/>
       <c r="X18" s="18"/>
-      <c r="Y18" s="18"/>
+      <c r="Y18" s="12"/>
       <c r="Z18" s="17"/>
       <c r="AA18" s="18"/>
       <c r="AB18" s="18"/>
@@ -4019,39 +5653,39 @@
       <c r="AZ18" s="18"/>
       <c r="BA18" s="18"/>
       <c r="BB18" s="18"/>
-      <c r="BC18" s="18"/>
+      <c r="BC18" s="40"/>
       <c r="BD18" s="17"/>
-      <c r="BE18" s="18"/>
-      <c r="BF18" s="18"/>
-      <c r="BG18" s="18"/>
-      <c r="BH18" s="18"/>
-      <c r="BI18" s="18"/>
-      <c r="BJ18" s="18"/>
-      <c r="BK18" s="18"/>
-      <c r="BL18" s="18"/>
-      <c r="BM18" s="18"/>
-      <c r="BN18" s="18"/>
-      <c r="BO18" s="18"/>
-      <c r="BP18" s="18"/>
-      <c r="BQ18" s="18"/>
+      <c r="BE18" s="12"/>
+      <c r="BF18" s="12"/>
+      <c r="BG18" s="12"/>
+      <c r="BH18" s="12"/>
+      <c r="BI18" s="12"/>
+      <c r="BJ18" s="12"/>
+      <c r="BK18" s="12"/>
+      <c r="BL18" s="12"/>
+      <c r="BM18" s="12"/>
+      <c r="BN18" s="12"/>
+      <c r="BO18" s="12"/>
+      <c r="BP18" s="12"/>
+      <c r="BQ18" s="12"/>
       <c r="BR18" s="17"/>
-      <c r="BS18" s="18"/>
-      <c r="BT18" s="18"/>
-      <c r="BU18" s="18"/>
-      <c r="BV18" s="18"/>
-      <c r="BW18" s="18"/>
-      <c r="BX18" s="18"/>
+      <c r="BS18" s="12"/>
+      <c r="BT18" s="12"/>
+      <c r="BU18" s="12"/>
+      <c r="BV18" s="12"/>
+      <c r="BW18" s="12"/>
+      <c r="BX18" s="12"/>
       <c r="BY18" s="17"/>
-      <c r="BZ18" s="18"/>
-      <c r="CA18" s="18"/>
-      <c r="CB18" s="18"/>
-      <c r="CC18" s="18"/>
-      <c r="CD18" s="18"/>
-      <c r="CE18" s="18"/>
-      <c r="CF18" s="18"/>
-      <c r="CG18" s="18"/>
-      <c r="CH18" s="18"/>
-      <c r="CI18" s="18"/>
+      <c r="BZ18" s="12"/>
+      <c r="CA18" s="12"/>
+      <c r="CB18" s="12"/>
+      <c r="CC18" s="12"/>
+      <c r="CD18" s="12"/>
+      <c r="CE18" s="12"/>
+      <c r="CF18" s="12"/>
+      <c r="CG18" s="12"/>
+      <c r="CH18" s="12"/>
+      <c r="CI18" s="12"/>
       <c r="CJ18" s="17"/>
       <c r="CK18" s="18"/>
       <c r="CL18" s="18"/>

</xml_diff>

<commit_message>
Trying to get Michigan points to work autoX
Journey's attempt
</commit_message>
<xml_diff>
--- a/Functions/SetupSheets.xlsx
+++ b/Functions/SetupSheets.xlsx
@@ -1419,7 +1419,7 @@
       <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D6" sqref="D6:D15"/>
+      <selection pane="bottomRight" activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2582,7 +2582,7 @@
     </row>
     <row r="6" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A6" s="19">
-        <v>0.41</v>
+        <v>0.47</v>
       </c>
       <c r="B6" s="1">
         <v>35065</v>
@@ -2633,8 +2633,7 @@
         <v>0</v>
       </c>
       <c r="R6" s="18">
-        <f>E6*(1-A6)</f>
-        <v>37.17</v>
+        <v>33.39</v>
       </c>
       <c r="S6" s="18">
         <v>0</v>
@@ -2867,2538 +2866,910 @@
       </c>
     </row>
     <row r="7" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A7" s="23">
-        <v>0.42</v>
-      </c>
       <c r="B7" s="1"/>
       <c r="C7" s="8"/>
-      <c r="D7" s="17">
-        <v>0</v>
-      </c>
-      <c r="E7" s="18">
-        <v>63</v>
-      </c>
-      <c r="F7" s="18">
-        <v>47</v>
-      </c>
-      <c r="G7" s="18">
-        <v>46</v>
-      </c>
-      <c r="H7" s="18">
-        <v>0</v>
-      </c>
-      <c r="I7" s="18">
-        <v>0</v>
-      </c>
-      <c r="J7" s="18">
-        <v>0</v>
-      </c>
-      <c r="K7" s="18">
-        <v>0</v>
-      </c>
-      <c r="L7" s="18">
-        <v>0</v>
-      </c>
-      <c r="M7" s="18">
-        <v>0</v>
-      </c>
-      <c r="N7" s="18">
-        <v>0</v>
-      </c>
-      <c r="O7" s="18">
-        <v>0</v>
-      </c>
-      <c r="P7" s="18">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="18">
-        <v>0</v>
-      </c>
-      <c r="R7" s="18">
-        <f t="shared" ref="R7:R8" si="3">E7*(1-A7)</f>
-        <v>36.540000000000006</v>
-      </c>
-      <c r="S7" s="18">
-        <v>0</v>
-      </c>
-      <c r="T7" s="41">
-        <v>12</v>
-      </c>
-      <c r="U7" s="18">
-        <v>175</v>
-      </c>
-      <c r="V7" s="18">
-        <v>33.9</v>
-      </c>
-      <c r="W7" s="18">
-        <v>0</v>
-      </c>
-      <c r="X7" s="18">
-        <v>12</v>
-      </c>
-      <c r="Y7" s="12">
-        <v>404</v>
-      </c>
+      <c r="D7" s="17"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="18"/>
+      <c r="R7" s="18"/>
+      <c r="S7" s="18"/>
+      <c r="T7" s="41"/>
+      <c r="U7" s="18"/>
+      <c r="V7" s="18"/>
+      <c r="W7" s="18"/>
+      <c r="X7" s="18"/>
+      <c r="Y7" s="12"/>
       <c r="Z7" s="17"/>
-      <c r="AA7" s="18">
-        <v>175</v>
-      </c>
-      <c r="AB7" s="18">
-        <v>200</v>
-      </c>
-      <c r="AC7" s="18">
-        <v>0</v>
-      </c>
-      <c r="AD7" s="18">
-        <v>0</v>
-      </c>
-      <c r="AE7" s="18">
-        <v>0</v>
-      </c>
-      <c r="AF7" s="18">
-        <v>0</v>
-      </c>
-      <c r="AG7" s="18">
-        <v>0</v>
-      </c>
-      <c r="AH7" s="18">
-        <v>0</v>
-      </c>
-      <c r="AI7" s="18">
-        <v>10.25</v>
-      </c>
-      <c r="AJ7" s="18">
-        <v>10.25</v>
-      </c>
-      <c r="AK7" s="18">
-        <v>-0.25</v>
-      </c>
-      <c r="AL7" s="18">
-        <v>1.9</v>
-      </c>
-      <c r="AM7" s="18">
-        <v>0</v>
-      </c>
-      <c r="AN7" s="18">
-        <v>0</v>
-      </c>
-      <c r="AO7" s="18">
-        <v>0</v>
-      </c>
-      <c r="AP7" s="18">
-        <v>0</v>
-      </c>
-      <c r="AQ7" s="18">
-        <v>0</v>
-      </c>
-      <c r="AR7" s="18">
-        <v>0</v>
-      </c>
-      <c r="AS7" s="18">
-        <v>0</v>
-      </c>
-      <c r="AT7" s="18">
-        <v>0</v>
-      </c>
-      <c r="AU7" s="18">
-        <v>10</v>
-      </c>
-      <c r="AV7" s="18">
-        <v>30</v>
-      </c>
+      <c r="AA7" s="18"/>
+      <c r="AB7" s="18"/>
+      <c r="AC7" s="18"/>
+      <c r="AD7" s="18"/>
+      <c r="AE7" s="18"/>
+      <c r="AF7" s="18"/>
+      <c r="AG7" s="18"/>
+      <c r="AH7" s="18"/>
+      <c r="AI7" s="18"/>
+      <c r="AJ7" s="18"/>
+      <c r="AK7" s="18"/>
+      <c r="AL7" s="18"/>
+      <c r="AM7" s="18"/>
+      <c r="AN7" s="18"/>
+      <c r="AO7" s="18"/>
+      <c r="AP7" s="18"/>
+      <c r="AQ7" s="18"/>
+      <c r="AR7" s="18"/>
+      <c r="AS7" s="18"/>
+      <c r="AT7" s="18"/>
+      <c r="AU7" s="18"/>
+      <c r="AV7" s="18"/>
       <c r="AW7" s="17"/>
-      <c r="AX7" s="18">
-        <v>900</v>
-      </c>
-      <c r="AY7" s="18">
-        <v>10.5</v>
-      </c>
-      <c r="AZ7" s="18">
-        <v>0.03</v>
-      </c>
-      <c r="BA7" s="18">
-        <v>120.628</v>
-      </c>
-      <c r="BB7" s="18">
-        <v>70.396699999999996</v>
-      </c>
-      <c r="BC7" s="18">
-        <v>0</v>
-      </c>
+      <c r="AX7" s="18"/>
+      <c r="AY7" s="18"/>
+      <c r="AZ7" s="18"/>
+      <c r="BA7" s="18"/>
+      <c r="BB7" s="18"/>
+      <c r="BC7" s="18"/>
       <c r="BD7" s="17"/>
-      <c r="BE7" s="12">
-        <v>1</v>
-      </c>
-      <c r="BF7" s="12">
-        <v>2.5</v>
-      </c>
-      <c r="BG7" s="12">
-        <v>2</v>
-      </c>
-      <c r="BH7" s="12">
-        <v>1.62</v>
-      </c>
-      <c r="BI7" s="12">
-        <v>1.333</v>
-      </c>
-      <c r="BJ7" s="12">
-        <v>1.095</v>
-      </c>
-      <c r="BK7" s="12">
-        <v>2.6520000000000001</v>
-      </c>
-      <c r="BL7" s="12">
-        <v>2.714</v>
-      </c>
-      <c r="BM7" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="BN7" s="12">
-        <v>0</v>
-      </c>
-      <c r="BO7" s="12">
-        <v>0</v>
-      </c>
-      <c r="BP7" s="12">
-        <v>0</v>
-      </c>
-      <c r="BQ7" s="12">
-        <v>20</v>
-      </c>
+      <c r="BE7" s="12"/>
+      <c r="BF7" s="12"/>
+      <c r="BG7" s="12"/>
+      <c r="BH7" s="12"/>
+      <c r="BI7" s="12"/>
+      <c r="BJ7" s="12"/>
+      <c r="BK7" s="12"/>
+      <c r="BL7" s="12"/>
+      <c r="BM7" s="12"/>
+      <c r="BN7" s="12"/>
+      <c r="BO7" s="12"/>
+      <c r="BP7" s="12"/>
+      <c r="BQ7" s="12"/>
       <c r="BR7" s="17"/>
-      <c r="BS7" s="12">
-        <v>6762.75</v>
-      </c>
-      <c r="BT7" s="12">
-        <v>3238.5</v>
-      </c>
-      <c r="BU7" s="12">
-        <v>0</v>
-      </c>
-      <c r="BV7" s="12">
-        <v>0</v>
-      </c>
-      <c r="BW7" s="12">
-        <v>0</v>
-      </c>
-      <c r="BX7" s="12">
-        <v>0.96699999999999997</v>
-      </c>
+      <c r="BS7" s="12"/>
+      <c r="BT7" s="12"/>
+      <c r="BU7" s="12"/>
+      <c r="BV7" s="12"/>
+      <c r="BW7" s="12"/>
+      <c r="BX7" s="12"/>
       <c r="BY7" s="17"/>
-      <c r="BZ7" s="12">
-        <v>0</v>
-      </c>
-      <c r="CA7" s="12">
-        <v>0</v>
-      </c>
-      <c r="CB7" s="12">
-        <v>0</v>
-      </c>
-      <c r="CC7" s="12">
-        <v>0.45</v>
-      </c>
-      <c r="CD7" s="12">
-        <v>-0.89</v>
-      </c>
-      <c r="CE7" s="12">
-        <v>2015</v>
-      </c>
-      <c r="CF7" s="12">
-        <v>2.3289999999999999E-3</v>
-      </c>
-      <c r="CG7" s="12">
-        <v>34.25</v>
-      </c>
-      <c r="CH7" s="12">
-        <v>0</v>
-      </c>
-      <c r="CI7" s="12">
-        <v>10</v>
-      </c>
+      <c r="BZ7" s="12"/>
+      <c r="CA7" s="12"/>
+      <c r="CB7" s="12"/>
+      <c r="CC7" s="12"/>
+      <c r="CD7" s="12"/>
+      <c r="CE7" s="12"/>
+      <c r="CF7" s="12"/>
+      <c r="CG7" s="12"/>
+      <c r="CH7" s="12"/>
+      <c r="CI7" s="12"/>
       <c r="CJ7" s="17"/>
-      <c r="CK7" s="18">
-        <v>0.7</v>
-      </c>
-      <c r="CL7" s="18">
-        <v>0</v>
-      </c>
-      <c r="CM7" s="18">
-        <v>0</v>
-      </c>
-      <c r="CN7" s="18">
-        <v>0</v>
-      </c>
-      <c r="CO7" s="18">
-        <v>0</v>
-      </c>
-      <c r="CP7" s="18">
-        <v>0</v>
-      </c>
-      <c r="CQ7" s="18">
-        <v>0</v>
-      </c>
+      <c r="CK7" s="18"/>
+      <c r="CL7" s="18"/>
+      <c r="CM7" s="18"/>
+      <c r="CN7" s="18"/>
+      <c r="CO7" s="18"/>
+      <c r="CP7" s="18"/>
+      <c r="CQ7" s="18"/>
       <c r="CR7" s="17"/>
-      <c r="CS7" s="18">
-        <v>280</v>
-      </c>
-      <c r="CT7" s="18">
-        <v>9900</v>
-      </c>
-      <c r="CU7" s="18">
-        <v>0</v>
-      </c>
+      <c r="CS7" s="18"/>
+      <c r="CT7" s="18"/>
+      <c r="CU7" s="18"/>
     </row>
     <row r="8" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A8" s="19">
-        <v>0.43</v>
-      </c>
+      <c r="A8" s="19"/>
       <c r="B8" s="1"/>
       <c r="C8" s="8"/>
-      <c r="D8" s="17">
-        <v>0</v>
-      </c>
-      <c r="E8" s="18">
-        <v>63</v>
-      </c>
-      <c r="F8" s="18">
-        <v>47</v>
-      </c>
-      <c r="G8" s="18">
-        <v>46</v>
-      </c>
-      <c r="H8" s="18">
-        <v>0</v>
-      </c>
-      <c r="I8" s="18">
-        <v>0</v>
-      </c>
-      <c r="J8" s="18">
-        <v>0</v>
-      </c>
-      <c r="K8" s="18">
-        <v>0</v>
-      </c>
-      <c r="L8" s="18">
-        <v>0</v>
-      </c>
-      <c r="M8" s="18">
-        <v>0</v>
-      </c>
-      <c r="N8" s="18">
-        <v>0</v>
-      </c>
-      <c r="O8" s="18">
-        <v>0</v>
-      </c>
-      <c r="P8" s="18">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="18">
-        <v>0</v>
-      </c>
-      <c r="R8" s="18">
-        <f t="shared" si="3"/>
-        <v>35.910000000000004</v>
-      </c>
-      <c r="S8" s="18">
-        <v>0</v>
-      </c>
-      <c r="T8" s="41">
-        <v>12</v>
-      </c>
-      <c r="U8" s="18">
-        <v>175</v>
-      </c>
-      <c r="V8" s="18">
-        <v>33.9</v>
-      </c>
-      <c r="W8" s="18">
-        <v>0</v>
-      </c>
-      <c r="X8" s="18">
-        <v>12</v>
-      </c>
-      <c r="Y8" s="12">
-        <v>404</v>
-      </c>
+      <c r="D8" s="17"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="18"/>
+      <c r="R8" s="18"/>
+      <c r="S8" s="18"/>
+      <c r="T8" s="41"/>
+      <c r="U8" s="18"/>
+      <c r="V8" s="18"/>
+      <c r="W8" s="18"/>
+      <c r="X8" s="18"/>
+      <c r="Y8" s="12"/>
       <c r="Z8" s="17"/>
-      <c r="AA8" s="18">
-        <v>175</v>
-      </c>
-      <c r="AB8" s="18">
-        <v>200</v>
-      </c>
-      <c r="AC8" s="18">
-        <v>0</v>
-      </c>
-      <c r="AD8" s="18">
-        <v>0</v>
-      </c>
-      <c r="AE8" s="18">
-        <v>0</v>
-      </c>
-      <c r="AF8" s="18">
-        <v>0</v>
-      </c>
-      <c r="AG8" s="18">
-        <v>0</v>
-      </c>
-      <c r="AH8" s="18">
-        <v>0</v>
-      </c>
-      <c r="AI8" s="18">
-        <v>10.25</v>
-      </c>
-      <c r="AJ8" s="18">
-        <v>10.25</v>
-      </c>
-      <c r="AK8" s="18">
-        <v>-0.25</v>
-      </c>
-      <c r="AL8" s="18">
-        <v>1.9</v>
-      </c>
-      <c r="AM8" s="18">
-        <v>0</v>
-      </c>
-      <c r="AN8" s="18">
-        <v>0</v>
-      </c>
-      <c r="AO8" s="18">
-        <v>0</v>
-      </c>
-      <c r="AP8" s="18">
-        <v>0</v>
-      </c>
-      <c r="AQ8" s="18">
-        <v>0</v>
-      </c>
-      <c r="AR8" s="18">
-        <v>0</v>
-      </c>
-      <c r="AS8" s="18">
-        <v>0</v>
-      </c>
-      <c r="AT8" s="18">
-        <v>0</v>
-      </c>
-      <c r="AU8" s="18">
-        <v>10</v>
-      </c>
-      <c r="AV8" s="18">
-        <v>30</v>
-      </c>
+      <c r="AA8" s="18"/>
+      <c r="AB8" s="18"/>
+      <c r="AC8" s="18"/>
+      <c r="AD8" s="18"/>
+      <c r="AE8" s="18"/>
+      <c r="AF8" s="18"/>
+      <c r="AG8" s="18"/>
+      <c r="AH8" s="18"/>
+      <c r="AI8" s="18"/>
+      <c r="AJ8" s="18"/>
+      <c r="AK8" s="18"/>
+      <c r="AL8" s="18"/>
+      <c r="AM8" s="18"/>
+      <c r="AN8" s="18"/>
+      <c r="AO8" s="18"/>
+      <c r="AP8" s="18"/>
+      <c r="AQ8" s="18"/>
+      <c r="AR8" s="18"/>
+      <c r="AS8" s="18"/>
+      <c r="AT8" s="18"/>
+      <c r="AU8" s="18"/>
+      <c r="AV8" s="18"/>
       <c r="AW8" s="17"/>
-      <c r="AX8" s="18">
-        <v>900</v>
-      </c>
-      <c r="AY8" s="18">
-        <v>10.5</v>
-      </c>
-      <c r="AZ8" s="18">
-        <v>0.03</v>
-      </c>
-      <c r="BA8" s="18">
-        <v>120.628</v>
-      </c>
-      <c r="BB8" s="18">
-        <v>70.396699999999996</v>
-      </c>
-      <c r="BC8" s="18">
-        <v>0</v>
-      </c>
+      <c r="AX8" s="18"/>
+      <c r="AY8" s="18"/>
+      <c r="AZ8" s="18"/>
+      <c r="BA8" s="18"/>
+      <c r="BB8" s="18"/>
+      <c r="BC8" s="18"/>
       <c r="BD8" s="17"/>
-      <c r="BE8" s="12">
-        <v>1</v>
-      </c>
-      <c r="BF8" s="12">
-        <v>2.5</v>
-      </c>
-      <c r="BG8" s="12">
-        <v>2</v>
-      </c>
-      <c r="BH8" s="12">
-        <v>1.62</v>
-      </c>
-      <c r="BI8" s="12">
-        <v>1.333</v>
-      </c>
-      <c r="BJ8" s="12">
-        <v>1.095</v>
-      </c>
-      <c r="BK8" s="12">
-        <v>2.6520000000000001</v>
-      </c>
-      <c r="BL8" s="12">
-        <v>2.714</v>
-      </c>
-      <c r="BM8" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="BN8" s="12">
-        <v>0</v>
-      </c>
-      <c r="BO8" s="12">
-        <v>0</v>
-      </c>
-      <c r="BP8" s="12">
-        <v>0</v>
-      </c>
-      <c r="BQ8" s="12">
-        <v>20</v>
-      </c>
+      <c r="BE8" s="12"/>
+      <c r="BF8" s="12"/>
+      <c r="BG8" s="12"/>
+      <c r="BH8" s="12"/>
+      <c r="BI8" s="12"/>
+      <c r="BJ8" s="12"/>
+      <c r="BK8" s="12"/>
+      <c r="BL8" s="12"/>
+      <c r="BM8" s="12"/>
+      <c r="BN8" s="12"/>
+      <c r="BO8" s="12"/>
+      <c r="BP8" s="12"/>
+      <c r="BQ8" s="12"/>
       <c r="BR8" s="17"/>
-      <c r="BS8" s="12">
-        <v>6762.75</v>
-      </c>
-      <c r="BT8" s="12">
-        <v>3238.5</v>
-      </c>
-      <c r="BU8" s="12">
-        <v>0</v>
-      </c>
-      <c r="BV8" s="12">
-        <v>0</v>
-      </c>
-      <c r="BW8" s="12">
-        <v>0</v>
-      </c>
-      <c r="BX8" s="12">
-        <v>0.96699999999999997</v>
-      </c>
+      <c r="BS8" s="12"/>
+      <c r="BT8" s="12"/>
+      <c r="BU8" s="12"/>
+      <c r="BV8" s="12"/>
+      <c r="BW8" s="12"/>
+      <c r="BX8" s="12"/>
       <c r="BY8" s="17"/>
-      <c r="BZ8" s="12">
-        <v>0</v>
-      </c>
-      <c r="CA8" s="12">
-        <v>0</v>
-      </c>
-      <c r="CB8" s="12">
-        <v>0</v>
-      </c>
-      <c r="CC8" s="12">
-        <v>0.45</v>
-      </c>
-      <c r="CD8" s="12">
-        <v>-0.89</v>
-      </c>
-      <c r="CE8" s="12">
-        <v>2015</v>
-      </c>
-      <c r="CF8" s="12">
-        <v>2.3289999999999999E-3</v>
-      </c>
-      <c r="CG8" s="12">
-        <v>34.25</v>
-      </c>
-      <c r="CH8" s="12">
-        <v>0</v>
-      </c>
-      <c r="CI8" s="12">
-        <v>10</v>
-      </c>
+      <c r="BZ8" s="12"/>
+      <c r="CA8" s="12"/>
+      <c r="CB8" s="12"/>
+      <c r="CC8" s="12"/>
+      <c r="CD8" s="12"/>
+      <c r="CE8" s="12"/>
+      <c r="CF8" s="12"/>
+      <c r="CG8" s="12"/>
+      <c r="CH8" s="12"/>
+      <c r="CI8" s="12"/>
       <c r="CJ8" s="17"/>
-      <c r="CK8" s="18">
-        <v>0.7</v>
-      </c>
-      <c r="CL8" s="18">
-        <v>0</v>
-      </c>
-      <c r="CM8" s="18">
-        <v>0</v>
-      </c>
-      <c r="CN8" s="18">
-        <v>0</v>
-      </c>
-      <c r="CO8" s="18">
-        <v>0</v>
-      </c>
-      <c r="CP8" s="18">
-        <v>0</v>
-      </c>
-      <c r="CQ8" s="18">
-        <v>0</v>
-      </c>
+      <c r="CK8" s="18"/>
+      <c r="CL8" s="18"/>
+      <c r="CM8" s="18"/>
+      <c r="CN8" s="18"/>
+      <c r="CO8" s="18"/>
+      <c r="CP8" s="18"/>
+      <c r="CQ8" s="18"/>
       <c r="CR8" s="17"/>
-      <c r="CS8" s="18">
-        <v>280</v>
-      </c>
-      <c r="CT8" s="18">
-        <v>9900</v>
-      </c>
-      <c r="CU8" s="18">
-        <v>0</v>
-      </c>
+      <c r="CS8" s="18"/>
+      <c r="CT8" s="18"/>
+      <c r="CU8" s="18"/>
     </row>
     <row r="9" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A9" s="19">
-        <v>0.44</v>
-      </c>
       <c r="B9" s="1"/>
       <c r="C9" s="8"/>
-      <c r="D9" s="17">
-        <v>0</v>
-      </c>
-      <c r="E9" s="18">
-        <v>63</v>
-      </c>
-      <c r="F9" s="18">
-        <v>47</v>
-      </c>
-      <c r="G9" s="18">
-        <v>46</v>
-      </c>
-      <c r="H9" s="18">
-        <v>0</v>
-      </c>
-      <c r="I9" s="18">
-        <v>0</v>
-      </c>
-      <c r="J9" s="18">
-        <v>0</v>
-      </c>
-      <c r="K9" s="18">
-        <v>0</v>
-      </c>
-      <c r="L9" s="18">
-        <v>0</v>
-      </c>
-      <c r="M9" s="18">
-        <v>0</v>
-      </c>
-      <c r="N9" s="18">
-        <v>0</v>
-      </c>
-      <c r="O9" s="18">
-        <v>0</v>
-      </c>
-      <c r="P9" s="18">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="18">
-        <v>0</v>
-      </c>
-      <c r="R9" s="18">
-        <v>35.28</v>
-      </c>
-      <c r="S9" s="18">
-        <v>0</v>
-      </c>
-      <c r="T9" s="41">
-        <v>12</v>
-      </c>
-      <c r="U9" s="18">
-        <v>175</v>
-      </c>
-      <c r="V9" s="18">
-        <v>33.9</v>
-      </c>
-      <c r="W9" s="18">
-        <v>0</v>
-      </c>
-      <c r="X9" s="18">
-        <v>12</v>
-      </c>
-      <c r="Y9" s="12">
-        <v>404</v>
-      </c>
+      <c r="D9" s="17"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="18"/>
+      <c r="R9" s="18"/>
+      <c r="S9" s="18"/>
+      <c r="T9" s="41"/>
+      <c r="U9" s="18"/>
+      <c r="V9" s="18"/>
+      <c r="W9" s="18"/>
+      <c r="X9" s="18"/>
+      <c r="Y9" s="12"/>
       <c r="Z9" s="17"/>
-      <c r="AA9" s="18">
-        <v>175</v>
-      </c>
-      <c r="AB9" s="18">
-        <v>200</v>
-      </c>
-      <c r="AC9" s="18">
-        <v>0</v>
-      </c>
-      <c r="AD9" s="18">
-        <v>0</v>
-      </c>
-      <c r="AE9" s="18">
-        <v>0</v>
-      </c>
-      <c r="AF9" s="18">
-        <v>0</v>
-      </c>
-      <c r="AG9" s="18">
-        <v>0</v>
-      </c>
-      <c r="AH9" s="18">
-        <v>0</v>
-      </c>
-      <c r="AI9" s="18">
-        <v>10.25</v>
-      </c>
-      <c r="AJ9" s="18">
-        <v>10.25</v>
-      </c>
-      <c r="AK9" s="18">
-        <v>-0.25</v>
-      </c>
-      <c r="AL9" s="18">
-        <v>1.9</v>
-      </c>
-      <c r="AM9" s="18">
-        <v>0</v>
-      </c>
-      <c r="AN9" s="18">
-        <v>0</v>
-      </c>
-      <c r="AO9" s="18">
-        <v>0</v>
-      </c>
-      <c r="AP9" s="18">
-        <v>0</v>
-      </c>
-      <c r="AQ9" s="18">
-        <v>0</v>
-      </c>
-      <c r="AR9" s="18">
-        <v>0</v>
-      </c>
-      <c r="AS9" s="18">
-        <v>0</v>
-      </c>
-      <c r="AT9" s="18">
-        <v>0</v>
-      </c>
-      <c r="AU9" s="18">
-        <v>10</v>
-      </c>
-      <c r="AV9" s="18">
-        <v>30</v>
-      </c>
+      <c r="AA9" s="18"/>
+      <c r="AB9" s="18"/>
+      <c r="AC9" s="18"/>
+      <c r="AD9" s="18"/>
+      <c r="AE9" s="18"/>
+      <c r="AF9" s="18"/>
+      <c r="AG9" s="18"/>
+      <c r="AH9" s="18"/>
+      <c r="AI9" s="18"/>
+      <c r="AJ9" s="18"/>
+      <c r="AK9" s="18"/>
+      <c r="AL9" s="18"/>
+      <c r="AM9" s="18"/>
+      <c r="AN9" s="18"/>
+      <c r="AO9" s="18"/>
+      <c r="AP9" s="18"/>
+      <c r="AQ9" s="18"/>
+      <c r="AR9" s="18"/>
+      <c r="AS9" s="18"/>
+      <c r="AT9" s="18"/>
+      <c r="AU9" s="18"/>
+      <c r="AV9" s="18"/>
       <c r="AW9" s="17"/>
-      <c r="AX9" s="18">
-        <v>900</v>
-      </c>
-      <c r="AY9" s="18">
-        <v>10.5</v>
-      </c>
-      <c r="AZ9" s="18">
-        <v>0.03</v>
-      </c>
-      <c r="BA9" s="18">
-        <v>120.628</v>
-      </c>
-      <c r="BB9" s="18">
-        <v>70.396699999999996</v>
-      </c>
-      <c r="BC9" s="18">
-        <v>0</v>
-      </c>
+      <c r="AX9" s="18"/>
+      <c r="AY9" s="18"/>
+      <c r="AZ9" s="18"/>
+      <c r="BA9" s="18"/>
+      <c r="BB9" s="18"/>
+      <c r="BC9" s="18"/>
       <c r="BD9" s="17"/>
-      <c r="BE9" s="12">
-        <v>1</v>
-      </c>
-      <c r="BF9" s="12">
-        <v>2.5</v>
-      </c>
-      <c r="BG9" s="12">
-        <v>2</v>
-      </c>
-      <c r="BH9" s="12">
-        <v>1.62</v>
-      </c>
-      <c r="BI9" s="12">
-        <v>1.333</v>
-      </c>
-      <c r="BJ9" s="12">
-        <v>1.095</v>
-      </c>
-      <c r="BK9" s="12">
-        <v>2.6520000000000001</v>
-      </c>
-      <c r="BL9" s="12">
-        <v>2.714</v>
-      </c>
-      <c r="BM9" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="BN9" s="12">
-        <v>0</v>
-      </c>
-      <c r="BO9" s="12">
-        <v>0</v>
-      </c>
-      <c r="BP9" s="12">
-        <v>0</v>
-      </c>
-      <c r="BQ9" s="12">
-        <v>20</v>
-      </c>
+      <c r="BE9" s="12"/>
+      <c r="BF9" s="12"/>
+      <c r="BG9" s="12"/>
+      <c r="BH9" s="12"/>
+      <c r="BI9" s="12"/>
+      <c r="BJ9" s="12"/>
+      <c r="BK9" s="12"/>
+      <c r="BL9" s="12"/>
+      <c r="BM9" s="12"/>
+      <c r="BN9" s="12"/>
+      <c r="BO9" s="12"/>
+      <c r="BP9" s="12"/>
+      <c r="BQ9" s="12"/>
       <c r="BR9" s="17"/>
-      <c r="BS9" s="12">
-        <v>6762.75</v>
-      </c>
-      <c r="BT9" s="12">
-        <v>3238.5</v>
-      </c>
-      <c r="BU9" s="12">
-        <v>0</v>
-      </c>
-      <c r="BV9" s="12">
-        <v>0</v>
-      </c>
-      <c r="BW9" s="12">
-        <v>0</v>
-      </c>
-      <c r="BX9" s="12">
-        <v>0.96699999999999997</v>
-      </c>
+      <c r="BS9" s="12"/>
+      <c r="BT9" s="12"/>
+      <c r="BU9" s="12"/>
+      <c r="BV9" s="12"/>
+      <c r="BW9" s="12"/>
+      <c r="BX9" s="12"/>
       <c r="BY9" s="17"/>
-      <c r="BZ9" s="12">
-        <v>0</v>
-      </c>
-      <c r="CA9" s="12">
-        <v>0</v>
-      </c>
-      <c r="CB9" s="12">
-        <v>0</v>
-      </c>
-      <c r="CC9" s="12">
-        <v>0.45</v>
-      </c>
-      <c r="CD9" s="12">
-        <v>-0.89</v>
-      </c>
-      <c r="CE9" s="12">
-        <v>2015</v>
-      </c>
-      <c r="CF9" s="12">
-        <v>2.3289999999999999E-3</v>
-      </c>
-      <c r="CG9" s="12">
-        <v>34.25</v>
-      </c>
-      <c r="CH9" s="12">
-        <v>0</v>
-      </c>
-      <c r="CI9" s="12">
-        <v>10</v>
-      </c>
+      <c r="BZ9" s="12"/>
+      <c r="CA9" s="12"/>
+      <c r="CB9" s="12"/>
+      <c r="CC9" s="12"/>
+      <c r="CD9" s="12"/>
+      <c r="CE9" s="12"/>
+      <c r="CF9" s="12"/>
+      <c r="CG9" s="12"/>
+      <c r="CH9" s="12"/>
+      <c r="CI9" s="12"/>
       <c r="CJ9" s="17"/>
-      <c r="CK9" s="18">
-        <v>0.7</v>
-      </c>
-      <c r="CL9" s="18">
-        <v>0</v>
-      </c>
-      <c r="CM9" s="18">
-        <v>0</v>
-      </c>
-      <c r="CN9" s="18">
-        <v>0</v>
-      </c>
-      <c r="CO9" s="18">
-        <v>0</v>
-      </c>
-      <c r="CP9" s="18">
-        <v>0</v>
-      </c>
-      <c r="CQ9" s="18">
-        <v>0</v>
-      </c>
+      <c r="CK9" s="18"/>
+      <c r="CL9" s="18"/>
+      <c r="CM9" s="18"/>
+      <c r="CN9" s="18"/>
+      <c r="CO9" s="18"/>
+      <c r="CP9" s="18"/>
+      <c r="CQ9" s="18"/>
       <c r="CR9" s="17"/>
-      <c r="CS9" s="18">
-        <v>280</v>
-      </c>
-      <c r="CT9" s="18">
-        <v>9900</v>
-      </c>
-      <c r="CU9" s="18">
-        <v>0</v>
-      </c>
+      <c r="CS9" s="18"/>
+      <c r="CT9" s="18"/>
+      <c r="CU9" s="18"/>
     </row>
     <row r="10" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A10" s="23">
-        <v>0.45</v>
-      </c>
+      <c r="A10" s="19"/>
       <c r="B10" s="1"/>
       <c r="C10" s="8"/>
-      <c r="D10" s="17">
-        <v>0</v>
-      </c>
-      <c r="E10" s="18">
-        <v>63</v>
-      </c>
-      <c r="F10" s="18">
-        <v>47</v>
-      </c>
-      <c r="G10" s="18">
-        <v>46</v>
-      </c>
-      <c r="H10" s="18">
-        <v>0</v>
-      </c>
-      <c r="I10" s="18">
-        <v>0</v>
-      </c>
-      <c r="J10" s="18">
-        <v>0</v>
-      </c>
-      <c r="K10" s="18">
-        <v>0</v>
-      </c>
-      <c r="L10" s="18">
-        <v>0</v>
-      </c>
-      <c r="M10" s="18">
-        <v>0</v>
-      </c>
-      <c r="N10" s="18">
-        <v>0</v>
-      </c>
-      <c r="O10" s="18">
-        <v>0</v>
-      </c>
-      <c r="P10" s="18">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="18">
-        <v>0</v>
-      </c>
-      <c r="R10" s="18">
-        <v>34.650000000000006</v>
-      </c>
-      <c r="S10" s="18">
-        <v>0</v>
-      </c>
-      <c r="T10" s="41">
-        <v>12</v>
-      </c>
-      <c r="U10" s="18">
-        <v>175</v>
-      </c>
-      <c r="V10" s="18">
-        <v>33.9</v>
-      </c>
-      <c r="W10" s="18">
-        <v>0</v>
-      </c>
-      <c r="X10" s="18">
-        <v>12</v>
-      </c>
-      <c r="Y10" s="12">
-        <v>404</v>
-      </c>
+      <c r="D10" s="17"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="18"/>
+      <c r="S10" s="18"/>
+      <c r="T10" s="41"/>
+      <c r="U10" s="18"/>
+      <c r="V10" s="18"/>
+      <c r="W10" s="18"/>
+      <c r="X10" s="18"/>
+      <c r="Y10" s="12"/>
       <c r="Z10" s="17"/>
-      <c r="AA10" s="18">
-        <v>175</v>
-      </c>
-      <c r="AB10" s="18">
-        <v>200</v>
-      </c>
-      <c r="AC10" s="18">
-        <v>0</v>
-      </c>
-      <c r="AD10" s="18">
-        <v>0</v>
-      </c>
-      <c r="AE10" s="18">
-        <v>0</v>
-      </c>
-      <c r="AF10" s="18">
-        <v>0</v>
-      </c>
-      <c r="AG10" s="18">
-        <v>0</v>
-      </c>
-      <c r="AH10" s="18">
-        <v>0</v>
-      </c>
-      <c r="AI10" s="18">
-        <v>10.25</v>
-      </c>
-      <c r="AJ10" s="18">
-        <v>10.25</v>
-      </c>
-      <c r="AK10" s="18">
-        <v>-0.25</v>
-      </c>
-      <c r="AL10" s="18">
-        <v>1.9</v>
-      </c>
-      <c r="AM10" s="18">
-        <v>0</v>
-      </c>
-      <c r="AN10" s="18">
-        <v>0</v>
-      </c>
-      <c r="AO10" s="18">
-        <v>0</v>
-      </c>
-      <c r="AP10" s="18">
-        <v>0</v>
-      </c>
-      <c r="AQ10" s="18">
-        <v>0</v>
-      </c>
-      <c r="AR10" s="18">
-        <v>0</v>
-      </c>
-      <c r="AS10" s="18">
-        <v>0</v>
-      </c>
-      <c r="AT10" s="18">
-        <v>0</v>
-      </c>
-      <c r="AU10" s="18">
-        <v>10</v>
-      </c>
-      <c r="AV10" s="18">
-        <v>30</v>
-      </c>
+      <c r="AA10" s="18"/>
+      <c r="AB10" s="18"/>
+      <c r="AC10" s="18"/>
+      <c r="AD10" s="18"/>
+      <c r="AE10" s="18"/>
+      <c r="AF10" s="18"/>
+      <c r="AG10" s="18"/>
+      <c r="AH10" s="18"/>
+      <c r="AI10" s="18"/>
+      <c r="AJ10" s="18"/>
+      <c r="AK10" s="18"/>
+      <c r="AL10" s="18"/>
+      <c r="AM10" s="18"/>
+      <c r="AN10" s="18"/>
+      <c r="AO10" s="18"/>
+      <c r="AP10" s="18"/>
+      <c r="AQ10" s="18"/>
+      <c r="AR10" s="18"/>
+      <c r="AS10" s="18"/>
+      <c r="AT10" s="18"/>
+      <c r="AU10" s="18"/>
+      <c r="AV10" s="18"/>
       <c r="AW10" s="17"/>
-      <c r="AX10" s="18">
-        <v>900</v>
-      </c>
-      <c r="AY10" s="18">
-        <v>10.5</v>
-      </c>
-      <c r="AZ10" s="18">
-        <v>0.03</v>
-      </c>
-      <c r="BA10" s="18">
-        <v>120.628</v>
-      </c>
-      <c r="BB10" s="18">
-        <v>70.396699999999996</v>
-      </c>
-      <c r="BC10" s="18">
-        <v>0</v>
-      </c>
+      <c r="AX10" s="18"/>
+      <c r="AY10" s="18"/>
+      <c r="AZ10" s="18"/>
+      <c r="BA10" s="18"/>
+      <c r="BB10" s="18"/>
+      <c r="BC10" s="18"/>
       <c r="BD10" s="17"/>
-      <c r="BE10" s="12">
-        <v>1</v>
-      </c>
-      <c r="BF10" s="12">
-        <v>2.5</v>
-      </c>
-      <c r="BG10" s="12">
-        <v>2</v>
-      </c>
-      <c r="BH10" s="12">
-        <v>1.62</v>
-      </c>
-      <c r="BI10" s="12">
-        <v>1.333</v>
-      </c>
-      <c r="BJ10" s="12">
-        <v>1.095</v>
-      </c>
-      <c r="BK10" s="12">
-        <v>2.6520000000000001</v>
-      </c>
-      <c r="BL10" s="12">
-        <v>2.714</v>
-      </c>
-      <c r="BM10" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="BN10" s="12">
-        <v>0</v>
-      </c>
-      <c r="BO10" s="12">
-        <v>0</v>
-      </c>
-      <c r="BP10" s="12">
-        <v>0</v>
-      </c>
-      <c r="BQ10" s="12">
-        <v>20</v>
-      </c>
+      <c r="BE10" s="12"/>
+      <c r="BF10" s="12"/>
+      <c r="BG10" s="12"/>
+      <c r="BH10" s="12"/>
+      <c r="BI10" s="12"/>
+      <c r="BJ10" s="12"/>
+      <c r="BK10" s="12"/>
+      <c r="BL10" s="12"/>
+      <c r="BM10" s="12"/>
+      <c r="BN10" s="12"/>
+      <c r="BO10" s="12"/>
+      <c r="BP10" s="12"/>
+      <c r="BQ10" s="12"/>
       <c r="BR10" s="17"/>
-      <c r="BS10" s="12">
-        <v>6762.75</v>
-      </c>
-      <c r="BT10" s="12">
-        <v>3238.5</v>
-      </c>
-      <c r="BU10" s="12">
-        <v>0</v>
-      </c>
-      <c r="BV10" s="12">
-        <v>0</v>
-      </c>
-      <c r="BW10" s="12">
-        <v>0</v>
-      </c>
-      <c r="BX10" s="12">
-        <v>0.96699999999999997</v>
-      </c>
+      <c r="BS10" s="12"/>
+      <c r="BT10" s="12"/>
+      <c r="BU10" s="12"/>
+      <c r="BV10" s="12"/>
+      <c r="BW10" s="12"/>
+      <c r="BX10" s="12"/>
       <c r="BY10" s="17"/>
-      <c r="BZ10" s="12">
-        <v>0</v>
-      </c>
-      <c r="CA10" s="12">
-        <v>0</v>
-      </c>
-      <c r="CB10" s="12">
-        <v>0</v>
-      </c>
-      <c r="CC10" s="12">
-        <v>0.45</v>
-      </c>
-      <c r="CD10" s="12">
-        <v>-0.89</v>
-      </c>
-      <c r="CE10" s="12">
-        <v>2015</v>
-      </c>
-      <c r="CF10" s="12">
-        <v>2.3289999999999999E-3</v>
-      </c>
-      <c r="CG10" s="12">
-        <v>34.25</v>
-      </c>
-      <c r="CH10" s="12">
-        <v>0</v>
-      </c>
-      <c r="CI10" s="12">
-        <v>10</v>
-      </c>
+      <c r="BZ10" s="12"/>
+      <c r="CA10" s="12"/>
+      <c r="CB10" s="12"/>
+      <c r="CC10" s="12"/>
+      <c r="CD10" s="12"/>
+      <c r="CE10" s="12"/>
+      <c r="CF10" s="12"/>
+      <c r="CG10" s="12"/>
+      <c r="CH10" s="12"/>
+      <c r="CI10" s="12"/>
       <c r="CJ10" s="17"/>
-      <c r="CK10" s="18">
-        <v>0.7</v>
-      </c>
-      <c r="CL10" s="18">
-        <v>0</v>
-      </c>
-      <c r="CM10" s="18">
-        <v>0</v>
-      </c>
-      <c r="CN10" s="18">
-        <v>0</v>
-      </c>
-      <c r="CO10" s="18">
-        <v>0</v>
-      </c>
-      <c r="CP10" s="18">
-        <v>0</v>
-      </c>
-      <c r="CQ10" s="18">
-        <v>0</v>
-      </c>
+      <c r="CK10" s="18"/>
+      <c r="CL10" s="18"/>
+      <c r="CM10" s="18"/>
+      <c r="CN10" s="18"/>
+      <c r="CO10" s="18"/>
+      <c r="CP10" s="18"/>
+      <c r="CQ10" s="18"/>
       <c r="CR10" s="17"/>
-      <c r="CS10" s="18">
-        <v>280</v>
-      </c>
-      <c r="CT10" s="18">
-        <v>9900</v>
-      </c>
-      <c r="CU10" s="18">
-        <v>0</v>
-      </c>
+      <c r="CS10" s="18"/>
+      <c r="CT10" s="18"/>
+      <c r="CU10" s="18"/>
     </row>
     <row r="11" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A11" s="19">
-        <v>0.46</v>
-      </c>
       <c r="B11" s="1"/>
       <c r="C11" s="8"/>
-      <c r="D11" s="17">
-        <v>0</v>
-      </c>
-      <c r="E11" s="18">
-        <v>63</v>
-      </c>
-      <c r="F11" s="18">
-        <v>47</v>
-      </c>
-      <c r="G11" s="18">
-        <v>46</v>
-      </c>
-      <c r="H11" s="18">
-        <v>0</v>
-      </c>
-      <c r="I11" s="18">
-        <v>0</v>
-      </c>
-      <c r="J11" s="18">
-        <v>0</v>
-      </c>
-      <c r="K11" s="18">
-        <v>0</v>
-      </c>
-      <c r="L11" s="18">
-        <v>0</v>
-      </c>
-      <c r="M11" s="18">
-        <v>0</v>
-      </c>
-      <c r="N11" s="18">
-        <v>0</v>
-      </c>
-      <c r="O11" s="18">
-        <v>0</v>
-      </c>
-      <c r="P11" s="18">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="18">
-        <v>0</v>
-      </c>
-      <c r="R11" s="18">
-        <v>34.020000000000003</v>
-      </c>
-      <c r="S11" s="18">
-        <v>0</v>
-      </c>
-      <c r="T11" s="41">
-        <v>12</v>
-      </c>
-      <c r="U11" s="18">
-        <v>175</v>
-      </c>
-      <c r="V11" s="18">
-        <v>33.9</v>
-      </c>
-      <c r="W11" s="18">
-        <v>0</v>
-      </c>
-      <c r="X11" s="18">
-        <v>12</v>
-      </c>
-      <c r="Y11" s="12">
-        <v>404</v>
-      </c>
+      <c r="D11" s="17"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="18"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="18"/>
+      <c r="S11" s="18"/>
+      <c r="T11" s="41"/>
+      <c r="U11" s="18"/>
+      <c r="V11" s="18"/>
+      <c r="W11" s="18"/>
+      <c r="X11" s="18"/>
+      <c r="Y11" s="12"/>
       <c r="Z11" s="17"/>
-      <c r="AA11" s="18">
-        <v>175</v>
-      </c>
-      <c r="AB11" s="18">
-        <v>200</v>
-      </c>
-      <c r="AC11" s="18">
-        <v>0</v>
-      </c>
-      <c r="AD11" s="18">
-        <v>0</v>
-      </c>
-      <c r="AE11" s="18">
-        <v>0</v>
-      </c>
-      <c r="AF11" s="18">
-        <v>0</v>
-      </c>
-      <c r="AG11" s="18">
-        <v>0</v>
-      </c>
-      <c r="AH11" s="18">
-        <v>0</v>
-      </c>
-      <c r="AI11" s="18">
-        <v>10.25</v>
-      </c>
-      <c r="AJ11" s="18">
-        <v>10.25</v>
-      </c>
-      <c r="AK11" s="18">
-        <v>-0.25</v>
-      </c>
-      <c r="AL11" s="18">
-        <v>1.9</v>
-      </c>
-      <c r="AM11" s="18">
-        <v>0</v>
-      </c>
-      <c r="AN11" s="18">
-        <v>0</v>
-      </c>
-      <c r="AO11" s="18">
-        <v>0</v>
-      </c>
-      <c r="AP11" s="18">
-        <v>0</v>
-      </c>
-      <c r="AQ11" s="18">
-        <v>0</v>
-      </c>
-      <c r="AR11" s="18">
-        <v>0</v>
-      </c>
-      <c r="AS11" s="18">
-        <v>0</v>
-      </c>
-      <c r="AT11" s="18">
-        <v>0</v>
-      </c>
-      <c r="AU11" s="18">
-        <v>10</v>
-      </c>
-      <c r="AV11" s="18">
-        <v>30</v>
-      </c>
+      <c r="AA11" s="18"/>
+      <c r="AB11" s="18"/>
+      <c r="AC11" s="18"/>
+      <c r="AD11" s="18"/>
+      <c r="AE11" s="18"/>
+      <c r="AF11" s="18"/>
+      <c r="AG11" s="18"/>
+      <c r="AH11" s="18"/>
+      <c r="AI11" s="18"/>
+      <c r="AJ11" s="18"/>
+      <c r="AK11" s="18"/>
+      <c r="AL11" s="18"/>
+      <c r="AM11" s="18"/>
+      <c r="AN11" s="18"/>
+      <c r="AO11" s="18"/>
+      <c r="AP11" s="18"/>
+      <c r="AQ11" s="18"/>
+      <c r="AR11" s="18"/>
+      <c r="AS11" s="18"/>
+      <c r="AT11" s="18"/>
+      <c r="AU11" s="18"/>
+      <c r="AV11" s="18"/>
       <c r="AW11" s="17"/>
-      <c r="AX11" s="18">
-        <v>900</v>
-      </c>
-      <c r="AY11" s="18">
-        <v>10.5</v>
-      </c>
-      <c r="AZ11" s="18">
-        <v>0.03</v>
-      </c>
-      <c r="BA11" s="18">
-        <v>120.628</v>
-      </c>
-      <c r="BB11" s="18">
-        <v>70.396699999999996</v>
-      </c>
-      <c r="BC11" s="18">
-        <v>0</v>
-      </c>
+      <c r="AX11" s="18"/>
+      <c r="AY11" s="18"/>
+      <c r="AZ11" s="18"/>
+      <c r="BA11" s="18"/>
+      <c r="BB11" s="18"/>
+      <c r="BC11" s="18"/>
       <c r="BD11" s="17"/>
-      <c r="BE11" s="12">
-        <v>1</v>
-      </c>
-      <c r="BF11" s="12">
-        <v>2.5</v>
-      </c>
-      <c r="BG11" s="12">
-        <v>2</v>
-      </c>
-      <c r="BH11" s="12">
-        <v>1.62</v>
-      </c>
-      <c r="BI11" s="12">
-        <v>1.333</v>
-      </c>
-      <c r="BJ11" s="12">
-        <v>1.095</v>
-      </c>
-      <c r="BK11" s="12">
-        <v>2.6520000000000001</v>
-      </c>
-      <c r="BL11" s="12">
-        <v>2.714</v>
-      </c>
-      <c r="BM11" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="BN11" s="12">
-        <v>0</v>
-      </c>
-      <c r="BO11" s="12">
-        <v>0</v>
-      </c>
-      <c r="BP11" s="12">
-        <v>0</v>
-      </c>
-      <c r="BQ11" s="12">
-        <v>20</v>
-      </c>
+      <c r="BE11" s="12"/>
+      <c r="BF11" s="12"/>
+      <c r="BG11" s="12"/>
+      <c r="BH11" s="12"/>
+      <c r="BI11" s="12"/>
+      <c r="BJ11" s="12"/>
+      <c r="BK11" s="12"/>
+      <c r="BL11" s="12"/>
+      <c r="BM11" s="12"/>
+      <c r="BN11" s="12"/>
+      <c r="BO11" s="12"/>
+      <c r="BP11" s="12"/>
+      <c r="BQ11" s="12"/>
       <c r="BR11" s="17"/>
-      <c r="BS11" s="12">
-        <v>6762.75</v>
-      </c>
-      <c r="BT11" s="12">
-        <v>3238.5</v>
-      </c>
-      <c r="BU11" s="12">
-        <v>0</v>
-      </c>
-      <c r="BV11" s="12">
-        <v>0</v>
-      </c>
-      <c r="BW11" s="12">
-        <v>0</v>
-      </c>
-      <c r="BX11" s="12">
-        <v>0.96699999999999997</v>
-      </c>
+      <c r="BS11" s="12"/>
+      <c r="BT11" s="12"/>
+      <c r="BU11" s="12"/>
+      <c r="BV11" s="12"/>
+      <c r="BW11" s="12"/>
+      <c r="BX11" s="12"/>
       <c r="BY11" s="17"/>
-      <c r="BZ11" s="12">
-        <v>0</v>
-      </c>
-      <c r="CA11" s="12">
-        <v>0</v>
-      </c>
-      <c r="CB11" s="12">
-        <v>0</v>
-      </c>
-      <c r="CC11" s="12">
-        <v>0.45</v>
-      </c>
-      <c r="CD11" s="12">
-        <v>-0.89</v>
-      </c>
-      <c r="CE11" s="12">
-        <v>2015</v>
-      </c>
-      <c r="CF11" s="12">
-        <v>2.3289999999999999E-3</v>
-      </c>
-      <c r="CG11" s="12">
-        <v>34.25</v>
-      </c>
-      <c r="CH11" s="12">
-        <v>0</v>
-      </c>
-      <c r="CI11" s="12">
-        <v>10</v>
-      </c>
+      <c r="BZ11" s="12"/>
+      <c r="CA11" s="12"/>
+      <c r="CB11" s="12"/>
+      <c r="CC11" s="12"/>
+      <c r="CD11" s="12"/>
+      <c r="CE11" s="12"/>
+      <c r="CF11" s="12"/>
+      <c r="CG11" s="12"/>
+      <c r="CH11" s="12"/>
+      <c r="CI11" s="12"/>
       <c r="CJ11" s="17"/>
-      <c r="CK11" s="18">
-        <v>0.7</v>
-      </c>
-      <c r="CL11" s="18">
-        <v>0</v>
-      </c>
-      <c r="CM11" s="18">
-        <v>0</v>
-      </c>
-      <c r="CN11" s="18">
-        <v>0</v>
-      </c>
-      <c r="CO11" s="18">
-        <v>0</v>
-      </c>
-      <c r="CP11" s="18">
-        <v>0</v>
-      </c>
-      <c r="CQ11" s="18">
-        <v>0</v>
-      </c>
+      <c r="CK11" s="18"/>
+      <c r="CL11" s="18"/>
+      <c r="CM11" s="18"/>
+      <c r="CN11" s="18"/>
+      <c r="CO11" s="18"/>
+      <c r="CP11" s="18"/>
+      <c r="CQ11" s="18"/>
       <c r="CR11" s="17"/>
-      <c r="CS11" s="18">
-        <v>280</v>
-      </c>
-      <c r="CT11" s="18">
-        <v>9900</v>
-      </c>
-      <c r="CU11" s="18">
-        <v>0</v>
-      </c>
+      <c r="CS11" s="18"/>
+      <c r="CT11" s="18"/>
+      <c r="CU11" s="18"/>
     </row>
     <row r="12" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A12" s="19">
-        <v>0.47</v>
-      </c>
+      <c r="A12" s="19"/>
       <c r="B12" s="1"/>
       <c r="C12" s="8"/>
-      <c r="D12" s="17">
-        <v>0</v>
-      </c>
-      <c r="E12" s="18">
-        <v>63</v>
-      </c>
-      <c r="F12" s="18">
-        <v>47</v>
-      </c>
-      <c r="G12" s="18">
-        <v>46</v>
-      </c>
-      <c r="H12" s="18">
-        <v>0</v>
-      </c>
-      <c r="I12" s="18">
-        <v>0</v>
-      </c>
-      <c r="J12" s="18">
-        <v>0</v>
-      </c>
-      <c r="K12" s="18">
-        <v>0</v>
-      </c>
-      <c r="L12" s="18">
-        <v>0</v>
-      </c>
-      <c r="M12" s="18">
-        <v>0</v>
-      </c>
-      <c r="N12" s="18">
-        <v>0</v>
-      </c>
-      <c r="O12" s="18">
-        <v>0</v>
-      </c>
-      <c r="P12" s="18">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="18">
-        <v>0</v>
-      </c>
-      <c r="R12" s="18">
-        <v>33.39</v>
-      </c>
-      <c r="S12" s="18">
-        <v>0</v>
-      </c>
-      <c r="T12" s="41">
-        <v>12</v>
-      </c>
-      <c r="U12" s="18">
-        <v>175</v>
-      </c>
-      <c r="V12" s="18">
-        <v>33.9</v>
-      </c>
-      <c r="W12" s="18">
-        <v>0</v>
-      </c>
-      <c r="X12" s="18">
-        <v>12</v>
-      </c>
-      <c r="Y12" s="12">
-        <v>404</v>
-      </c>
+      <c r="D12" s="17"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="18"/>
+      <c r="R12" s="18"/>
+      <c r="S12" s="18"/>
+      <c r="T12" s="41"/>
+      <c r="U12" s="18"/>
+      <c r="V12" s="18"/>
+      <c r="W12" s="18"/>
+      <c r="X12" s="18"/>
+      <c r="Y12" s="12"/>
       <c r="Z12" s="17"/>
-      <c r="AA12" s="18">
-        <v>175</v>
-      </c>
-      <c r="AB12" s="18">
-        <v>200</v>
-      </c>
-      <c r="AC12" s="18">
-        <v>0</v>
-      </c>
-      <c r="AD12" s="18">
-        <v>0</v>
-      </c>
-      <c r="AE12" s="18">
-        <v>0</v>
-      </c>
-      <c r="AF12" s="18">
-        <v>0</v>
-      </c>
-      <c r="AG12" s="18">
-        <v>0</v>
-      </c>
-      <c r="AH12" s="18">
-        <v>0</v>
-      </c>
-      <c r="AI12" s="18">
-        <v>10.25</v>
-      </c>
-      <c r="AJ12" s="18">
-        <v>10.25</v>
-      </c>
-      <c r="AK12" s="18">
-        <v>-0.25</v>
-      </c>
-      <c r="AL12" s="18">
-        <v>1.9</v>
-      </c>
-      <c r="AM12" s="18">
-        <v>0</v>
-      </c>
-      <c r="AN12" s="18">
-        <v>0</v>
-      </c>
-      <c r="AO12" s="18">
-        <v>0</v>
-      </c>
-      <c r="AP12" s="18">
-        <v>0</v>
-      </c>
-      <c r="AQ12" s="18">
-        <v>0</v>
-      </c>
-      <c r="AR12" s="18">
-        <v>0</v>
-      </c>
-      <c r="AS12" s="18">
-        <v>0</v>
-      </c>
-      <c r="AT12" s="18">
-        <v>0</v>
-      </c>
-      <c r="AU12" s="18">
-        <v>10</v>
-      </c>
-      <c r="AV12" s="18">
-        <v>30</v>
-      </c>
+      <c r="AA12" s="18"/>
+      <c r="AB12" s="18"/>
+      <c r="AC12" s="18"/>
+      <c r="AD12" s="18"/>
+      <c r="AE12" s="18"/>
+      <c r="AF12" s="18"/>
+      <c r="AG12" s="18"/>
+      <c r="AH12" s="18"/>
+      <c r="AI12" s="18"/>
+      <c r="AJ12" s="18"/>
+      <c r="AK12" s="18"/>
+      <c r="AL12" s="18"/>
+      <c r="AM12" s="18"/>
+      <c r="AN12" s="18"/>
+      <c r="AO12" s="18"/>
+      <c r="AP12" s="18"/>
+      <c r="AQ12" s="18"/>
+      <c r="AR12" s="18"/>
+      <c r="AS12" s="18"/>
+      <c r="AT12" s="18"/>
+      <c r="AU12" s="18"/>
+      <c r="AV12" s="18"/>
       <c r="AW12" s="17"/>
-      <c r="AX12" s="18">
-        <v>900</v>
-      </c>
-      <c r="AY12" s="18">
-        <v>10.5</v>
-      </c>
-      <c r="AZ12" s="18">
-        <v>0.03</v>
-      </c>
-      <c r="BA12" s="18">
-        <v>120.628</v>
-      </c>
-      <c r="BB12" s="18">
-        <v>70.396699999999996</v>
-      </c>
-      <c r="BC12" s="18">
-        <v>0</v>
-      </c>
+      <c r="AX12" s="18"/>
+      <c r="AY12" s="18"/>
+      <c r="AZ12" s="18"/>
+      <c r="BA12" s="18"/>
+      <c r="BB12" s="18"/>
+      <c r="BC12" s="18"/>
       <c r="BD12" s="17"/>
-      <c r="BE12" s="12">
-        <v>1</v>
-      </c>
-      <c r="BF12" s="12">
-        <v>2.5</v>
-      </c>
-      <c r="BG12" s="12">
-        <v>2</v>
-      </c>
-      <c r="BH12" s="12">
-        <v>1.62</v>
-      </c>
-      <c r="BI12" s="12">
-        <v>1.333</v>
-      </c>
-      <c r="BJ12" s="12">
-        <v>1.095</v>
-      </c>
-      <c r="BK12" s="12">
-        <v>2.6520000000000001</v>
-      </c>
-      <c r="BL12" s="12">
-        <v>2.714</v>
-      </c>
-      <c r="BM12" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="BN12" s="12">
-        <v>0</v>
-      </c>
-      <c r="BO12" s="12">
-        <v>0</v>
-      </c>
-      <c r="BP12" s="12">
-        <v>0</v>
-      </c>
-      <c r="BQ12" s="12">
-        <v>20</v>
-      </c>
+      <c r="BE12" s="12"/>
+      <c r="BF12" s="12"/>
+      <c r="BG12" s="12"/>
+      <c r="BH12" s="12"/>
+      <c r="BI12" s="12"/>
+      <c r="BJ12" s="12"/>
+      <c r="BK12" s="12"/>
+      <c r="BL12" s="12"/>
+      <c r="BM12" s="12"/>
+      <c r="BN12" s="12"/>
+      <c r="BO12" s="12"/>
+      <c r="BP12" s="12"/>
+      <c r="BQ12" s="12"/>
       <c r="BR12" s="17"/>
-      <c r="BS12" s="12">
-        <v>6762.75</v>
-      </c>
-      <c r="BT12" s="12">
-        <v>3238.5</v>
-      </c>
-      <c r="BU12" s="12">
-        <v>0</v>
-      </c>
-      <c r="BV12" s="12">
-        <v>0</v>
-      </c>
-      <c r="BW12" s="12">
-        <v>0</v>
-      </c>
-      <c r="BX12" s="12">
-        <v>0.96699999999999997</v>
-      </c>
+      <c r="BS12" s="12"/>
+      <c r="BT12" s="12"/>
+      <c r="BU12" s="12"/>
+      <c r="BV12" s="12"/>
+      <c r="BW12" s="12"/>
+      <c r="BX12" s="12"/>
       <c r="BY12" s="17"/>
-      <c r="BZ12" s="12">
-        <v>0</v>
-      </c>
-      <c r="CA12" s="12">
-        <v>0</v>
-      </c>
-      <c r="CB12" s="12">
-        <v>0</v>
-      </c>
-      <c r="CC12" s="12">
-        <v>0.45</v>
-      </c>
-      <c r="CD12" s="12">
-        <v>-0.89</v>
-      </c>
-      <c r="CE12" s="12">
-        <v>2015</v>
-      </c>
-      <c r="CF12" s="12">
-        <v>2.3289999999999999E-3</v>
-      </c>
-      <c r="CG12" s="12">
-        <v>34.25</v>
-      </c>
-      <c r="CH12" s="12">
-        <v>0</v>
-      </c>
-      <c r="CI12" s="12">
-        <v>10</v>
-      </c>
+      <c r="BZ12" s="12"/>
+      <c r="CA12" s="12"/>
+      <c r="CB12" s="12"/>
+      <c r="CC12" s="12"/>
+      <c r="CD12" s="12"/>
+      <c r="CE12" s="12"/>
+      <c r="CF12" s="12"/>
+      <c r="CG12" s="12"/>
+      <c r="CH12" s="12"/>
+      <c r="CI12" s="12"/>
       <c r="CJ12" s="17"/>
-      <c r="CK12" s="18">
-        <v>0.7</v>
-      </c>
-      <c r="CL12" s="18">
-        <v>0</v>
-      </c>
-      <c r="CM12" s="18">
-        <v>0</v>
-      </c>
-      <c r="CN12" s="18">
-        <v>0</v>
-      </c>
-      <c r="CO12" s="18">
-        <v>0</v>
-      </c>
-      <c r="CP12" s="18">
-        <v>0</v>
-      </c>
-      <c r="CQ12" s="18">
-        <v>0</v>
-      </c>
+      <c r="CK12" s="18"/>
+      <c r="CL12" s="18"/>
+      <c r="CM12" s="18"/>
+      <c r="CN12" s="18"/>
+      <c r="CO12" s="18"/>
+      <c r="CP12" s="18"/>
+      <c r="CQ12" s="18"/>
       <c r="CR12" s="17"/>
-      <c r="CS12" s="18">
-        <v>280</v>
-      </c>
-      <c r="CT12" s="18">
-        <v>9900</v>
-      </c>
-      <c r="CU12" s="18">
-        <v>0</v>
-      </c>
+      <c r="CS12" s="18"/>
+      <c r="CT12" s="18"/>
+      <c r="CU12" s="18"/>
     </row>
     <row r="13" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A13" s="23">
-        <v>0.48</v>
-      </c>
       <c r="B13" s="1"/>
       <c r="C13" s="8"/>
-      <c r="D13" s="17">
-        <v>0</v>
-      </c>
-      <c r="E13" s="18">
-        <v>63</v>
-      </c>
-      <c r="F13" s="18">
-        <v>47</v>
-      </c>
-      <c r="G13" s="18">
-        <v>46</v>
-      </c>
-      <c r="H13" s="18">
-        <v>0</v>
-      </c>
-      <c r="I13" s="18">
-        <v>0</v>
-      </c>
-      <c r="J13" s="18">
-        <v>0</v>
-      </c>
-      <c r="K13" s="18">
-        <v>0</v>
-      </c>
-      <c r="L13" s="18">
-        <v>0</v>
-      </c>
-      <c r="M13" s="18">
-        <v>0</v>
-      </c>
-      <c r="N13" s="18">
-        <v>0</v>
-      </c>
-      <c r="O13" s="18">
-        <v>0</v>
-      </c>
-      <c r="P13" s="18">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="18">
-        <v>0</v>
-      </c>
-      <c r="R13" s="18">
-        <v>32.76</v>
-      </c>
-      <c r="S13" s="18">
-        <v>0</v>
-      </c>
-      <c r="T13" s="41">
-        <v>12</v>
-      </c>
-      <c r="U13" s="18">
-        <v>175</v>
-      </c>
-      <c r="V13" s="18">
-        <v>33.9</v>
-      </c>
-      <c r="W13" s="18">
-        <v>0</v>
-      </c>
-      <c r="X13" s="18">
-        <v>12</v>
-      </c>
-      <c r="Y13" s="12">
-        <v>404</v>
-      </c>
+      <c r="D13" s="17"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="18"/>
+      <c r="P13" s="18"/>
+      <c r="Q13" s="18"/>
+      <c r="R13" s="18"/>
+      <c r="S13" s="18"/>
+      <c r="T13" s="41"/>
+      <c r="U13" s="18"/>
+      <c r="V13" s="18"/>
+      <c r="W13" s="18"/>
+      <c r="X13" s="18"/>
+      <c r="Y13" s="12"/>
       <c r="Z13" s="17"/>
-      <c r="AA13" s="18">
-        <v>175</v>
-      </c>
-      <c r="AB13" s="18">
-        <v>200</v>
-      </c>
-      <c r="AC13" s="18">
-        <v>0</v>
-      </c>
-      <c r="AD13" s="18">
-        <v>0</v>
-      </c>
-      <c r="AE13" s="18">
-        <v>0</v>
-      </c>
-      <c r="AF13" s="18">
-        <v>0</v>
-      </c>
-      <c r="AG13" s="18">
-        <v>0</v>
-      </c>
-      <c r="AH13" s="18">
-        <v>0</v>
-      </c>
-      <c r="AI13" s="18">
-        <v>10.25</v>
-      </c>
-      <c r="AJ13" s="18">
-        <v>10.25</v>
-      </c>
-      <c r="AK13" s="18">
-        <v>-0.25</v>
-      </c>
-      <c r="AL13" s="18">
-        <v>1.9</v>
-      </c>
-      <c r="AM13" s="18">
-        <v>0</v>
-      </c>
-      <c r="AN13" s="18">
-        <v>0</v>
-      </c>
-      <c r="AO13" s="18">
-        <v>0</v>
-      </c>
-      <c r="AP13" s="18">
-        <v>0</v>
-      </c>
-      <c r="AQ13" s="18">
-        <v>0</v>
-      </c>
-      <c r="AR13" s="18">
-        <v>0</v>
-      </c>
-      <c r="AS13" s="18">
-        <v>0</v>
-      </c>
-      <c r="AT13" s="18">
-        <v>0</v>
-      </c>
-      <c r="AU13" s="18">
-        <v>10</v>
-      </c>
-      <c r="AV13" s="18">
-        <v>30</v>
-      </c>
+      <c r="AA13" s="18"/>
+      <c r="AB13" s="18"/>
+      <c r="AC13" s="18"/>
+      <c r="AD13" s="18"/>
+      <c r="AE13" s="18"/>
+      <c r="AF13" s="18"/>
+      <c r="AG13" s="18"/>
+      <c r="AH13" s="18"/>
+      <c r="AI13" s="18"/>
+      <c r="AJ13" s="18"/>
+      <c r="AK13" s="18"/>
+      <c r="AL13" s="18"/>
+      <c r="AM13" s="18"/>
+      <c r="AN13" s="18"/>
+      <c r="AO13" s="18"/>
+      <c r="AP13" s="18"/>
+      <c r="AQ13" s="18"/>
+      <c r="AR13" s="18"/>
+      <c r="AS13" s="18"/>
+      <c r="AT13" s="18"/>
+      <c r="AU13" s="18"/>
+      <c r="AV13" s="18"/>
       <c r="AW13" s="17"/>
-      <c r="AX13" s="18">
-        <v>900</v>
-      </c>
-      <c r="AY13" s="18">
-        <v>10.5</v>
-      </c>
-      <c r="AZ13" s="18">
-        <v>0.03</v>
-      </c>
-      <c r="BA13" s="18">
-        <v>120.628</v>
-      </c>
-      <c r="BB13" s="18">
-        <v>70.396699999999996</v>
-      </c>
-      <c r="BC13" s="18">
-        <v>0</v>
-      </c>
+      <c r="AX13" s="18"/>
+      <c r="AY13" s="18"/>
+      <c r="AZ13" s="18"/>
+      <c r="BA13" s="18"/>
+      <c r="BB13" s="18"/>
+      <c r="BC13" s="18"/>
       <c r="BD13" s="17"/>
-      <c r="BE13" s="12">
-        <v>1</v>
-      </c>
-      <c r="BF13" s="12">
-        <v>2.5</v>
-      </c>
-      <c r="BG13" s="12">
-        <v>2</v>
-      </c>
-      <c r="BH13" s="12">
-        <v>1.62</v>
-      </c>
-      <c r="BI13" s="12">
-        <v>1.333</v>
-      </c>
-      <c r="BJ13" s="12">
-        <v>1.095</v>
-      </c>
-      <c r="BK13" s="12">
-        <v>2.6520000000000001</v>
-      </c>
-      <c r="BL13" s="12">
-        <v>2.714</v>
-      </c>
-      <c r="BM13" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="BN13" s="12">
-        <v>0</v>
-      </c>
-      <c r="BO13" s="12">
-        <v>0</v>
-      </c>
-      <c r="BP13" s="12">
-        <v>0</v>
-      </c>
-      <c r="BQ13" s="12">
-        <v>20</v>
-      </c>
+      <c r="BE13" s="12"/>
+      <c r="BF13" s="12"/>
+      <c r="BG13" s="12"/>
+      <c r="BH13" s="12"/>
+      <c r="BI13" s="12"/>
+      <c r="BJ13" s="12"/>
+      <c r="BK13" s="12"/>
+      <c r="BL13" s="12"/>
+      <c r="BM13" s="12"/>
+      <c r="BN13" s="12"/>
+      <c r="BO13" s="12"/>
+      <c r="BP13" s="12"/>
+      <c r="BQ13" s="12"/>
       <c r="BR13" s="17"/>
-      <c r="BS13" s="12">
-        <v>6762.75</v>
-      </c>
-      <c r="BT13" s="12">
-        <v>3238.5</v>
-      </c>
-      <c r="BU13" s="12">
-        <v>0</v>
-      </c>
-      <c r="BV13" s="12">
-        <v>0</v>
-      </c>
-      <c r="BW13" s="12">
-        <v>0</v>
-      </c>
-      <c r="BX13" s="12">
-        <v>0.96699999999999997</v>
-      </c>
+      <c r="BS13" s="12"/>
+      <c r="BT13" s="12"/>
+      <c r="BU13" s="12"/>
+      <c r="BV13" s="12"/>
+      <c r="BW13" s="12"/>
+      <c r="BX13" s="12"/>
       <c r="BY13" s="17"/>
-      <c r="BZ13" s="12">
-        <v>0</v>
-      </c>
-      <c r="CA13" s="12">
-        <v>0</v>
-      </c>
-      <c r="CB13" s="12">
-        <v>0</v>
-      </c>
-      <c r="CC13" s="12">
-        <v>0.45</v>
-      </c>
-      <c r="CD13" s="12">
-        <v>-0.89</v>
-      </c>
-      <c r="CE13" s="12">
-        <v>2015</v>
-      </c>
-      <c r="CF13" s="12">
-        <v>2.3289999999999999E-3</v>
-      </c>
-      <c r="CG13" s="12">
-        <v>34.25</v>
-      </c>
-      <c r="CH13" s="12">
-        <v>0</v>
-      </c>
-      <c r="CI13" s="12">
-        <v>10</v>
-      </c>
+      <c r="BZ13" s="12"/>
+      <c r="CA13" s="12"/>
+      <c r="CB13" s="12"/>
+      <c r="CC13" s="12"/>
+      <c r="CD13" s="12"/>
+      <c r="CE13" s="12"/>
+      <c r="CF13" s="12"/>
+      <c r="CG13" s="12"/>
+      <c r="CH13" s="12"/>
+      <c r="CI13" s="12"/>
       <c r="CJ13" s="17"/>
-      <c r="CK13" s="18">
-        <v>0.7</v>
-      </c>
-      <c r="CL13" s="18">
-        <v>0</v>
-      </c>
-      <c r="CM13" s="18">
-        <v>0</v>
-      </c>
-      <c r="CN13" s="18">
-        <v>0</v>
-      </c>
-      <c r="CO13" s="18">
-        <v>0</v>
-      </c>
-      <c r="CP13" s="18">
-        <v>0</v>
-      </c>
-      <c r="CQ13" s="18">
-        <v>0</v>
-      </c>
+      <c r="CK13" s="18"/>
+      <c r="CL13" s="18"/>
+      <c r="CM13" s="18"/>
+      <c r="CN13" s="18"/>
+      <c r="CO13" s="18"/>
+      <c r="CP13" s="18"/>
+      <c r="CQ13" s="18"/>
       <c r="CR13" s="17"/>
-      <c r="CS13" s="18">
-        <v>280</v>
-      </c>
-      <c r="CT13" s="18">
-        <v>9900</v>
-      </c>
-      <c r="CU13" s="18">
-        <v>0</v>
-      </c>
+      <c r="CS13" s="18"/>
+      <c r="CT13" s="18"/>
+      <c r="CU13" s="18"/>
     </row>
     <row r="14" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A14" s="19">
-        <v>0.49</v>
-      </c>
+      <c r="A14" s="19"/>
       <c r="B14" s="1"/>
       <c r="C14" s="8"/>
-      <c r="D14" s="17">
-        <v>0</v>
-      </c>
-      <c r="E14" s="18">
-        <v>63</v>
-      </c>
-      <c r="F14" s="18">
-        <v>47</v>
-      </c>
-      <c r="G14" s="18">
-        <v>46</v>
-      </c>
-      <c r="H14" s="18">
-        <v>0</v>
-      </c>
-      <c r="I14" s="18">
-        <v>0</v>
-      </c>
-      <c r="J14" s="18">
-        <v>0</v>
-      </c>
-      <c r="K14" s="18">
-        <v>0</v>
-      </c>
-      <c r="L14" s="18">
-        <v>0</v>
-      </c>
-      <c r="M14" s="18">
-        <v>0</v>
-      </c>
-      <c r="N14" s="18">
-        <v>0</v>
-      </c>
-      <c r="O14" s="18">
-        <v>0</v>
-      </c>
-      <c r="P14" s="18">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="18">
-        <v>0</v>
-      </c>
-      <c r="R14" s="18">
-        <v>32.130000000000003</v>
-      </c>
-      <c r="S14" s="18">
-        <v>0</v>
-      </c>
-      <c r="T14" s="41">
-        <v>12</v>
-      </c>
-      <c r="U14" s="18">
-        <v>175</v>
-      </c>
-      <c r="V14" s="18">
-        <v>33.9</v>
-      </c>
-      <c r="W14" s="18">
-        <v>0</v>
-      </c>
-      <c r="X14" s="18">
-        <v>12</v>
-      </c>
-      <c r="Y14" s="12">
-        <v>404</v>
-      </c>
+      <c r="D14" s="17"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="18"/>
+      <c r="R14" s="18"/>
+      <c r="S14" s="18"/>
+      <c r="T14" s="41"/>
+      <c r="U14" s="18"/>
+      <c r="V14" s="18"/>
+      <c r="W14" s="18"/>
+      <c r="X14" s="18"/>
+      <c r="Y14" s="12"/>
       <c r="Z14" s="17"/>
-      <c r="AA14" s="18">
-        <v>175</v>
-      </c>
-      <c r="AB14" s="18">
-        <v>200</v>
-      </c>
-      <c r="AC14" s="18">
-        <v>0</v>
-      </c>
-      <c r="AD14" s="18">
-        <v>0</v>
-      </c>
-      <c r="AE14" s="18">
-        <v>0</v>
-      </c>
-      <c r="AF14" s="18">
-        <v>0</v>
-      </c>
-      <c r="AG14" s="18">
-        <v>0</v>
-      </c>
-      <c r="AH14" s="18">
-        <v>0</v>
-      </c>
-      <c r="AI14" s="18">
-        <v>10.25</v>
-      </c>
-      <c r="AJ14" s="18">
-        <v>10.25</v>
-      </c>
-      <c r="AK14" s="18">
-        <v>-0.25</v>
-      </c>
-      <c r="AL14" s="18">
-        <v>1.9</v>
-      </c>
-      <c r="AM14" s="18">
-        <v>0</v>
-      </c>
-      <c r="AN14" s="18">
-        <v>0</v>
-      </c>
-      <c r="AO14" s="18">
-        <v>0</v>
-      </c>
-      <c r="AP14" s="18">
-        <v>0</v>
-      </c>
-      <c r="AQ14" s="18">
-        <v>0</v>
-      </c>
-      <c r="AR14" s="18">
-        <v>0</v>
-      </c>
-      <c r="AS14" s="18">
-        <v>0</v>
-      </c>
-      <c r="AT14" s="18">
-        <v>0</v>
-      </c>
-      <c r="AU14" s="18">
-        <v>10</v>
-      </c>
-      <c r="AV14" s="18">
-        <v>30</v>
-      </c>
+      <c r="AA14" s="18"/>
+      <c r="AB14" s="18"/>
+      <c r="AC14" s="18"/>
+      <c r="AD14" s="18"/>
+      <c r="AE14" s="18"/>
+      <c r="AF14" s="18"/>
+      <c r="AG14" s="18"/>
+      <c r="AH14" s="18"/>
+      <c r="AI14" s="18"/>
+      <c r="AJ14" s="18"/>
+      <c r="AK14" s="18"/>
+      <c r="AL14" s="18"/>
+      <c r="AM14" s="18"/>
+      <c r="AN14" s="18"/>
+      <c r="AO14" s="18"/>
+      <c r="AP14" s="18"/>
+      <c r="AQ14" s="18"/>
+      <c r="AR14" s="18"/>
+      <c r="AS14" s="18"/>
+      <c r="AT14" s="18"/>
+      <c r="AU14" s="18"/>
+      <c r="AV14" s="18"/>
       <c r="AW14" s="17"/>
-      <c r="AX14" s="18">
-        <v>900</v>
-      </c>
-      <c r="AY14" s="18">
-        <v>10.5</v>
-      </c>
-      <c r="AZ14" s="18">
-        <v>0.03</v>
-      </c>
-      <c r="BA14" s="18">
-        <v>120.628</v>
-      </c>
-      <c r="BB14" s="18">
-        <v>70.396699999999996</v>
-      </c>
-      <c r="BC14" s="18">
-        <v>0</v>
-      </c>
+      <c r="AX14" s="18"/>
+      <c r="AY14" s="18"/>
+      <c r="AZ14" s="18"/>
+      <c r="BA14" s="18"/>
+      <c r="BB14" s="18"/>
+      <c r="BC14" s="18"/>
       <c r="BD14" s="17"/>
-      <c r="BE14" s="12">
-        <v>1</v>
-      </c>
-      <c r="BF14" s="12">
-        <v>2.5</v>
-      </c>
-      <c r="BG14" s="12">
-        <v>2</v>
-      </c>
-      <c r="BH14" s="12">
-        <v>1.62</v>
-      </c>
-      <c r="BI14" s="12">
-        <v>1.333</v>
-      </c>
-      <c r="BJ14" s="12">
-        <v>1.095</v>
-      </c>
-      <c r="BK14" s="12">
-        <v>2.6520000000000001</v>
-      </c>
-      <c r="BL14" s="12">
-        <v>2.714</v>
-      </c>
-      <c r="BM14" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="BN14" s="12">
-        <v>0</v>
-      </c>
-      <c r="BO14" s="12">
-        <v>0</v>
-      </c>
-      <c r="BP14" s="12">
-        <v>0</v>
-      </c>
-      <c r="BQ14" s="12">
-        <v>20</v>
-      </c>
+      <c r="BE14" s="12"/>
+      <c r="BF14" s="12"/>
+      <c r="BG14" s="12"/>
+      <c r="BH14" s="12"/>
+      <c r="BI14" s="12"/>
+      <c r="BJ14" s="12"/>
+      <c r="BK14" s="12"/>
+      <c r="BL14" s="12"/>
+      <c r="BM14" s="12"/>
+      <c r="BN14" s="12"/>
+      <c r="BO14" s="12"/>
+      <c r="BP14" s="12"/>
+      <c r="BQ14" s="12"/>
       <c r="BR14" s="17"/>
-      <c r="BS14" s="12">
-        <v>6762.75</v>
-      </c>
-      <c r="BT14" s="12">
-        <v>3238.5</v>
-      </c>
-      <c r="BU14" s="12">
-        <v>0</v>
-      </c>
-      <c r="BV14" s="12">
-        <v>0</v>
-      </c>
-      <c r="BW14" s="12">
-        <v>0</v>
-      </c>
-      <c r="BX14" s="12">
-        <v>0.96699999999999997</v>
-      </c>
+      <c r="BS14" s="12"/>
+      <c r="BT14" s="12"/>
+      <c r="BU14" s="12"/>
+      <c r="BV14" s="12"/>
+      <c r="BW14" s="12"/>
+      <c r="BX14" s="12"/>
       <c r="BY14" s="17"/>
-      <c r="BZ14" s="12">
-        <v>0</v>
-      </c>
-      <c r="CA14" s="12">
-        <v>0</v>
-      </c>
-      <c r="CB14" s="12">
-        <v>0</v>
-      </c>
-      <c r="CC14" s="12">
-        <v>0.45</v>
-      </c>
-      <c r="CD14" s="12">
-        <v>-0.89</v>
-      </c>
-      <c r="CE14" s="12">
-        <v>2015</v>
-      </c>
-      <c r="CF14" s="12">
-        <v>2.3289999999999999E-3</v>
-      </c>
-      <c r="CG14" s="12">
-        <v>34.25</v>
-      </c>
-      <c r="CH14" s="12">
-        <v>0</v>
-      </c>
-      <c r="CI14" s="12">
-        <v>10</v>
-      </c>
+      <c r="BZ14" s="12"/>
+      <c r="CA14" s="12"/>
+      <c r="CB14" s="12"/>
+      <c r="CC14" s="12"/>
+      <c r="CD14" s="12"/>
+      <c r="CE14" s="12"/>
+      <c r="CF14" s="12"/>
+      <c r="CG14" s="12"/>
+      <c r="CH14" s="12"/>
+      <c r="CI14" s="12"/>
       <c r="CJ14" s="17"/>
-      <c r="CK14" s="18">
-        <v>0.7</v>
-      </c>
-      <c r="CL14" s="18">
-        <v>0</v>
-      </c>
-      <c r="CM14" s="18">
-        <v>0</v>
-      </c>
-      <c r="CN14" s="18">
-        <v>0</v>
-      </c>
-      <c r="CO14" s="18">
-        <v>0</v>
-      </c>
-      <c r="CP14" s="18">
-        <v>0</v>
-      </c>
-      <c r="CQ14" s="18">
-        <v>0</v>
-      </c>
+      <c r="CK14" s="18"/>
+      <c r="CL14" s="18"/>
+      <c r="CM14" s="18"/>
+      <c r="CN14" s="18"/>
+      <c r="CO14" s="18"/>
+      <c r="CP14" s="18"/>
+      <c r="CQ14" s="18"/>
       <c r="CR14" s="17"/>
-      <c r="CS14" s="18">
-        <v>280</v>
-      </c>
-      <c r="CT14" s="18">
-        <v>9900</v>
-      </c>
-      <c r="CU14" s="18">
-        <v>0</v>
-      </c>
+      <c r="CS14" s="18"/>
+      <c r="CT14" s="18"/>
+      <c r="CU14" s="18"/>
     </row>
     <row r="15" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A15" s="19">
-        <v>0.5</v>
-      </c>
       <c r="B15" s="1"/>
       <c r="C15" s="8"/>
-      <c r="D15" s="17">
-        <v>0</v>
-      </c>
-      <c r="E15" s="18">
-        <v>63</v>
-      </c>
-      <c r="F15" s="18">
-        <v>47</v>
-      </c>
-      <c r="G15" s="18">
-        <v>46</v>
-      </c>
-      <c r="H15" s="18">
-        <v>0</v>
-      </c>
-      <c r="I15" s="18">
-        <v>0</v>
-      </c>
-      <c r="J15" s="18">
-        <v>0</v>
-      </c>
-      <c r="K15" s="18">
-        <v>0</v>
-      </c>
-      <c r="L15" s="18">
-        <v>0</v>
-      </c>
-      <c r="M15" s="18">
-        <v>0</v>
-      </c>
-      <c r="N15" s="18">
-        <v>0</v>
-      </c>
-      <c r="O15" s="18">
-        <v>0</v>
-      </c>
-      <c r="P15" s="18">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="18">
-        <v>0</v>
-      </c>
-      <c r="R15" s="18">
-        <v>31.5</v>
-      </c>
-      <c r="S15" s="18">
-        <v>0</v>
-      </c>
-      <c r="T15" s="41">
-        <v>12</v>
-      </c>
-      <c r="U15" s="18">
-        <v>175</v>
-      </c>
-      <c r="V15" s="18">
-        <v>33.9</v>
-      </c>
-      <c r="W15" s="18">
-        <v>0</v>
-      </c>
-      <c r="X15" s="18">
-        <v>12</v>
-      </c>
-      <c r="Y15" s="12">
-        <v>404</v>
-      </c>
+      <c r="D15" s="17"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="18"/>
+      <c r="S15" s="18"/>
+      <c r="T15" s="41"/>
+      <c r="U15" s="18"/>
+      <c r="V15" s="18"/>
+      <c r="W15" s="18"/>
+      <c r="X15" s="18"/>
+      <c r="Y15" s="12"/>
       <c r="Z15" s="17"/>
-      <c r="AA15" s="18">
-        <v>175</v>
-      </c>
-      <c r="AB15" s="18">
-        <v>200</v>
-      </c>
-      <c r="AC15" s="18">
-        <v>0</v>
-      </c>
-      <c r="AD15" s="18">
-        <v>0</v>
-      </c>
-      <c r="AE15" s="18">
-        <v>0</v>
-      </c>
-      <c r="AF15" s="18">
-        <v>0</v>
-      </c>
-      <c r="AG15" s="18">
-        <v>0</v>
-      </c>
-      <c r="AH15" s="18">
-        <v>0</v>
-      </c>
-      <c r="AI15" s="18">
-        <v>10.25</v>
-      </c>
-      <c r="AJ15" s="18">
-        <v>10.25</v>
-      </c>
-      <c r="AK15" s="18">
-        <v>-0.25</v>
-      </c>
-      <c r="AL15" s="18">
-        <v>1.9</v>
-      </c>
-      <c r="AM15" s="18">
-        <v>0</v>
-      </c>
-      <c r="AN15" s="18">
-        <v>0</v>
-      </c>
-      <c r="AO15" s="18">
-        <v>0</v>
-      </c>
-      <c r="AP15" s="18">
-        <v>0</v>
-      </c>
-      <c r="AQ15" s="18">
-        <v>0</v>
-      </c>
-      <c r="AR15" s="18">
-        <v>0</v>
-      </c>
-      <c r="AS15" s="18">
-        <v>0</v>
-      </c>
-      <c r="AT15" s="18">
-        <v>0</v>
-      </c>
-      <c r="AU15" s="18">
-        <v>10</v>
-      </c>
-      <c r="AV15" s="18">
-        <v>30</v>
-      </c>
+      <c r="AA15" s="18"/>
+      <c r="AB15" s="18"/>
+      <c r="AC15" s="18"/>
+      <c r="AD15" s="18"/>
+      <c r="AE15" s="18"/>
+      <c r="AF15" s="18"/>
+      <c r="AG15" s="18"/>
+      <c r="AH15" s="18"/>
+      <c r="AI15" s="18"/>
+      <c r="AJ15" s="18"/>
+      <c r="AK15" s="18"/>
+      <c r="AL15" s="18"/>
+      <c r="AM15" s="18"/>
+      <c r="AN15" s="18"/>
+      <c r="AO15" s="18"/>
+      <c r="AP15" s="18"/>
+      <c r="AQ15" s="18"/>
+      <c r="AR15" s="18"/>
+      <c r="AS15" s="18"/>
+      <c r="AT15" s="18"/>
+      <c r="AU15" s="18"/>
+      <c r="AV15" s="18"/>
       <c r="AW15" s="17"/>
-      <c r="AX15" s="18">
-        <v>900</v>
-      </c>
-      <c r="AY15" s="18">
-        <v>10.5</v>
-      </c>
-      <c r="AZ15" s="18">
-        <v>0.03</v>
-      </c>
-      <c r="BA15" s="18">
-        <v>120.628</v>
-      </c>
-      <c r="BB15" s="18">
-        <v>70.396699999999996</v>
-      </c>
-      <c r="BC15" s="18">
-        <v>0</v>
-      </c>
+      <c r="AX15" s="18"/>
+      <c r="AY15" s="18"/>
+      <c r="AZ15" s="18"/>
+      <c r="BA15" s="18"/>
+      <c r="BB15" s="18"/>
+      <c r="BC15" s="18"/>
       <c r="BD15" s="17"/>
-      <c r="BE15" s="12">
-        <v>1</v>
-      </c>
-      <c r="BF15" s="12">
-        <v>2.5</v>
-      </c>
-      <c r="BG15" s="12">
-        <v>2</v>
-      </c>
-      <c r="BH15" s="12">
-        <v>1.62</v>
-      </c>
-      <c r="BI15" s="12">
-        <v>1.333</v>
-      </c>
-      <c r="BJ15" s="12">
-        <v>1.095</v>
-      </c>
-      <c r="BK15" s="12">
-        <v>2.6520000000000001</v>
-      </c>
-      <c r="BL15" s="12">
-        <v>2.714</v>
-      </c>
-      <c r="BM15" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="BN15" s="12">
-        <v>0</v>
-      </c>
-      <c r="BO15" s="12">
-        <v>0</v>
-      </c>
-      <c r="BP15" s="12">
-        <v>0</v>
-      </c>
-      <c r="BQ15" s="12">
-        <v>20</v>
-      </c>
+      <c r="BE15" s="12"/>
+      <c r="BF15" s="12"/>
+      <c r="BG15" s="12"/>
+      <c r="BH15" s="12"/>
+      <c r="BI15" s="12"/>
+      <c r="BJ15" s="12"/>
+      <c r="BK15" s="12"/>
+      <c r="BL15" s="12"/>
+      <c r="BM15" s="12"/>
+      <c r="BN15" s="12"/>
+      <c r="BO15" s="12"/>
+      <c r="BP15" s="12"/>
+      <c r="BQ15" s="12"/>
       <c r="BR15" s="17"/>
-      <c r="BS15" s="12">
-        <v>6762.75</v>
-      </c>
-      <c r="BT15" s="12">
-        <v>3238.5</v>
-      </c>
-      <c r="BU15" s="12">
-        <v>0</v>
-      </c>
-      <c r="BV15" s="12">
-        <v>0</v>
-      </c>
-      <c r="BW15" s="12">
-        <v>0</v>
-      </c>
-      <c r="BX15" s="12">
-        <v>0.96699999999999997</v>
-      </c>
+      <c r="BS15" s="12"/>
+      <c r="BT15" s="12"/>
+      <c r="BU15" s="12"/>
+      <c r="BV15" s="12"/>
+      <c r="BW15" s="12"/>
+      <c r="BX15" s="12"/>
       <c r="BY15" s="17"/>
-      <c r="BZ15" s="12">
-        <v>0</v>
-      </c>
-      <c r="CA15" s="12">
-        <v>0</v>
-      </c>
-      <c r="CB15" s="12">
-        <v>0</v>
-      </c>
-      <c r="CC15" s="12">
-        <v>0.45</v>
-      </c>
-      <c r="CD15" s="12">
-        <v>-0.89</v>
-      </c>
-      <c r="CE15" s="12">
-        <v>2015</v>
-      </c>
-      <c r="CF15" s="12">
-        <v>2.3289999999999999E-3</v>
-      </c>
-      <c r="CG15" s="12">
-        <v>34.25</v>
-      </c>
-      <c r="CH15" s="12">
-        <v>0</v>
-      </c>
-      <c r="CI15" s="12">
-        <v>10</v>
-      </c>
+      <c r="BZ15" s="12"/>
+      <c r="CA15" s="12"/>
+      <c r="CB15" s="12"/>
+      <c r="CC15" s="12"/>
+      <c r="CD15" s="12"/>
+      <c r="CE15" s="12"/>
+      <c r="CF15" s="12"/>
+      <c r="CG15" s="12"/>
+      <c r="CH15" s="12"/>
+      <c r="CI15" s="12"/>
       <c r="CJ15" s="17"/>
-      <c r="CK15" s="18">
-        <v>0.7</v>
-      </c>
-      <c r="CL15" s="18">
-        <v>0</v>
-      </c>
-      <c r="CM15" s="18">
-        <v>0</v>
-      </c>
-      <c r="CN15" s="18">
-        <v>0</v>
-      </c>
-      <c r="CO15" s="18">
-        <v>0</v>
-      </c>
-      <c r="CP15" s="18">
-        <v>0</v>
-      </c>
-      <c r="CQ15" s="18">
-        <v>0</v>
-      </c>
+      <c r="CK15" s="18"/>
+      <c r="CL15" s="18"/>
+      <c r="CM15" s="18"/>
+      <c r="CN15" s="18"/>
+      <c r="CO15" s="18"/>
+      <c r="CP15" s="18"/>
+      <c r="CQ15" s="18"/>
       <c r="CR15" s="17"/>
-      <c r="CS15" s="18">
-        <v>280</v>
-      </c>
-      <c r="CT15" s="18">
-        <v>9900</v>
-      </c>
-      <c r="CU15" s="18">
-        <v>0</v>
-      </c>
+      <c r="CS15" s="18"/>
+      <c r="CT15" s="18"/>
+      <c r="CU15" s="18"/>
     </row>
     <row r="16" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
       <c r="B16" s="1"/>
       <c r="C16" s="8"/>
       <c r="D16" s="17"/>
@@ -5452,7 +3823,7 @@
       <c r="AZ16" s="18"/>
       <c r="BA16" s="18"/>
       <c r="BB16" s="18"/>
-      <c r="BC16" s="40"/>
+      <c r="BC16" s="18"/>
       <c r="BD16" s="17"/>
       <c r="BE16" s="12"/>
       <c r="BF16" s="12"/>
@@ -5499,7 +3870,6 @@
       <c r="CU16" s="18"/>
     </row>
     <row r="17" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
       <c r="B17" s="1"/>
       <c r="C17" s="8"/>
       <c r="D17" s="17"/>
@@ -5553,7 +3923,7 @@
       <c r="AZ17" s="18"/>
       <c r="BA17" s="18"/>
       <c r="BB17" s="18"/>
-      <c r="BC17" s="40"/>
+      <c r="BC17" s="18"/>
       <c r="BD17" s="17"/>
       <c r="BE17" s="12"/>
       <c r="BF17" s="12"/>

</xml_diff>

<commit_message>
Intermediary Commit. Trying to run car with extremely rear-biased weight distributions but running into tire normal loads outside the range of the tire data.
</commit_message>
<xml_diff>
--- a/Functions/SetupSheets.xlsx
+++ b/Functions/SetupSheets.xlsx
@@ -5137,19 +5137,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="9217" r:id="rId4" name="SetDateTimeRef">
+        <control shapeId="9219" r:id="rId4" name="SetDateTimeMain">
           <controlPr print="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>2</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -5157,7 +5157,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="9217" r:id="rId4" name="SetDateTimeRef"/>
+        <control shapeId="9219" r:id="rId4" name="SetDateTimeMain"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -5187,19 +5187,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="9219" r:id="rId8" name="SetDateTimeMain">
+        <control shapeId="9217" r:id="rId8" name="SetDateTimeRef">
           <controlPr print="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -5207,7 +5207,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="9219" r:id="rId8" name="SetDateTimeMain"/>
+        <control shapeId="9217" r:id="rId8" name="SetDateTimeRef"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -5223,7 +5223,7 @@
       <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="Y6" sqref="Y6"/>
+      <selection pane="bottomRight" activeCell="Y7" sqref="Y7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6456,7 +6456,7 @@
         <v>9.5</v>
       </c>
       <c r="Y6" s="12">
-        <v>675</v>
+        <v>604</v>
       </c>
       <c r="Z6" s="17"/>
       <c r="AA6" s="18">
@@ -9084,19 +9084,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8195" r:id="rId4" name="SetDateTimeMain">
+        <control shapeId="8193" r:id="rId4" name="SetDateTimeRef">
           <controlPr print="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -9104,7 +9104,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8195" r:id="rId4" name="SetDateTimeMain"/>
+        <control shapeId="8193" r:id="rId4" name="SetDateTimeRef"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9134,19 +9134,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8193" r:id="rId8" name="SetDateTimeRef">
+        <control shapeId="8195" r:id="rId8" name="SetDateTimeMain">
           <controlPr print="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>2</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -9154,7 +9154,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8193" r:id="rId8" name="SetDateTimeRef"/>
+        <control shapeId="8195" r:id="rId8" name="SetDateTimeMain"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>